<commit_message>
fix all templates to start at A7, and have event title beging at D2 and date at D4
</commit_message>
<xml_diff>
--- a/templates/entry_list_template.xlsx
+++ b/templates/entry_list_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brendanwoo/projects/sro_sign_in/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E5828F-E824-6242-8124-964AFFF64DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1CF7972-DCD8-074F-9318-D763C905B913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{542D648B-9180-43EF-9053-182057C63D4C}"/>
+    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="3" xr2:uid="{542D648B-9180-43EF-9053-182057C63D4C}"/>
   </bookViews>
   <sheets>
     <sheet name="GTWCA" sheetId="10" r:id="rId1"/>
@@ -20,11 +20,11 @@
     <sheet name="GR Cup" sheetId="8" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">'GR Cup'!$A$1:$H$40</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'GR Cup'!$A$1:$H$39</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">GTAM!$A$2:$J$33</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">GTWCA!$A$2:$N$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">GTWCA!$A$2:$N$34</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">PGT4A!$A$1:$N$41</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">TCAM!$A$1:$H$37</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">TCAM!$A$2:$H$37</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -1738,7 +1738,7 @@
     <xf numFmtId="0" fontId="23" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="56" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="490">
+  <cellXfs count="489">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2401,9 +2401,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5407,14 +5404,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>234678</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>7677</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>267225</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>277090</xdr:rowOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>277089</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5457,14 +5454,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>308972</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>332773</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>854364</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>461817</xdr:rowOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>461816</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5634,9 +5631,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{006C041B-C32A-5442-9D54-6FB0F2E1703A}" name="Table22" displayName="Table22" ref="A7:N28" totalsRowShown="0" headerRowDxfId="64" dataDxfId="62" headerRowBorderDxfId="63" tableBorderDxfId="61" totalsRowBorderDxfId="60">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:N29">
-    <sortCondition ref="B29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{006C041B-C32A-5442-9D54-6FB0F2E1703A}" name="Table22" displayName="Table22" ref="A6:N27" totalsRowShown="0" headerRowDxfId="64" dataDxfId="62" headerRowBorderDxfId="63" tableBorderDxfId="61" totalsRowBorderDxfId="60">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:N28">
+    <sortCondition ref="B28"/>
   </sortState>
   <tableColumns count="14">
     <tableColumn id="2" xr3:uid="{8EAC187A-4BC7-044D-A24C-EE683FF40EDC}" name="Series" dataDxfId="59" dataCellStyle="Neutral"/>
@@ -6024,694 +6021,694 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:X35"/>
+  <dimension ref="A2:X34"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="80" zoomScaleNormal="90" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView view="pageLayout" zoomScale="80" zoomScaleNormal="90" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="284" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" style="285" customWidth="1"/>
-    <col min="3" max="3" width="27.1640625" style="284" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" style="284" customWidth="1"/>
-    <col min="5" max="7" width="8.6640625" style="284" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" style="284" customWidth="1"/>
-    <col min="9" max="11" width="8.6640625" style="284" customWidth="1"/>
-    <col min="12" max="13" width="35.6640625" style="284" customWidth="1"/>
-    <col min="14" max="14" width="14.33203125" style="284" customWidth="1"/>
-    <col min="15" max="17" width="4.5" style="284"/>
-    <col min="18" max="19" width="8.6640625" style="284" customWidth="1"/>
-    <col min="20" max="20" width="10.6640625" style="284" customWidth="1"/>
-    <col min="21" max="24" width="8.6640625" style="284" customWidth="1"/>
-    <col min="25" max="16384" width="4.5" style="284"/>
+    <col min="1" max="1" width="10.6640625" style="283" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" style="284" customWidth="1"/>
+    <col min="3" max="3" width="27.1640625" style="283" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" style="283" customWidth="1"/>
+    <col min="5" max="7" width="8.6640625" style="283" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" style="283" customWidth="1"/>
+    <col min="9" max="11" width="8.6640625" style="283" customWidth="1"/>
+    <col min="12" max="13" width="35.6640625" style="283" customWidth="1"/>
+    <col min="14" max="14" width="14.33203125" style="283" customWidth="1"/>
+    <col min="15" max="17" width="4.5" style="283"/>
+    <col min="18" max="19" width="8.6640625" style="283" customWidth="1"/>
+    <col min="20" max="20" width="10.6640625" style="283" customWidth="1"/>
+    <col min="21" max="24" width="8.6640625" style="283" customWidth="1"/>
+    <col min="25" max="16384" width="4.5" style="283"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="483"/>
-      <c r="B2" s="483"/>
-      <c r="C2" s="483"/>
-      <c r="F2" s="235"/>
-      <c r="G2" s="235"/>
+      <c r="A2" s="482"/>
+      <c r="B2" s="482"/>
+      <c r="C2" s="482"/>
+      <c r="F2" s="234"/>
+      <c r="G2" s="234"/>
       <c r="H2" s="227"/>
-      <c r="I2" s="235"/>
-      <c r="J2" s="235"/>
-      <c r="M2" s="483"/>
-      <c r="N2" s="483"/>
+      <c r="I2" s="234"/>
+      <c r="J2" s="234"/>
+      <c r="M2" s="482"/>
+      <c r="N2" s="482"/>
     </row>
     <row r="3" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="483"/>
-      <c r="B3" s="483"/>
-      <c r="C3" s="483"/>
-      <c r="F3" s="235"/>
-      <c r="G3" s="235"/>
+      <c r="A3" s="482"/>
+      <c r="B3" s="482"/>
+      <c r="C3" s="482"/>
+      <c r="F3" s="234"/>
+      <c r="G3" s="234"/>
       <c r="H3" s="227" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="235"/>
-      <c r="J3" s="235"/>
-      <c r="M3" s="483"/>
-      <c r="N3" s="483"/>
+      <c r="I3" s="234"/>
+      <c r="J3" s="234"/>
+      <c r="M3" s="482"/>
+      <c r="N3" s="482"/>
     </row>
     <row r="4" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="483"/>
-      <c r="B4" s="483"/>
-      <c r="C4" s="483"/>
-      <c r="F4" s="235"/>
-      <c r="G4" s="235"/>
+      <c r="A4" s="482"/>
+      <c r="B4" s="482"/>
+      <c r="C4" s="482"/>
+      <c r="F4" s="234"/>
+      <c r="G4" s="234"/>
       <c r="H4" s="227"/>
-      <c r="I4" s="235"/>
-      <c r="J4" s="235"/>
-      <c r="M4" s="483"/>
-      <c r="N4" s="483"/>
-    </row>
-    <row r="6" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="R6" s="483" t="s">
+      <c r="I4" s="234"/>
+      <c r="J4" s="234"/>
+      <c r="M4" s="482"/>
+      <c r="N4" s="482"/>
+    </row>
+    <row r="5" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R5" s="482" t="s">
         <v>0</v>
       </c>
-      <c r="S6" s="483"/>
-      <c r="T6" s="483"/>
-      <c r="U6" s="483"/>
-      <c r="V6" s="483"/>
-      <c r="W6" s="483"/>
-      <c r="X6" s="483"/>
-    </row>
-    <row r="7" spans="1:24" ht="32.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="286" t="s">
+      <c r="S5" s="482"/>
+      <c r="T5" s="482"/>
+      <c r="U5" s="482"/>
+      <c r="V5" s="482"/>
+      <c r="W5" s="482"/>
+      <c r="X5" s="482"/>
+    </row>
+    <row r="6" spans="1:24" ht="32.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="285" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="286" t="s">
+      <c r="B6" s="285" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="286" t="s">
+      <c r="C6" s="285" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="286" t="s">
+      <c r="D6" s="285" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="286" t="s">
+      <c r="E6" s="285" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="286" t="s">
+      <c r="F6" s="285" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="286" t="s">
+      <c r="G6" s="285" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="286" t="s">
+      <c r="H6" s="285" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="286" t="s">
+      <c r="I6" s="285" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="286" t="s">
+      <c r="J6" s="285" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="286" t="s">
+      <c r="K6" s="285" t="s">
         <v>21</v>
       </c>
-      <c r="L7" s="287" t="s">
+      <c r="L6" s="286" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="286" t="s">
+      <c r="M6" s="285" t="s">
         <v>9</v>
       </c>
-      <c r="N7" s="288" t="s">
+      <c r="N6" s="287" t="s">
         <v>22</v>
       </c>
-      <c r="Q7" s="284" t="s">
+      <c r="Q6" s="283" t="s">
         <v>11</v>
       </c>
-      <c r="R7" s="289" t="s">
+      <c r="R6" s="288" t="s">
         <v>12</v>
       </c>
-      <c r="S7" s="290" t="s">
+      <c r="S6" s="289" t="s">
         <v>13</v>
       </c>
-      <c r="T7" s="291" t="s">
+      <c r="T6" s="290" t="s">
         <v>14</v>
       </c>
-      <c r="U7" s="291" t="s">
+      <c r="U6" s="290" t="s">
         <v>15</v>
       </c>
-      <c r="V7" s="291" t="s">
+      <c r="V6" s="290" t="s">
         <v>16</v>
       </c>
-      <c r="W7" s="291" t="s">
+      <c r="W6" s="290" t="s">
         <v>23</v>
       </c>
-      <c r="X7" s="291" t="s">
+      <c r="X6" s="290" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:24" s="298" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="292"/>
-      <c r="B8" s="293"/>
-      <c r="C8" s="292"/>
-      <c r="D8" s="292"/>
-      <c r="E8" s="292"/>
-      <c r="F8" s="292"/>
-      <c r="G8" s="292"/>
-      <c r="H8" s="292"/>
-      <c r="I8" s="292"/>
-      <c r="J8" s="292"/>
-      <c r="K8" s="292"/>
-      <c r="L8" s="292"/>
-      <c r="M8" s="292"/>
-      <c r="N8" s="294"/>
-      <c r="O8" s="295"/>
-      <c r="P8" s="295"/>
-      <c r="Q8" s="295"/>
-      <c r="R8" s="296"/>
-      <c r="S8" s="292"/>
-      <c r="T8" s="292"/>
-      <c r="U8" s="292"/>
-      <c r="V8" s="292"/>
-      <c r="W8" s="292"/>
-      <c r="X8" s="297"/>
-    </row>
-    <row r="9" spans="1:24" s="298" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="299"/>
-      <c r="B9" s="300"/>
+    <row r="7" spans="1:24" s="297" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="291"/>
+      <c r="B7" s="292"/>
+      <c r="C7" s="291"/>
+      <c r="D7" s="291"/>
+      <c r="E7" s="291"/>
+      <c r="F7" s="291"/>
+      <c r="G7" s="291"/>
+      <c r="H7" s="291"/>
+      <c r="I7" s="291"/>
+      <c r="J7" s="291"/>
+      <c r="K7" s="291"/>
+      <c r="L7" s="291"/>
+      <c r="M7" s="291"/>
+      <c r="N7" s="293"/>
+      <c r="O7" s="294"/>
+      <c r="P7" s="294"/>
+      <c r="Q7" s="294"/>
+      <c r="R7" s="295"/>
+      <c r="S7" s="291"/>
+      <c r="T7" s="291"/>
+      <c r="U7" s="291"/>
+      <c r="V7" s="291"/>
+      <c r="W7" s="291"/>
+      <c r="X7" s="296"/>
+    </row>
+    <row r="8" spans="1:24" s="297" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="298"/>
+      <c r="B8" s="299"/>
+      <c r="C8" s="300"/>
+      <c r="D8" s="300"/>
+      <c r="E8" s="300"/>
+      <c r="F8" s="301"/>
+      <c r="G8" s="301"/>
+      <c r="H8" s="301"/>
+      <c r="I8" s="301"/>
+      <c r="J8" s="302"/>
+      <c r="K8" s="301"/>
+      <c r="L8" s="303"/>
+      <c r="M8" s="304"/>
+      <c r="N8" s="305"/>
+      <c r="O8" s="294"/>
+      <c r="P8" s="294"/>
+      <c r="Q8" s="294"/>
+      <c r="R8" s="306"/>
+      <c r="S8" s="307"/>
+      <c r="T8" s="307"/>
+      <c r="U8" s="307"/>
+      <c r="V8" s="307"/>
+      <c r="W8" s="307"/>
+      <c r="X8" s="308"/>
+    </row>
+    <row r="9" spans="1:24" s="297" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="298"/>
+      <c r="B9" s="299"/>
       <c r="C9" s="301"/>
       <c r="D9" s="301"/>
       <c r="E9" s="301"/>
-      <c r="F9" s="302"/>
-      <c r="G9" s="302"/>
-      <c r="H9" s="302"/>
-      <c r="I9" s="302"/>
-      <c r="J9" s="303"/>
-      <c r="K9" s="302"/>
-      <c r="L9" s="304"/>
-      <c r="M9" s="305"/>
-      <c r="N9" s="306"/>
-      <c r="O9" s="295"/>
-      <c r="P9" s="295"/>
-      <c r="Q9" s="295"/>
-      <c r="R9" s="307"/>
-      <c r="S9" s="308"/>
-      <c r="T9" s="308"/>
-      <c r="U9" s="308"/>
-      <c r="V9" s="308"/>
-      <c r="W9" s="308"/>
-      <c r="X9" s="309"/>
-    </row>
-    <row r="10" spans="1:24" s="298" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="299"/>
-      <c r="B10" s="300"/>
-      <c r="C10" s="302"/>
-      <c r="D10" s="302"/>
-      <c r="E10" s="302"/>
-      <c r="F10" s="302"/>
-      <c r="G10" s="302"/>
-      <c r="H10" s="302"/>
-      <c r="I10" s="302"/>
-      <c r="J10" s="302"/>
-      <c r="K10" s="310"/>
-      <c r="L10" s="311"/>
-      <c r="M10" s="305"/>
-      <c r="N10" s="306"/>
-      <c r="O10" s="295"/>
-      <c r="P10" s="295"/>
-      <c r="Q10" s="295"/>
-      <c r="R10" s="307"/>
-      <c r="S10" s="308"/>
-      <c r="T10" s="308"/>
-      <c r="U10" s="308"/>
-      <c r="V10" s="308"/>
-      <c r="W10" s="308"/>
-      <c r="X10" s="309"/>
-    </row>
-    <row r="11" spans="1:24" s="322" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="312"/>
-      <c r="B11" s="313"/>
-      <c r="C11" s="314"/>
-      <c r="D11" s="315"/>
-      <c r="E11" s="315"/>
-      <c r="F11" s="316"/>
-      <c r="G11" s="317"/>
-      <c r="H11" s="317"/>
-      <c r="I11" s="317"/>
-      <c r="J11" s="316"/>
-      <c r="K11" s="318"/>
-      <c r="L11" s="319"/>
-      <c r="M11" s="320"/>
-      <c r="N11" s="321"/>
-      <c r="R11" s="323"/>
-      <c r="S11" s="324"/>
-      <c r="T11" s="324"/>
-      <c r="U11" s="324"/>
-      <c r="V11" s="324"/>
-      <c r="W11" s="324"/>
-      <c r="X11" s="325"/>
-    </row>
-    <row r="12" spans="1:24" s="298" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="326"/>
-      <c r="B12" s="327"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="328"/>
-      <c r="G12" s="328"/>
-      <c r="H12" s="328"/>
-      <c r="I12" s="328"/>
-      <c r="J12" s="328"/>
-      <c r="K12" s="328"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="329"/>
-      <c r="N12" s="330"/>
-      <c r="R12" s="331"/>
-      <c r="S12" s="332"/>
-      <c r="T12" s="332"/>
-      <c r="U12" s="332"/>
-      <c r="V12" s="332"/>
-      <c r="W12" s="332"/>
-      <c r="X12" s="333"/>
-    </row>
-    <row r="13" spans="1:24" s="298" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="292"/>
-      <c r="B13" s="292"/>
-      <c r="C13" s="292"/>
-      <c r="D13" s="292"/>
-      <c r="E13" s="292"/>
-      <c r="F13" s="292"/>
-      <c r="G13" s="292"/>
-      <c r="H13" s="292"/>
-      <c r="I13" s="292"/>
-      <c r="J13" s="292"/>
-      <c r="K13" s="292"/>
-      <c r="L13" s="292"/>
-      <c r="M13" s="292"/>
-      <c r="N13" s="292"/>
-      <c r="R13" s="331"/>
-      <c r="S13" s="332"/>
-      <c r="T13" s="332"/>
-      <c r="U13" s="332"/>
-      <c r="V13" s="332"/>
-      <c r="W13" s="332"/>
-      <c r="X13" s="333"/>
-    </row>
-    <row r="14" spans="1:24" s="298" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="334"/>
-      <c r="B14" s="335"/>
-      <c r="C14" s="336"/>
-      <c r="D14" s="336"/>
-      <c r="E14" s="336"/>
-      <c r="F14" s="303"/>
-      <c r="G14" s="303"/>
-      <c r="H14" s="303"/>
-      <c r="I14" s="303"/>
-      <c r="J14" s="303"/>
-      <c r="K14" s="337"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="338"/>
-      <c r="N14" s="339"/>
-      <c r="R14" s="340"/>
-      <c r="S14" s="341"/>
-      <c r="T14" s="341"/>
-      <c r="U14" s="341"/>
-      <c r="V14" s="341"/>
-      <c r="W14" s="341"/>
-      <c r="X14" s="342"/>
-    </row>
-    <row r="15" spans="1:24" s="298" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="292"/>
-      <c r="B15" s="292"/>
-      <c r="C15" s="292"/>
-      <c r="D15" s="292"/>
-      <c r="E15" s="292"/>
-      <c r="F15" s="292"/>
-      <c r="G15" s="292"/>
-      <c r="H15" s="292"/>
-      <c r="I15" s="292"/>
-      <c r="J15" s="292"/>
-      <c r="K15" s="292"/>
-      <c r="L15" s="292"/>
-      <c r="M15" s="292"/>
-      <c r="N15" s="292"/>
-      <c r="R15" s="340"/>
-      <c r="S15" s="341"/>
-      <c r="T15" s="341"/>
-      <c r="U15" s="341"/>
-      <c r="V15" s="341"/>
-      <c r="W15" s="341"/>
-      <c r="X15" s="342"/>
-    </row>
-    <row r="16" spans="1:24" s="322" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="299"/>
-      <c r="B16" s="162"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="328"/>
-      <c r="G16" s="303"/>
-      <c r="H16" s="162"/>
-      <c r="I16" s="328"/>
-      <c r="J16" s="328"/>
-      <c r="K16" s="328"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="162"/>
-      <c r="N16" s="343"/>
-      <c r="R16" s="344"/>
-      <c r="S16" s="345"/>
-      <c r="T16" s="345"/>
-      <c r="U16" s="345"/>
-      <c r="V16" s="345"/>
-      <c r="W16" s="345"/>
-      <c r="X16" s="346"/>
-    </row>
-    <row r="17" spans="1:24" s="351" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="347"/>
-      <c r="B17" s="335"/>
-      <c r="C17" s="336"/>
-      <c r="D17" s="348"/>
-      <c r="E17" s="303"/>
-      <c r="F17" s="303"/>
-      <c r="G17" s="349"/>
-      <c r="H17" s="348"/>
-      <c r="I17" s="336"/>
-      <c r="J17" s="303"/>
-      <c r="K17" s="337"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="350"/>
-      <c r="N17" s="321"/>
-      <c r="R17" s="352"/>
-      <c r="S17" s="353"/>
-      <c r="T17" s="353"/>
-      <c r="U17" s="353"/>
-      <c r="V17" s="353"/>
-      <c r="W17" s="353"/>
-      <c r="X17" s="354"/>
-    </row>
-    <row r="18" spans="1:24" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="355"/>
-      <c r="B18" s="292"/>
-      <c r="C18" s="292"/>
-      <c r="D18" s="292"/>
-      <c r="E18" s="292"/>
-      <c r="F18" s="292"/>
-      <c r="G18" s="292"/>
-      <c r="H18" s="292"/>
-      <c r="I18" s="292"/>
-      <c r="J18" s="292"/>
-      <c r="K18" s="292"/>
-      <c r="L18" s="292"/>
-      <c r="M18" s="292"/>
-      <c r="N18" s="292"/>
-      <c r="R18" s="356"/>
-      <c r="S18" s="357"/>
-      <c r="T18" s="357"/>
-      <c r="U18" s="357"/>
-      <c r="V18" s="357"/>
-      <c r="W18" s="357"/>
-      <c r="X18" s="358"/>
-    </row>
-    <row r="19" spans="1:24" s="365" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="334"/>
-      <c r="B19" s="335"/>
-      <c r="C19" s="359"/>
-      <c r="D19" s="360"/>
-      <c r="E19" s="336"/>
-      <c r="F19" s="303"/>
-      <c r="G19" s="303"/>
-      <c r="H19" s="361"/>
-      <c r="I19" s="303"/>
-      <c r="J19" s="303"/>
-      <c r="K19" s="303"/>
-      <c r="L19" s="362"/>
-      <c r="M19" s="363"/>
-      <c r="N19" s="364"/>
-      <c r="R19" s="366"/>
-      <c r="S19" s="367"/>
-      <c r="T19" s="367"/>
-      <c r="U19" s="367"/>
-      <c r="V19" s="367"/>
-      <c r="W19" s="367"/>
-      <c r="X19" s="368"/>
-    </row>
-    <row r="20" spans="1:24" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="299"/>
-      <c r="B20" s="300"/>
-      <c r="C20" s="369"/>
-      <c r="D20" s="301"/>
-      <c r="E20" s="301"/>
-      <c r="F20" s="302"/>
-      <c r="G20" s="370"/>
-      <c r="H20" s="302"/>
-      <c r="I20" s="302"/>
-      <c r="J20" s="302"/>
-      <c r="K20" s="310"/>
-      <c r="L20" s="304"/>
-      <c r="M20" s="371"/>
-      <c r="N20" s="372"/>
-      <c r="R20" s="356"/>
-      <c r="S20" s="357"/>
-      <c r="T20" s="357"/>
-      <c r="U20" s="357"/>
-      <c r="V20" s="357"/>
-      <c r="W20" s="357"/>
-      <c r="X20" s="358"/>
-    </row>
-    <row r="21" spans="1:24" s="150" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="326"/>
+      <c r="F9" s="301"/>
+      <c r="G9" s="301"/>
+      <c r="H9" s="301"/>
+      <c r="I9" s="301"/>
+      <c r="J9" s="301"/>
+      <c r="K9" s="309"/>
+      <c r="L9" s="310"/>
+      <c r="M9" s="304"/>
+      <c r="N9" s="305"/>
+      <c r="O9" s="294"/>
+      <c r="P9" s="294"/>
+      <c r="Q9" s="294"/>
+      <c r="R9" s="306"/>
+      <c r="S9" s="307"/>
+      <c r="T9" s="307"/>
+      <c r="U9" s="307"/>
+      <c r="V9" s="307"/>
+      <c r="W9" s="307"/>
+      <c r="X9" s="308"/>
+    </row>
+    <row r="10" spans="1:24" s="321" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="311"/>
+      <c r="B10" s="312"/>
+      <c r="C10" s="313"/>
+      <c r="D10" s="314"/>
+      <c r="E10" s="314"/>
+      <c r="F10" s="315"/>
+      <c r="G10" s="316"/>
+      <c r="H10" s="316"/>
+      <c r="I10" s="316"/>
+      <c r="J10" s="315"/>
+      <c r="K10" s="317"/>
+      <c r="L10" s="318"/>
+      <c r="M10" s="319"/>
+      <c r="N10" s="320"/>
+      <c r="R10" s="322"/>
+      <c r="S10" s="323"/>
+      <c r="T10" s="323"/>
+      <c r="U10" s="323"/>
+      <c r="V10" s="323"/>
+      <c r="W10" s="323"/>
+      <c r="X10" s="324"/>
+    </row>
+    <row r="11" spans="1:24" s="297" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="325"/>
+      <c r="B11" s="326"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="327"/>
+      <c r="G11" s="327"/>
+      <c r="H11" s="327"/>
+      <c r="I11" s="327"/>
+      <c r="J11" s="327"/>
+      <c r="K11" s="327"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="328"/>
+      <c r="N11" s="329"/>
+      <c r="R11" s="330"/>
+      <c r="S11" s="331"/>
+      <c r="T11" s="331"/>
+      <c r="U11" s="331"/>
+      <c r="V11" s="331"/>
+      <c r="W11" s="331"/>
+      <c r="X11" s="332"/>
+    </row>
+    <row r="12" spans="1:24" s="297" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="291"/>
+      <c r="B12" s="291"/>
+      <c r="C12" s="291"/>
+      <c r="D12" s="291"/>
+      <c r="E12" s="291"/>
+      <c r="F12" s="291"/>
+      <c r="G12" s="291"/>
+      <c r="H12" s="291"/>
+      <c r="I12" s="291"/>
+      <c r="J12" s="291"/>
+      <c r="K12" s="291"/>
+      <c r="L12" s="291"/>
+      <c r="M12" s="291"/>
+      <c r="N12" s="291"/>
+      <c r="R12" s="330"/>
+      <c r="S12" s="331"/>
+      <c r="T12" s="331"/>
+      <c r="U12" s="331"/>
+      <c r="V12" s="331"/>
+      <c r="W12" s="331"/>
+      <c r="X12" s="332"/>
+    </row>
+    <row r="13" spans="1:24" s="297" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="333"/>
+      <c r="B13" s="334"/>
+      <c r="C13" s="335"/>
+      <c r="D13" s="335"/>
+      <c r="E13" s="335"/>
+      <c r="F13" s="302"/>
+      <c r="G13" s="302"/>
+      <c r="H13" s="302"/>
+      <c r="I13" s="302"/>
+      <c r="J13" s="302"/>
+      <c r="K13" s="336"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="337"/>
+      <c r="N13" s="338"/>
+      <c r="R13" s="339"/>
+      <c r="S13" s="340"/>
+      <c r="T13" s="340"/>
+      <c r="U13" s="340"/>
+      <c r="V13" s="340"/>
+      <c r="W13" s="340"/>
+      <c r="X13" s="341"/>
+    </row>
+    <row r="14" spans="1:24" s="297" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="291"/>
+      <c r="B14" s="291"/>
+      <c r="C14" s="291"/>
+      <c r="D14" s="291"/>
+      <c r="E14" s="291"/>
+      <c r="F14" s="291"/>
+      <c r="G14" s="291"/>
+      <c r="H14" s="291"/>
+      <c r="I14" s="291"/>
+      <c r="J14" s="291"/>
+      <c r="K14" s="291"/>
+      <c r="L14" s="291"/>
+      <c r="M14" s="291"/>
+      <c r="N14" s="291"/>
+      <c r="R14" s="339"/>
+      <c r="S14" s="340"/>
+      <c r="T14" s="340"/>
+      <c r="U14" s="340"/>
+      <c r="V14" s="340"/>
+      <c r="W14" s="340"/>
+      <c r="X14" s="341"/>
+    </row>
+    <row r="15" spans="1:24" s="321" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="298"/>
+      <c r="B15" s="162"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="327"/>
+      <c r="G15" s="302"/>
+      <c r="H15" s="162"/>
+      <c r="I15" s="327"/>
+      <c r="J15" s="327"/>
+      <c r="K15" s="327"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="162"/>
+      <c r="N15" s="342"/>
+      <c r="R15" s="343"/>
+      <c r="S15" s="344"/>
+      <c r="T15" s="344"/>
+      <c r="U15" s="344"/>
+      <c r="V15" s="344"/>
+      <c r="W15" s="344"/>
+      <c r="X15" s="345"/>
+    </row>
+    <row r="16" spans="1:24" s="350" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="346"/>
+      <c r="B16" s="334"/>
+      <c r="C16" s="335"/>
+      <c r="D16" s="347"/>
+      <c r="E16" s="302"/>
+      <c r="F16" s="302"/>
+      <c r="G16" s="348"/>
+      <c r="H16" s="347"/>
+      <c r="I16" s="335"/>
+      <c r="J16" s="302"/>
+      <c r="K16" s="336"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="349"/>
+      <c r="N16" s="320"/>
+      <c r="R16" s="351"/>
+      <c r="S16" s="352"/>
+      <c r="T16" s="352"/>
+      <c r="U16" s="352"/>
+      <c r="V16" s="352"/>
+      <c r="W16" s="352"/>
+      <c r="X16" s="353"/>
+    </row>
+    <row r="17" spans="1:24" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="354"/>
+      <c r="B17" s="291"/>
+      <c r="C17" s="291"/>
+      <c r="D17" s="291"/>
+      <c r="E17" s="291"/>
+      <c r="F17" s="291"/>
+      <c r="G17" s="291"/>
+      <c r="H17" s="291"/>
+      <c r="I17" s="291"/>
+      <c r="J17" s="291"/>
+      <c r="K17" s="291"/>
+      <c r="L17" s="291"/>
+      <c r="M17" s="291"/>
+      <c r="N17" s="291"/>
+      <c r="R17" s="355"/>
+      <c r="S17" s="356"/>
+      <c r="T17" s="356"/>
+      <c r="U17" s="356"/>
+      <c r="V17" s="356"/>
+      <c r="W17" s="356"/>
+      <c r="X17" s="357"/>
+    </row>
+    <row r="18" spans="1:24" s="364" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="333"/>
+      <c r="B18" s="334"/>
+      <c r="C18" s="358"/>
+      <c r="D18" s="359"/>
+      <c r="E18" s="335"/>
+      <c r="F18" s="302"/>
+      <c r="G18" s="302"/>
+      <c r="H18" s="360"/>
+      <c r="I18" s="302"/>
+      <c r="J18" s="302"/>
+      <c r="K18" s="302"/>
+      <c r="L18" s="361"/>
+      <c r="M18" s="362"/>
+      <c r="N18" s="363"/>
+      <c r="R18" s="365"/>
+      <c r="S18" s="366"/>
+      <c r="T18" s="366"/>
+      <c r="U18" s="366"/>
+      <c r="V18" s="366"/>
+      <c r="W18" s="366"/>
+      <c r="X18" s="367"/>
+    </row>
+    <row r="19" spans="1:24" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="298"/>
+      <c r="B19" s="299"/>
+      <c r="C19" s="368"/>
+      <c r="D19" s="300"/>
+      <c r="E19" s="300"/>
+      <c r="F19" s="301"/>
+      <c r="G19" s="369"/>
+      <c r="H19" s="301"/>
+      <c r="I19" s="301"/>
+      <c r="J19" s="301"/>
+      <c r="K19" s="309"/>
+      <c r="L19" s="303"/>
+      <c r="M19" s="370"/>
+      <c r="N19" s="371"/>
+      <c r="R19" s="355"/>
+      <c r="S19" s="356"/>
+      <c r="T19" s="356"/>
+      <c r="U19" s="356"/>
+      <c r="V19" s="356"/>
+      <c r="W19" s="356"/>
+      <c r="X19" s="357"/>
+    </row>
+    <row r="20" spans="1:24" s="150" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="325"/>
+      <c r="B20" s="327"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="327"/>
+      <c r="G20" s="327"/>
+      <c r="H20" s="327"/>
+      <c r="I20" s="327"/>
+      <c r="J20" s="327"/>
+      <c r="K20" s="327"/>
+      <c r="L20" s="31"/>
+      <c r="M20" s="327"/>
+      <c r="N20" s="329"/>
+      <c r="R20" s="372"/>
+      <c r="S20" s="122"/>
+      <c r="T20" s="122"/>
+      <c r="U20" s="122"/>
+      <c r="V20" s="122"/>
+      <c r="W20" s="122"/>
+      <c r="X20" s="373"/>
+    </row>
+    <row r="21" spans="1:24" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="374"/>
       <c r="B21" s="328"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
+      <c r="C21" s="328"/>
+      <c r="D21" s="328"/>
+      <c r="E21" s="328"/>
       <c r="F21" s="328"/>
       <c r="G21" s="328"/>
       <c r="H21" s="328"/>
       <c r="I21" s="328"/>
       <c r="J21" s="328"/>
       <c r="K21" s="328"/>
-      <c r="L21" s="31"/>
+      <c r="L21" s="375"/>
       <c r="M21" s="328"/>
-      <c r="N21" s="330"/>
-      <c r="R21" s="373"/>
-      <c r="S21" s="122"/>
-      <c r="T21" s="122"/>
-      <c r="U21" s="122"/>
-      <c r="V21" s="122"/>
-      <c r="W21" s="122"/>
-      <c r="X21" s="374"/>
+      <c r="N21" s="328"/>
+      <c r="R21" s="355"/>
+      <c r="S21" s="356"/>
+      <c r="T21" s="356"/>
+      <c r="U21" s="356"/>
+      <c r="V21" s="356"/>
+      <c r="W21" s="356"/>
+      <c r="X21" s="357"/>
     </row>
     <row r="22" spans="1:24" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="375"/>
-      <c r="B22" s="329"/>
-      <c r="C22" s="329"/>
-      <c r="D22" s="329"/>
-      <c r="E22" s="329"/>
-      <c r="F22" s="329"/>
-      <c r="G22" s="329"/>
-      <c r="H22" s="329"/>
-      <c r="I22" s="329"/>
-      <c r="J22" s="329"/>
-      <c r="K22" s="329"/>
-      <c r="L22" s="376"/>
-      <c r="M22" s="329"/>
-      <c r="N22" s="329"/>
-      <c r="R22" s="356"/>
-      <c r="S22" s="357"/>
-      <c r="T22" s="357"/>
-      <c r="U22" s="357"/>
-      <c r="V22" s="357"/>
-      <c r="W22" s="357"/>
-      <c r="X22" s="358"/>
+      <c r="A22" s="374"/>
+      <c r="B22" s="376"/>
+      <c r="C22" s="377"/>
+      <c r="D22" s="377"/>
+      <c r="E22" s="377"/>
+      <c r="F22" s="377"/>
+      <c r="G22" s="377"/>
+      <c r="H22" s="377"/>
+      <c r="I22" s="377"/>
+      <c r="J22" s="377"/>
+      <c r="K22" s="328"/>
+      <c r="L22" s="375"/>
+      <c r="M22" s="328"/>
+      <c r="N22" s="377"/>
+      <c r="R22" s="355"/>
+      <c r="S22" s="356"/>
+      <c r="T22" s="356"/>
+      <c r="U22" s="356"/>
+      <c r="V22" s="356"/>
+      <c r="W22" s="356"/>
+      <c r="X22" s="357"/>
     </row>
     <row r="23" spans="1:24" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="375"/>
-      <c r="B23" s="377"/>
-      <c r="C23" s="378"/>
-      <c r="D23" s="378"/>
-      <c r="E23" s="378"/>
-      <c r="F23" s="378"/>
-      <c r="G23" s="378"/>
-      <c r="H23" s="378"/>
-      <c r="I23" s="378"/>
-      <c r="J23" s="378"/>
-      <c r="K23" s="329"/>
-      <c r="L23" s="376"/>
-      <c r="M23" s="329"/>
-      <c r="N23" s="378"/>
-      <c r="R23" s="356"/>
-      <c r="S23" s="357"/>
-      <c r="T23" s="357"/>
-      <c r="U23" s="357"/>
-      <c r="V23" s="357"/>
-      <c r="W23" s="357"/>
-      <c r="X23" s="358"/>
+      <c r="A23" s="374"/>
+      <c r="B23" s="376"/>
+      <c r="C23" s="377"/>
+      <c r="D23" s="377"/>
+      <c r="E23" s="377"/>
+      <c r="F23" s="377"/>
+      <c r="G23" s="377"/>
+      <c r="H23" s="377"/>
+      <c r="I23" s="377"/>
+      <c r="J23" s="377"/>
+      <c r="K23" s="328"/>
+      <c r="L23" s="375"/>
+      <c r="M23" s="328"/>
+      <c r="N23" s="377"/>
+      <c r="R23" s="355"/>
+      <c r="S23" s="356"/>
+      <c r="T23" s="356"/>
+      <c r="U23" s="356"/>
+      <c r="V23" s="356"/>
+      <c r="W23" s="356"/>
+      <c r="X23" s="357"/>
     </row>
     <row r="24" spans="1:24" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="375"/>
-      <c r="B24" s="377"/>
-      <c r="C24" s="378"/>
-      <c r="D24" s="378"/>
-      <c r="E24" s="378"/>
-      <c r="F24" s="378"/>
-      <c r="G24" s="378"/>
-      <c r="H24" s="378"/>
-      <c r="I24" s="378"/>
-      <c r="J24" s="378"/>
-      <c r="K24" s="329"/>
-      <c r="L24" s="376"/>
-      <c r="M24" s="329"/>
-      <c r="N24" s="378"/>
-      <c r="R24" s="356"/>
-      <c r="S24" s="357"/>
-      <c r="T24" s="357"/>
-      <c r="U24" s="357"/>
-      <c r="V24" s="357"/>
-      <c r="W24" s="357"/>
-      <c r="X24" s="358"/>
+      <c r="A24" s="374"/>
+      <c r="B24" s="376"/>
+      <c r="C24" s="377"/>
+      <c r="D24" s="377"/>
+      <c r="E24" s="377"/>
+      <c r="F24" s="377"/>
+      <c r="G24" s="377"/>
+      <c r="H24" s="377"/>
+      <c r="I24" s="377"/>
+      <c r="J24" s="377"/>
+      <c r="K24" s="328"/>
+      <c r="L24" s="375"/>
+      <c r="M24" s="328"/>
+      <c r="N24" s="377"/>
+      <c r="R24" s="355"/>
+      <c r="S24" s="356"/>
+      <c r="T24" s="356"/>
+      <c r="U24" s="356"/>
+      <c r="V24" s="356"/>
+      <c r="W24" s="356"/>
+      <c r="X24" s="357"/>
     </row>
     <row r="25" spans="1:24" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="375"/>
-      <c r="B25" s="377"/>
-      <c r="C25" s="378"/>
-      <c r="D25" s="378"/>
-      <c r="E25" s="378"/>
-      <c r="F25" s="378"/>
-      <c r="G25" s="378"/>
-      <c r="H25" s="378"/>
-      <c r="I25" s="378"/>
-      <c r="J25" s="378"/>
-      <c r="K25" s="329"/>
-      <c r="L25" s="376"/>
-      <c r="M25" s="329"/>
-      <c r="N25" s="378"/>
-      <c r="R25" s="356"/>
-      <c r="S25" s="357"/>
-      <c r="T25" s="357"/>
-      <c r="U25" s="357"/>
-      <c r="V25" s="357"/>
-      <c r="W25" s="357"/>
-      <c r="X25" s="358"/>
+      <c r="A25" s="374"/>
+      <c r="B25" s="376"/>
+      <c r="C25" s="377"/>
+      <c r="D25" s="377"/>
+      <c r="E25" s="377"/>
+      <c r="F25" s="377"/>
+      <c r="G25" s="377"/>
+      <c r="H25" s="377"/>
+      <c r="I25" s="377"/>
+      <c r="J25" s="377"/>
+      <c r="K25" s="328"/>
+      <c r="L25" s="375"/>
+      <c r="M25" s="328"/>
+      <c r="N25" s="377"/>
+      <c r="R25" s="355"/>
+      <c r="S25" s="356"/>
+      <c r="T25" s="356"/>
+      <c r="U25" s="356"/>
+      <c r="V25" s="356"/>
+      <c r="W25" s="356"/>
+      <c r="X25" s="357"/>
     </row>
     <row r="26" spans="1:24" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="375"/>
-      <c r="B26" s="377"/>
-      <c r="C26" s="378"/>
-      <c r="D26" s="378"/>
-      <c r="E26" s="378"/>
-      <c r="F26" s="378"/>
-      <c r="G26" s="378"/>
-      <c r="H26" s="378"/>
-      <c r="I26" s="378"/>
-      <c r="J26" s="378"/>
-      <c r="K26" s="329"/>
-      <c r="L26" s="376"/>
-      <c r="M26" s="329"/>
-      <c r="N26" s="378"/>
-      <c r="R26" s="356"/>
-      <c r="S26" s="357"/>
-      <c r="T26" s="357"/>
-      <c r="U26" s="357"/>
-      <c r="V26" s="357"/>
-      <c r="W26" s="357"/>
-      <c r="X26" s="358"/>
-    </row>
-    <row r="27" spans="1:24" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="375"/>
-      <c r="B27" s="379"/>
-      <c r="C27" s="380"/>
-      <c r="D27" s="380"/>
-      <c r="E27" s="380"/>
-      <c r="F27" s="380"/>
-      <c r="G27" s="380"/>
-      <c r="H27" s="380"/>
-      <c r="I27" s="380"/>
-      <c r="J27" s="380"/>
-      <c r="K27" s="381"/>
-      <c r="L27" s="381"/>
-      <c r="M27" s="329"/>
-      <c r="N27" s="380"/>
-      <c r="R27" s="356"/>
-      <c r="S27" s="357"/>
-      <c r="T27" s="357"/>
-      <c r="U27" s="357"/>
-      <c r="V27" s="357"/>
-      <c r="W27" s="357"/>
-      <c r="X27" s="358"/>
-    </row>
-    <row r="28" spans="1:24" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="375"/>
-      <c r="B28" s="329"/>
-      <c r="C28" s="329"/>
-      <c r="D28" s="329"/>
-      <c r="E28" s="329"/>
-      <c r="F28" s="329"/>
-      <c r="G28" s="329"/>
-      <c r="H28" s="329"/>
-      <c r="I28" s="329"/>
-      <c r="J28" s="329"/>
-      <c r="K28" s="329"/>
-      <c r="L28" s="329"/>
-      <c r="M28" s="329"/>
-      <c r="N28" s="329"/>
-      <c r="R28" s="382"/>
-      <c r="S28" s="383"/>
-      <c r="T28" s="383"/>
-      <c r="U28" s="383"/>
-      <c r="V28" s="383"/>
-      <c r="W28" s="383"/>
-      <c r="X28" s="384"/>
-    </row>
-    <row r="29" spans="1:24" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="385"/>
-      <c r="B29" s="386"/>
-      <c r="C29" s="385"/>
-      <c r="D29" s="385"/>
-      <c r="E29" s="385"/>
-      <c r="F29" s="385"/>
-      <c r="G29" s="387"/>
-      <c r="H29" s="387"/>
-      <c r="I29" s="387"/>
-      <c r="J29" s="387"/>
-      <c r="K29" s="387"/>
-      <c r="L29" s="388"/>
-      <c r="M29" s="389"/>
-      <c r="N29" s="387"/>
-    </row>
-    <row r="30" spans="1:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="390" t="s">
+      <c r="A26" s="374"/>
+      <c r="B26" s="378"/>
+      <c r="C26" s="379"/>
+      <c r="D26" s="379"/>
+      <c r="E26" s="379"/>
+      <c r="F26" s="379"/>
+      <c r="G26" s="379"/>
+      <c r="H26" s="379"/>
+      <c r="I26" s="379"/>
+      <c r="J26" s="379"/>
+      <c r="K26" s="380"/>
+      <c r="L26" s="380"/>
+      <c r="M26" s="328"/>
+      <c r="N26" s="379"/>
+      <c r="R26" s="355"/>
+      <c r="S26" s="356"/>
+      <c r="T26" s="356"/>
+      <c r="U26" s="356"/>
+      <c r="V26" s="356"/>
+      <c r="W26" s="356"/>
+      <c r="X26" s="357"/>
+    </row>
+    <row r="27" spans="1:24" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="374"/>
+      <c r="B27" s="328"/>
+      <c r="C27" s="328"/>
+      <c r="D27" s="328"/>
+      <c r="E27" s="328"/>
+      <c r="F27" s="328"/>
+      <c r="G27" s="328"/>
+      <c r="H27" s="328"/>
+      <c r="I27" s="328"/>
+      <c r="J27" s="328"/>
+      <c r="K27" s="328"/>
+      <c r="L27" s="328"/>
+      <c r="M27" s="328"/>
+      <c r="N27" s="328"/>
+      <c r="R27" s="381"/>
+      <c r="S27" s="382"/>
+      <c r="T27" s="382"/>
+      <c r="U27" s="382"/>
+      <c r="V27" s="382"/>
+      <c r="W27" s="382"/>
+      <c r="X27" s="383"/>
+    </row>
+    <row r="28" spans="1:24" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="384"/>
+      <c r="B28" s="385"/>
+      <c r="C28" s="384"/>
+      <c r="D28" s="384"/>
+      <c r="E28" s="384"/>
+      <c r="F28" s="384"/>
+      <c r="G28" s="386"/>
+      <c r="H28" s="386"/>
+      <c r="I28" s="386"/>
+      <c r="J28" s="386"/>
+      <c r="K28" s="386"/>
+      <c r="L28" s="387"/>
+      <c r="M28" s="388"/>
+      <c r="N28" s="386"/>
+    </row>
+    <row r="29" spans="1:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="389" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="252">
-        <f>COUNTA(B8:B28)</f>
+      <c r="B29" s="251">
+        <f>COUNTA(B7:B27)</f>
         <v>0</v>
       </c>
-      <c r="C30" s="369"/>
-      <c r="D30" s="369"/>
-      <c r="E30" s="369"/>
-      <c r="F30" s="391"/>
-      <c r="G30" s="369"/>
-      <c r="H30" s="392"/>
-      <c r="I30" s="391"/>
-      <c r="J30" s="391"/>
-      <c r="K30" s="393"/>
-      <c r="L30" s="394"/>
-      <c r="M30" s="391"/>
-      <c r="N30" s="391"/>
-    </row>
-    <row r="31" spans="1:24" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="395"/>
-      <c r="B31" s="391"/>
-      <c r="C31" s="395"/>
-      <c r="D31" s="396"/>
-      <c r="E31" s="395"/>
-      <c r="F31" s="395"/>
-      <c r="G31" s="397"/>
-      <c r="H31" s="396"/>
-      <c r="I31" s="395"/>
-      <c r="J31" s="395"/>
-      <c r="K31" s="397"/>
-      <c r="L31" s="398"/>
-      <c r="M31" s="17"/>
-      <c r="N31" s="395"/>
-    </row>
-    <row r="35" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H35" s="284" t="s">
+      <c r="C29" s="368"/>
+      <c r="D29" s="368"/>
+      <c r="E29" s="368"/>
+      <c r="F29" s="390"/>
+      <c r="G29" s="368"/>
+      <c r="H29" s="391"/>
+      <c r="I29" s="390"/>
+      <c r="J29" s="390"/>
+      <c r="K29" s="392"/>
+      <c r="L29" s="393"/>
+      <c r="M29" s="390"/>
+      <c r="N29" s="390"/>
+    </row>
+    <row r="30" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="394"/>
+      <c r="B30" s="390"/>
+      <c r="C30" s="394"/>
+      <c r="D30" s="395"/>
+      <c r="E30" s="394"/>
+      <c r="F30" s="394"/>
+      <c r="G30" s="396"/>
+      <c r="H30" s="395"/>
+      <c r="I30" s="394"/>
+      <c r="J30" s="394"/>
+      <c r="K30" s="396"/>
+      <c r="L30" s="397"/>
+      <c r="M30" s="17"/>
+      <c r="N30" s="394"/>
+    </row>
+    <row r="34" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H34" s="283" t="s">
         <v>11</v>
       </c>
     </row>
@@ -6719,11 +6716,11 @@
   <mergeCells count="3">
     <mergeCell ref="A2:C4"/>
     <mergeCell ref="M2:N4"/>
-    <mergeCell ref="R6:X6"/>
+    <mergeCell ref="R5:X5"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.8"/>
-  <pageSetup scale="46" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="35" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;G</oddFooter>
   </headerFooter>
@@ -6743,7 +6740,7 @@
   <dimension ref="A2:R32"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6763,51 +6760,51 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="484"/>
-      <c r="B2" s="484"/>
-      <c r="C2" s="484"/>
-      <c r="D2" s="485"/>
-      <c r="E2" s="485"/>
-      <c r="F2" s="485"/>
-      <c r="G2" s="485"/>
-      <c r="H2" s="485"/>
-      <c r="I2" s="484"/>
-      <c r="J2" s="484"/>
+      <c r="A2" s="483"/>
+      <c r="B2" s="483"/>
+      <c r="C2" s="483"/>
+      <c r="D2" s="484"/>
+      <c r="E2" s="484"/>
+      <c r="F2" s="484"/>
+      <c r="G2" s="484"/>
+      <c r="H2" s="484"/>
+      <c r="I2" s="483"/>
+      <c r="J2" s="483"/>
     </row>
     <row r="3" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="484"/>
-      <c r="B3" s="484"/>
-      <c r="C3" s="484"/>
-      <c r="D3" s="485" t="s">
+      <c r="A3" s="483"/>
+      <c r="B3" s="483"/>
+      <c r="C3" s="483"/>
+      <c r="D3" s="484" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="485"/>
-      <c r="F3" s="485"/>
-      <c r="G3" s="485"/>
-      <c r="H3" s="485"/>
-      <c r="I3" s="484"/>
-      <c r="J3" s="484"/>
+      <c r="E3" s="484"/>
+      <c r="F3" s="484"/>
+      <c r="G3" s="484"/>
+      <c r="H3" s="484"/>
+      <c r="I3" s="483"/>
+      <c r="J3" s="483"/>
     </row>
     <row r="4" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="484"/>
-      <c r="B4" s="484"/>
-      <c r="C4" s="484"/>
-      <c r="D4" s="485"/>
-      <c r="E4" s="485"/>
-      <c r="F4" s="485"/>
-      <c r="G4" s="485"/>
-      <c r="H4" s="485"/>
-      <c r="I4" s="484"/>
-      <c r="J4" s="484"/>
+      <c r="A4" s="483"/>
+      <c r="B4" s="483"/>
+      <c r="C4" s="483"/>
+      <c r="D4" s="484"/>
+      <c r="E4" s="484"/>
+      <c r="F4" s="484"/>
+      <c r="G4" s="484"/>
+      <c r="H4" s="484"/>
+      <c r="I4" s="483"/>
+      <c r="J4" s="483"/>
     </row>
     <row r="5" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="N5" s="484" t="s">
+      <c r="N5" s="483" t="s">
         <v>0</v>
       </c>
-      <c r="O5" s="484"/>
-      <c r="P5" s="484"/>
-      <c r="Q5" s="484"/>
-      <c r="R5" s="484"/>
+      <c r="O5" s="483"/>
+      <c r="P5" s="483"/>
+      <c r="Q5" s="483"/>
+      <c r="R5" s="483"/>
     </row>
     <row r="6" spans="1:18" s="2" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -6843,7 +6840,7 @@
       <c r="M6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N6" s="254" t="s">
+      <c r="N6" s="253" t="s">
         <v>12</v>
       </c>
       <c r="O6" s="212" t="s">
@@ -6870,11 +6867,11 @@
       <c r="H7" s="73"/>
       <c r="I7" s="74"/>
       <c r="J7" s="71"/>
-      <c r="N7" s="255"/>
+      <c r="N7" s="254"/>
       <c r="O7" s="53"/>
       <c r="P7" s="55"/>
       <c r="Q7" s="55"/>
-      <c r="R7" s="256"/>
+      <c r="R7" s="255"/>
     </row>
     <row r="8" spans="1:18" s="52" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="48"/>
@@ -6887,11 +6884,11 @@
       <c r="H8" s="50"/>
       <c r="I8" s="50"/>
       <c r="J8" s="50"/>
-      <c r="N8" s="255"/>
+      <c r="N8" s="254"/>
       <c r="O8" s="53"/>
       <c r="P8" s="54"/>
       <c r="Q8" s="54"/>
-      <c r="R8" s="257"/>
+      <c r="R8" s="256"/>
     </row>
     <row r="9" spans="1:18" s="32" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="115"/>
@@ -6904,11 +6901,11 @@
       <c r="H9" s="148"/>
       <c r="I9" s="147"/>
       <c r="J9" s="174"/>
-      <c r="N9" s="258"/>
+      <c r="N9" s="257"/>
       <c r="O9" s="53"/>
       <c r="P9" s="33"/>
       <c r="Q9" s="33"/>
-      <c r="R9" s="259"/>
+      <c r="R9" s="258"/>
     </row>
     <row r="10" spans="1:18" s="32" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="114"/>
@@ -6921,11 +6918,11 @@
       <c r="H10" s="196"/>
       <c r="I10" s="162"/>
       <c r="J10" s="40"/>
-      <c r="N10" s="258"/>
+      <c r="N10" s="257"/>
       <c r="O10" s="53"/>
       <c r="P10" s="33"/>
       <c r="Q10" s="33"/>
-      <c r="R10" s="259"/>
+      <c r="R10" s="258"/>
     </row>
     <row r="11" spans="1:18" s="46" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="62"/>
@@ -6938,11 +6935,11 @@
       <c r="H11" s="65"/>
       <c r="I11" s="66"/>
       <c r="J11" s="61"/>
-      <c r="N11" s="258"/>
+      <c r="N11" s="257"/>
       <c r="O11" s="53"/>
       <c r="P11" s="47"/>
       <c r="Q11" s="47"/>
-      <c r="R11" s="260"/>
+      <c r="R11" s="259"/>
     </row>
     <row r="12" spans="1:18" s="46" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="62"/>
@@ -6955,11 +6952,11 @@
       <c r="H12" s="31"/>
       <c r="I12" s="41"/>
       <c r="J12" s="40"/>
-      <c r="N12" s="258"/>
+      <c r="N12" s="257"/>
       <c r="O12" s="53"/>
       <c r="P12" s="47"/>
       <c r="Q12" s="47"/>
-      <c r="R12" s="260"/>
+      <c r="R12" s="259"/>
     </row>
     <row r="13" spans="1:18" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="48"/>
@@ -6972,11 +6969,11 @@
       <c r="H13" s="50"/>
       <c r="I13" s="50"/>
       <c r="J13" s="50"/>
-      <c r="N13" s="261"/>
+      <c r="N13" s="260"/>
       <c r="O13" s="53"/>
       <c r="P13" s="145"/>
       <c r="Q13" s="146"/>
-      <c r="R13" s="262"/>
+      <c r="R13" s="261"/>
     </row>
     <row r="14" spans="1:18" s="150" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="115"/>
@@ -6989,11 +6986,11 @@
       <c r="H14" s="118"/>
       <c r="I14" s="116"/>
       <c r="J14" s="119"/>
-      <c r="N14" s="263"/>
+      <c r="N14" s="262"/>
       <c r="O14" s="53"/>
       <c r="P14" s="151"/>
       <c r="Q14" s="151"/>
-      <c r="R14" s="264"/>
+      <c r="R14" s="263"/>
     </row>
     <row r="15" spans="1:18" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="48"/>
@@ -7006,11 +7003,11 @@
       <c r="H15" s="57"/>
       <c r="I15" s="57"/>
       <c r="J15" s="57"/>
-      <c r="N15" s="255"/>
+      <c r="N15" s="254"/>
       <c r="O15" s="53"/>
       <c r="P15" s="55"/>
       <c r="Q15" s="55"/>
-      <c r="R15" s="256"/>
+      <c r="R15" s="255"/>
     </row>
     <row r="16" spans="1:18" s="120" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="48"/>
@@ -7023,11 +7020,11 @@
       <c r="H16" s="50"/>
       <c r="I16" s="61"/>
       <c r="J16" s="50"/>
-      <c r="N16" s="265"/>
+      <c r="N16" s="264"/>
       <c r="O16" s="53"/>
       <c r="P16" s="121"/>
       <c r="Q16" s="121"/>
-      <c r="R16" s="266"/>
+      <c r="R16" s="265"/>
     </row>
     <row r="17" spans="1:18" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="48"/>
@@ -7040,11 +7037,11 @@
       <c r="H17" s="69"/>
       <c r="I17" s="69"/>
       <c r="J17" s="50"/>
-      <c r="N17" s="255"/>
+      <c r="N17" s="254"/>
       <c r="O17" s="53"/>
       <c r="P17" s="58"/>
       <c r="Q17" s="58"/>
-      <c r="R17" s="267"/>
+      <c r="R17" s="266"/>
     </row>
     <row r="18" spans="1:18" s="52" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="48"/>
@@ -7057,11 +7054,11 @@
       <c r="H18" s="31"/>
       <c r="I18" s="41"/>
       <c r="J18" s="40"/>
-      <c r="N18" s="255"/>
+      <c r="N18" s="254"/>
       <c r="O18" s="53"/>
       <c r="P18" s="54"/>
       <c r="Q18" s="54"/>
-      <c r="R18" s="257"/>
+      <c r="R18" s="256"/>
     </row>
     <row r="19" spans="1:18" s="52" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="161"/>
@@ -7074,11 +7071,11 @@
       <c r="H19" s="31"/>
       <c r="I19" s="41"/>
       <c r="J19" s="40"/>
-      <c r="N19" s="268"/>
+      <c r="N19" s="267"/>
       <c r="O19" s="53"/>
       <c r="P19" s="220"/>
       <c r="Q19" s="220"/>
-      <c r="R19" s="269"/>
+      <c r="R19" s="268"/>
     </row>
     <row r="20" spans="1:18" s="52" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="111"/>
@@ -7091,11 +7088,11 @@
       <c r="H20" s="44"/>
       <c r="I20" s="41"/>
       <c r="J20" s="40"/>
-      <c r="N20" s="255"/>
+      <c r="N20" s="254"/>
       <c r="O20" s="53"/>
       <c r="P20" s="53"/>
       <c r="Q20" s="53"/>
-      <c r="R20" s="270"/>
+      <c r="R20" s="269"/>
     </row>
     <row r="21" spans="1:18" s="52" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="48"/>
@@ -7108,11 +7105,11 @@
       <c r="H21" s="79"/>
       <c r="I21" s="50"/>
       <c r="J21" s="56"/>
-      <c r="N21" s="261"/>
+      <c r="N21" s="260"/>
       <c r="O21" s="53"/>
       <c r="P21" s="221"/>
       <c r="Q21" s="221"/>
-      <c r="R21" s="271"/>
+      <c r="R21" s="270"/>
     </row>
     <row r="22" spans="1:18" s="34" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="115"/>
@@ -7125,11 +7122,11 @@
       <c r="H22" s="138"/>
       <c r="I22" s="124"/>
       <c r="J22" s="134"/>
-      <c r="N22" s="258"/>
+      <c r="N22" s="257"/>
       <c r="O22" s="53"/>
       <c r="P22" s="35"/>
       <c r="Q22" s="35"/>
-      <c r="R22" s="272"/>
+      <c r="R22" s="271"/>
     </row>
     <row r="23" spans="1:18" s="139" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="48"/>
@@ -7142,11 +7139,11 @@
       <c r="H23" s="86"/>
       <c r="I23" s="71"/>
       <c r="J23" s="40"/>
-      <c r="N23" s="255"/>
+      <c r="N23" s="254"/>
       <c r="O23" s="53"/>
       <c r="P23" s="140"/>
       <c r="Q23" s="140"/>
-      <c r="R23" s="273"/>
+      <c r="R23" s="272"/>
     </row>
     <row r="24" spans="1:18" s="34" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="115"/>
@@ -7159,11 +7156,11 @@
       <c r="H24" s="31"/>
       <c r="I24" s="41"/>
       <c r="J24" s="40"/>
-      <c r="N24" s="258"/>
+      <c r="N24" s="257"/>
       <c r="O24" s="53"/>
       <c r="P24" s="35"/>
       <c r="Q24" s="35"/>
-      <c r="R24" s="272"/>
+      <c r="R24" s="271"/>
     </row>
     <row r="25" spans="1:18" s="139" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="115"/>
@@ -7176,11 +7173,11 @@
       <c r="H25" s="143"/>
       <c r="I25" s="129"/>
       <c r="J25" s="222"/>
-      <c r="N25" s="255"/>
+      <c r="N25" s="254"/>
       <c r="O25" s="53"/>
       <c r="P25" s="140"/>
       <c r="Q25" s="140"/>
-      <c r="R25" s="273"/>
+      <c r="R25" s="272"/>
     </row>
     <row r="26" spans="1:18" s="52" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="48"/>
@@ -7193,11 +7190,11 @@
       <c r="H26" s="83"/>
       <c r="I26" s="84"/>
       <c r="J26" s="40"/>
-      <c r="N26" s="255"/>
+      <c r="N26" s="254"/>
       <c r="O26" s="53"/>
       <c r="P26" s="53"/>
       <c r="Q26" s="54"/>
-      <c r="R26" s="257"/>
+      <c r="R26" s="256"/>
     </row>
     <row r="27" spans="1:18" s="52" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="48"/>
@@ -7210,59 +7207,59 @@
       <c r="H27" s="59"/>
       <c r="I27" s="85"/>
       <c r="J27" s="77"/>
-      <c r="N27" s="255"/>
+      <c r="N27" s="254"/>
       <c r="O27" s="53"/>
       <c r="P27" s="54"/>
       <c r="Q27" s="54"/>
-      <c r="R27" s="257"/>
+      <c r="R27" s="256"/>
     </row>
     <row r="28" spans="1:18" s="135" customFormat="1" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="237"/>
-      <c r="B28" s="238"/>
-      <c r="C28" s="239"/>
-      <c r="D28" s="240"/>
-      <c r="E28" s="241"/>
-      <c r="F28" s="242"/>
-      <c r="G28" s="243"/>
+      <c r="A28" s="236"/>
+      <c r="B28" s="237"/>
+      <c r="C28" s="238"/>
+      <c r="D28" s="239"/>
+      <c r="E28" s="240"/>
+      <c r="F28" s="241"/>
+      <c r="G28" s="242"/>
       <c r="H28" s="133"/>
-      <c r="I28" s="244"/>
-      <c r="J28" s="245"/>
-      <c r="N28" s="274"/>
-      <c r="O28" s="275"/>
-      <c r="P28" s="276"/>
-      <c r="Q28" s="276"/>
-      <c r="R28" s="277"/>
+      <c r="I28" s="243"/>
+      <c r="J28" s="244"/>
+      <c r="N28" s="273"/>
+      <c r="O28" s="274"/>
+      <c r="P28" s="275"/>
+      <c r="Q28" s="275"/>
+      <c r="R28" s="276"/>
     </row>
     <row r="29" spans="1:18" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="246"/>
-      <c r="B29" s="247"/>
-      <c r="C29" s="248"/>
-      <c r="D29" s="248"/>
-      <c r="E29" s="248"/>
-      <c r="F29" s="234"/>
-      <c r="G29" s="248"/>
-      <c r="H29" s="248"/>
-      <c r="I29" s="248"/>
-      <c r="J29" s="248"/>
+      <c r="A29" s="245"/>
+      <c r="B29" s="246"/>
+      <c r="C29" s="247"/>
+      <c r="D29" s="247"/>
+      <c r="E29" s="247"/>
+      <c r="F29" s="233"/>
+      <c r="G29" s="247"/>
+      <c r="H29" s="247"/>
+      <c r="I29" s="247"/>
+      <c r="J29" s="247"/>
       <c r="N29" s="139"/>
       <c r="O29" s="52"/>
     </row>
     <row r="30" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="253" t="s">
+      <c r="A30" s="252" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="252">
+      <c r="B30" s="251">
         <f>COUNTA(B7:B28)</f>
         <v>0</v>
       </c>
-      <c r="C30" s="250"/>
-      <c r="D30" s="250"/>
-      <c r="E30" s="250"/>
-      <c r="F30" s="249"/>
-      <c r="G30" s="249"/>
-      <c r="H30" s="251"/>
-      <c r="I30" s="249"/>
-      <c r="J30" s="249"/>
+      <c r="C30" s="249"/>
+      <c r="D30" s="249"/>
+      <c r="E30" s="249"/>
+      <c r="F30" s="248"/>
+      <c r="G30" s="248"/>
+      <c r="H30" s="250"/>
+      <c r="I30" s="248"/>
+      <c r="J30" s="248"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" s="8"/>
@@ -7318,7 +7315,7 @@
   </sheetPr>
   <dimension ref="A2:Y40"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A4" zoomScale="80" zoomScaleNormal="115" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A2" zoomScale="80" zoomScaleNormal="115" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -7340,107 +7337,107 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="484"/>
-      <c r="B2" s="484"/>
-      <c r="C2" s="484"/>
-      <c r="D2" s="484"/>
-      <c r="E2" s="484"/>
-      <c r="F2" s="484"/>
-      <c r="G2" s="484"/>
-      <c r="H2" s="484"/>
-      <c r="I2" s="484"/>
-      <c r="J2" s="484"/>
-      <c r="K2" s="484"/>
-      <c r="L2" s="484"/>
-      <c r="M2" s="484"/>
-      <c r="N2" s="484"/>
+      <c r="A2" s="483"/>
+      <c r="B2" s="483"/>
+      <c r="C2" s="483"/>
+      <c r="D2" s="483"/>
+      <c r="E2" s="483"/>
+      <c r="F2" s="483"/>
+      <c r="G2" s="483"/>
+      <c r="H2" s="483"/>
+      <c r="I2" s="483"/>
+      <c r="J2" s="483"/>
+      <c r="K2" s="483"/>
+      <c r="L2" s="483"/>
+      <c r="M2" s="483"/>
+      <c r="N2" s="483"/>
     </row>
     <row r="3" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="484"/>
-      <c r="B3" s="484"/>
-      <c r="C3" s="484"/>
-      <c r="D3" s="487" t="s">
+      <c r="A3" s="483"/>
+      <c r="B3" s="483"/>
+      <c r="C3" s="483"/>
+      <c r="D3" s="486" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="487"/>
-      <c r="F3" s="487"/>
-      <c r="G3" s="487"/>
-      <c r="H3" s="487"/>
-      <c r="I3" s="487"/>
-      <c r="J3" s="487"/>
-      <c r="K3" s="487"/>
-      <c r="L3" s="487"/>
-      <c r="M3" s="484"/>
-      <c r="N3" s="484"/>
+      <c r="E3" s="486"/>
+      <c r="F3" s="486"/>
+      <c r="G3" s="486"/>
+      <c r="H3" s="486"/>
+      <c r="I3" s="486"/>
+      <c r="J3" s="486"/>
+      <c r="K3" s="486"/>
+      <c r="L3" s="486"/>
+      <c r="M3" s="483"/>
+      <c r="N3" s="483"/>
     </row>
     <row r="4" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="484"/>
-      <c r="B4" s="484"/>
-      <c r="C4" s="484"/>
-      <c r="D4" s="484"/>
-      <c r="E4" s="484"/>
-      <c r="F4" s="484"/>
-      <c r="G4" s="484"/>
-      <c r="H4" s="484"/>
-      <c r="I4" s="484"/>
-      <c r="J4" s="484"/>
-      <c r="K4" s="484"/>
-      <c r="L4" s="484"/>
-      <c r="M4" s="484"/>
-      <c r="N4" s="484"/>
+      <c r="A4" s="483"/>
+      <c r="B4" s="483"/>
+      <c r="C4" s="483"/>
+      <c r="D4" s="483"/>
+      <c r="E4" s="483"/>
+      <c r="F4" s="483"/>
+      <c r="G4" s="483"/>
+      <c r="H4" s="483"/>
+      <c r="I4" s="483"/>
+      <c r="J4" s="483"/>
+      <c r="K4" s="483"/>
+      <c r="L4" s="483"/>
+      <c r="M4" s="483"/>
+      <c r="N4" s="483"/>
     </row>
     <row r="5" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="R5" s="486" t="s">
+      <c r="R5" s="485" t="s">
         <v>0</v>
       </c>
-      <c r="S5" s="486"/>
-      <c r="T5" s="486"/>
-      <c r="U5" s="486"/>
-      <c r="V5" s="486"/>
-      <c r="W5" s="486"/>
-      <c r="X5" s="486"/>
+      <c r="S5" s="485"/>
+      <c r="T5" s="485"/>
+      <c r="U5" s="485"/>
+      <c r="V5" s="485"/>
+      <c r="W5" s="485"/>
+      <c r="X5" s="485"/>
     </row>
     <row r="6" spans="1:24" s="2" customFormat="1" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="281" t="s">
+      <c r="A6" s="280" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="281" t="s">
+      <c r="B6" s="280" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="281" t="s">
+      <c r="C6" s="280" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="281" t="s">
+      <c r="D6" s="280" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="281" t="s">
+      <c r="E6" s="280" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="281" t="s">
+      <c r="F6" s="280" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="281" t="s">
+      <c r="G6" s="280" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="281" t="s">
+      <c r="H6" s="280" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="281" t="s">
+      <c r="I6" s="280" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="281" t="s">
+      <c r="J6" s="280" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="281" t="s">
+      <c r="K6" s="280" t="s">
         <v>21</v>
       </c>
-      <c r="L6" s="282" t="s">
+      <c r="L6" s="281" t="s">
         <v>8</v>
       </c>
-      <c r="M6" s="281" t="s">
+      <c r="M6" s="280" t="s">
         <v>9</v>
       </c>
-      <c r="N6" s="283" t="s">
+      <c r="N6" s="282" t="s">
         <v>22</v>
       </c>
       <c r="Q6" s="2" t="s">
@@ -7469,20 +7466,20 @@
       </c>
     </row>
     <row r="7" spans="1:24" s="209" customFormat="1" ht="32.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="278"/>
-      <c r="B7" s="279"/>
-      <c r="C7" s="280"/>
-      <c r="D7" s="280"/>
-      <c r="E7" s="280"/>
-      <c r="F7" s="279"/>
-      <c r="G7" s="279"/>
-      <c r="H7" s="279"/>
-      <c r="I7" s="279"/>
-      <c r="J7" s="279"/>
-      <c r="K7" s="279"/>
-      <c r="L7" s="278"/>
-      <c r="M7" s="279"/>
-      <c r="N7" s="279"/>
+      <c r="A7" s="277"/>
+      <c r="B7" s="278"/>
+      <c r="C7" s="279"/>
+      <c r="D7" s="279"/>
+      <c r="E7" s="279"/>
+      <c r="F7" s="278"/>
+      <c r="G7" s="278"/>
+      <c r="H7" s="278"/>
+      <c r="I7" s="278"/>
+      <c r="J7" s="278"/>
+      <c r="K7" s="278"/>
+      <c r="L7" s="277"/>
+      <c r="M7" s="278"/>
+      <c r="N7" s="278"/>
       <c r="R7" s="29"/>
       <c r="S7" s="216"/>
       <c r="T7" s="29"/>
@@ -8182,7 +8179,7 @@
       <c r="X37" s="67"/>
     </row>
     <row r="38" spans="1:25" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="229"/>
+      <c r="A38" s="228"/>
       <c r="B38" s="86"/>
       <c r="C38" s="86"/>
       <c r="D38" s="86"/>
@@ -8190,7 +8187,7 @@
       <c r="F38" s="86"/>
       <c r="G38" s="86"/>
       <c r="H38" s="86"/>
-      <c r="I38" s="230"/>
+      <c r="I38" s="229"/>
       <c r="J38" s="86"/>
       <c r="K38" s="86"/>
       <c r="L38" s="86"/>
@@ -8206,23 +8203,23 @@
       <c r="Y38" s="141"/>
     </row>
     <row r="39" spans="1:25" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="231"/>
-      <c r="B39" s="232"/>
-      <c r="C39" s="231"/>
-      <c r="D39" s="233"/>
-      <c r="E39" s="233"/>
-      <c r="F39" s="233"/>
-      <c r="G39" s="233"/>
-      <c r="H39" s="234"/>
-      <c r="I39" s="234"/>
-      <c r="J39" s="234"/>
-      <c r="K39" s="234"/>
-      <c r="L39" s="231"/>
-      <c r="M39" s="234"/>
-      <c r="N39" s="234"/>
+      <c r="A39" s="230"/>
+      <c r="B39" s="231"/>
+      <c r="C39" s="230"/>
+      <c r="D39" s="232"/>
+      <c r="E39" s="232"/>
+      <c r="F39" s="232"/>
+      <c r="G39" s="232"/>
+      <c r="H39" s="233"/>
+      <c r="I39" s="233"/>
+      <c r="J39" s="233"/>
+      <c r="K39" s="233"/>
+      <c r="L39" s="230"/>
+      <c r="M39" s="233"/>
+      <c r="N39" s="233"/>
     </row>
     <row r="40" spans="1:25" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="236" t="s">
+      <c r="A40" s="235" t="s">
         <v>17</v>
       </c>
       <c r="B40" s="23">
@@ -8261,10 +8258,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BP36"/>
+  <dimension ref="A2:BP36"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScale="55" zoomScaleNormal="70" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="80" zoomScaleNormal="70" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8282,72 +8279,72 @@
     <col min="15" max="18" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="484"/>
-      <c r="B1" s="484"/>
-      <c r="C1" s="484"/>
-      <c r="D1" s="485"/>
-      <c r="E1" s="485"/>
-      <c r="F1" s="485"/>
-      <c r="G1" s="484"/>
-      <c r="H1" s="484"/>
-    </row>
     <row r="2" spans="1:68" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="484"/>
-      <c r="B2" s="484"/>
-      <c r="C2" s="484"/>
-      <c r="D2" s="485" t="s">
+      <c r="A2" s="483"/>
+      <c r="B2" s="483"/>
+      <c r="C2" s="483"/>
+      <c r="D2" s="484"/>
+      <c r="E2" s="484"/>
+      <c r="F2" s="484"/>
+      <c r="G2" s="483"/>
+      <c r="H2" s="483"/>
+    </row>
+    <row r="3" spans="1:68" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="483"/>
+      <c r="B3" s="483"/>
+      <c r="C3" s="483"/>
+      <c r="D3" s="484" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="485"/>
-      <c r="F2" s="485"/>
-      <c r="G2" s="484"/>
-      <c r="H2" s="484"/>
-    </row>
-    <row r="3" spans="1:68" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="484"/>
-      <c r="B3" s="484"/>
-      <c r="C3" s="484"/>
-      <c r="D3" s="485"/>
-      <c r="E3" s="485"/>
-      <c r="F3" s="485"/>
-      <c r="G3" s="484"/>
-      <c r="H3" s="484"/>
+      <c r="E3" s="484"/>
+      <c r="F3" s="484"/>
+      <c r="G3" s="483"/>
+      <c r="H3" s="483"/>
+    </row>
+    <row r="4" spans="1:68" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="483"/>
+      <c r="B4" s="483"/>
+      <c r="C4" s="483"/>
+      <c r="D4" s="484"/>
+      <c r="E4" s="484"/>
+      <c r="F4" s="484"/>
+      <c r="G4" s="483"/>
+      <c r="H4" s="483"/>
     </row>
     <row r="5" spans="1:68" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L5" s="484" t="s">
+      <c r="L5" s="483" t="s">
         <v>0</v>
       </c>
-      <c r="M5" s="484"/>
-      <c r="N5" s="484"/>
-      <c r="O5" s="484"/>
-      <c r="P5" s="484"/>
-      <c r="Q5" s="484"/>
-      <c r="R5" s="484"/>
+      <c r="M5" s="483"/>
+      <c r="N5" s="483"/>
+      <c r="O5" s="483"/>
+      <c r="P5" s="483"/>
+      <c r="Q5" s="483"/>
+      <c r="R5" s="483"/>
     </row>
     <row r="6" spans="1:68" s="10" customFormat="1" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="470" t="s">
+      <c r="A6" s="469" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="471" t="s">
+      <c r="B6" s="470" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="471" t="s">
+      <c r="C6" s="470" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="471" t="s">
+      <c r="D6" s="470" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="471" t="s">
+      <c r="E6" s="470" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="471" t="s">
+      <c r="F6" s="470" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="471" t="s">
+      <c r="G6" s="470" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="472" t="s">
+      <c r="H6" s="471" t="s">
         <v>10</v>
       </c>
       <c r="I6" s="25"/>
@@ -8355,19 +8352,19 @@
       <c r="K6" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="L6" s="399" t="s">
+      <c r="L6" s="398" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="400" t="s">
+      <c r="M6" s="399" t="s">
         <v>13</v>
       </c>
-      <c r="N6" s="400" t="s">
+      <c r="N6" s="399" t="s">
         <v>14</v>
       </c>
-      <c r="O6" s="400" t="s">
+      <c r="O6" s="399" t="s">
         <v>15</v>
       </c>
-      <c r="P6" s="401" t="s">
+      <c r="P6" s="400" t="s">
         <v>16</v>
       </c>
       <c r="Q6" s="3"/>
@@ -8424,39 +8421,39 @@
       <c r="BP6" s="26"/>
     </row>
     <row r="7" spans="1:68" s="25" customFormat="1" ht="46.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="473"/>
-      <c r="B7" s="464"/>
-      <c r="C7" s="465"/>
-      <c r="D7" s="466"/>
-      <c r="E7" s="465"/>
-      <c r="F7" s="465"/>
-      <c r="G7" s="465"/>
-      <c r="H7" s="467"/>
-      <c r="L7" s="402"/>
-      <c r="M7" s="403"/>
-      <c r="N7" s="404"/>
-      <c r="O7" s="404"/>
-      <c r="P7" s="405"/>
+      <c r="A7" s="472"/>
+      <c r="B7" s="463"/>
+      <c r="C7" s="464"/>
+      <c r="D7" s="465"/>
+      <c r="E7" s="464"/>
+      <c r="F7" s="464"/>
+      <c r="G7" s="464"/>
+      <c r="H7" s="466"/>
+      <c r="L7" s="401"/>
+      <c r="M7" s="402"/>
+      <c r="N7" s="403"/>
+      <c r="O7" s="403"/>
+      <c r="P7" s="404"/>
       <c r="Q7" s="110"/>
       <c r="R7" s="110"/>
     </row>
     <row r="8" spans="1:68" s="10" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="474"/>
-      <c r="B8" s="406"/>
-      <c r="C8" s="406"/>
-      <c r="D8" s="406"/>
-      <c r="E8" s="406"/>
-      <c r="F8" s="406"/>
-      <c r="G8" s="406"/>
-      <c r="H8" s="407"/>
+      <c r="A8" s="473"/>
+      <c r="B8" s="405"/>
+      <c r="C8" s="405"/>
+      <c r="D8" s="405"/>
+      <c r="E8" s="405"/>
+      <c r="F8" s="405"/>
+      <c r="G8" s="405"/>
+      <c r="H8" s="406"/>
       <c r="I8" s="25"/>
       <c r="J8" s="25"/>
       <c r="K8" s="25"/>
-      <c r="L8" s="408"/>
+      <c r="L8" s="407"/>
       <c r="M8" s="140"/>
       <c r="N8" s="67"/>
       <c r="O8" s="67"/>
-      <c r="P8" s="409"/>
+      <c r="P8" s="408"/>
       <c r="Q8" s="110"/>
       <c r="R8" s="110"/>
       <c r="S8" s="25"/>
@@ -8511,24 +8508,24 @@
       <c r="BP8" s="26"/>
     </row>
     <row r="9" spans="1:68" s="10" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="475"/>
-      <c r="B9" s="410"/>
-      <c r="C9" s="411"/>
-      <c r="D9" s="412"/>
-      <c r="E9" s="411"/>
-      <c r="F9" s="411"/>
-      <c r="G9" s="411"/>
-      <c r="H9" s="413"/>
-      <c r="I9" s="414"/>
-      <c r="J9" s="415"/>
-      <c r="K9" s="414"/>
-      <c r="L9" s="416"/>
-      <c r="M9" s="411"/>
-      <c r="N9" s="411"/>
-      <c r="O9" s="411"/>
-      <c r="P9" s="417"/>
-      <c r="Q9" s="414"/>
-      <c r="R9" s="415"/>
+      <c r="A9" s="474"/>
+      <c r="B9" s="409"/>
+      <c r="C9" s="410"/>
+      <c r="D9" s="411"/>
+      <c r="E9" s="410"/>
+      <c r="F9" s="410"/>
+      <c r="G9" s="410"/>
+      <c r="H9" s="412"/>
+      <c r="I9" s="413"/>
+      <c r="J9" s="414"/>
+      <c r="K9" s="413"/>
+      <c r="L9" s="415"/>
+      <c r="M9" s="410"/>
+      <c r="N9" s="410"/>
+      <c r="O9" s="410"/>
+      <c r="P9" s="416"/>
+      <c r="Q9" s="413"/>
+      <c r="R9" s="414"/>
       <c r="S9" s="25"/>
       <c r="T9" s="25"/>
       <c r="U9" s="25"/>
@@ -8581,22 +8578,22 @@
       <c r="BP9" s="26"/>
     </row>
     <row r="10" spans="1:68" s="10" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="475"/>
-      <c r="B10" s="410"/>
-      <c r="C10" s="411"/>
-      <c r="D10" s="412"/>
-      <c r="E10" s="412"/>
+      <c r="A10" s="474"/>
+      <c r="B10" s="409"/>
+      <c r="C10" s="410"/>
+      <c r="D10" s="411"/>
+      <c r="E10" s="411"/>
       <c r="F10" s="28"/>
       <c r="G10" s="28"/>
-      <c r="H10" s="413"/>
+      <c r="H10" s="412"/>
       <c r="I10" s="25"/>
       <c r="J10" s="25"/>
       <c r="K10" s="25"/>
-      <c r="L10" s="408"/>
+      <c r="L10" s="407"/>
       <c r="M10" s="140"/>
       <c r="N10" s="67"/>
       <c r="O10" s="67"/>
-      <c r="P10" s="409"/>
+      <c r="P10" s="408"/>
       <c r="Q10" s="110"/>
       <c r="R10" s="110"/>
       <c r="S10" s="25"/>
@@ -8651,22 +8648,22 @@
       <c r="BP10" s="26"/>
     </row>
     <row r="11" spans="1:68" s="10" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="475"/>
-      <c r="B11" s="418"/>
-      <c r="C11" s="411"/>
-      <c r="D11" s="412"/>
-      <c r="E11" s="411"/>
-      <c r="F11" s="411"/>
+      <c r="A11" s="474"/>
+      <c r="B11" s="417"/>
+      <c r="C11" s="410"/>
+      <c r="D11" s="411"/>
+      <c r="E11" s="410"/>
+      <c r="F11" s="410"/>
       <c r="G11" s="28"/>
-      <c r="H11" s="413"/>
+      <c r="H11" s="412"/>
       <c r="I11" s="25"/>
       <c r="J11" s="25"/>
       <c r="K11" s="25"/>
-      <c r="L11" s="408"/>
+      <c r="L11" s="407"/>
       <c r="M11" s="140"/>
       <c r="N11" s="67"/>
       <c r="O11" s="67"/>
-      <c r="P11" s="409"/>
+      <c r="P11" s="408"/>
       <c r="Q11" s="110"/>
       <c r="R11" s="110"/>
       <c r="S11" s="25"/>
@@ -8721,22 +8718,22 @@
       <c r="BP11" s="26"/>
     </row>
     <row r="12" spans="1:68" s="10" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="474"/>
-      <c r="B12" s="376"/>
-      <c r="C12" s="376"/>
-      <c r="D12" s="376"/>
-      <c r="E12" s="376"/>
-      <c r="F12" s="376"/>
-      <c r="G12" s="376"/>
-      <c r="H12" s="419"/>
+      <c r="A12" s="473"/>
+      <c r="B12" s="375"/>
+      <c r="C12" s="375"/>
+      <c r="D12" s="375"/>
+      <c r="E12" s="375"/>
+      <c r="F12" s="375"/>
+      <c r="G12" s="375"/>
+      <c r="H12" s="418"/>
       <c r="I12" s="25"/>
       <c r="J12" s="25"/>
       <c r="K12" s="25"/>
-      <c r="L12" s="408"/>
+      <c r="L12" s="407"/>
       <c r="M12" s="140"/>
       <c r="N12" s="67"/>
       <c r="O12" s="67"/>
-      <c r="P12" s="409"/>
+      <c r="P12" s="408"/>
       <c r="Q12" s="25"/>
       <c r="R12" s="25"/>
       <c r="S12" s="25"/>
@@ -8791,22 +8788,22 @@
       <c r="BP12" s="26"/>
     </row>
     <row r="13" spans="1:68" s="170" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="476"/>
-      <c r="B13" s="420"/>
-      <c r="C13" s="421"/>
-      <c r="D13" s="421"/>
-      <c r="E13" s="421"/>
-      <c r="F13" s="421"/>
-      <c r="G13" s="421"/>
-      <c r="H13" s="422"/>
+      <c r="A13" s="475"/>
+      <c r="B13" s="419"/>
+      <c r="C13" s="420"/>
+      <c r="D13" s="420"/>
+      <c r="E13" s="420"/>
+      <c r="F13" s="420"/>
+      <c r="G13" s="420"/>
+      <c r="H13" s="421"/>
       <c r="I13" s="167"/>
       <c r="J13" s="167"/>
       <c r="K13" s="167"/>
-      <c r="L13" s="408"/>
+      <c r="L13" s="407"/>
       <c r="M13" s="140"/>
       <c r="N13" s="168"/>
       <c r="O13" s="168"/>
-      <c r="P13" s="423"/>
+      <c r="P13" s="422"/>
       <c r="Q13" s="167"/>
       <c r="R13" s="167"/>
       <c r="S13" s="167"/>
@@ -8861,22 +8858,22 @@
       <c r="BP13" s="169"/>
     </row>
     <row r="14" spans="1:68" s="10" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="474"/>
-      <c r="B14" s="328"/>
+      <c r="A14" s="473"/>
+      <c r="B14" s="327"/>
       <c r="C14" s="30"/>
       <c r="D14" s="30"/>
       <c r="E14" s="30"/>
       <c r="F14" s="31"/>
-      <c r="G14" s="328"/>
-      <c r="H14" s="330"/>
+      <c r="G14" s="327"/>
+      <c r="H14" s="329"/>
       <c r="I14" s="25"/>
       <c r="J14" s="25"/>
       <c r="K14" s="25"/>
-      <c r="L14" s="408"/>
+      <c r="L14" s="407"/>
       <c r="M14" s="140"/>
       <c r="N14" s="67"/>
       <c r="O14" s="67"/>
-      <c r="P14" s="409"/>
+      <c r="P14" s="408"/>
       <c r="Q14" s="25"/>
       <c r="R14" s="25"/>
       <c r="S14" s="25"/>
@@ -8931,22 +8928,22 @@
       <c r="BP14" s="26"/>
     </row>
     <row r="15" spans="1:68" s="170" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="476"/>
+      <c r="A15" s="475"/>
       <c r="B15" s="162"/>
       <c r="C15" s="163"/>
       <c r="D15" s="163"/>
       <c r="E15" s="163"/>
       <c r="F15" s="183"/>
       <c r="G15" s="162"/>
-      <c r="H15" s="424"/>
+      <c r="H15" s="423"/>
       <c r="I15" s="167"/>
       <c r="J15" s="167"/>
       <c r="K15" s="167"/>
-      <c r="L15" s="408"/>
+      <c r="L15" s="407"/>
       <c r="M15" s="140"/>
       <c r="N15" s="168"/>
       <c r="O15" s="168"/>
-      <c r="P15" s="423"/>
+      <c r="P15" s="422"/>
       <c r="Q15" s="167"/>
       <c r="R15" s="167"/>
       <c r="S15" s="167"/>
@@ -9001,19 +8998,19 @@
       <c r="BP15" s="169"/>
     </row>
     <row r="16" spans="1:68" s="170" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="477"/>
-      <c r="B16" s="425"/>
-      <c r="C16" s="425"/>
-      <c r="D16" s="425"/>
-      <c r="E16" s="425"/>
-      <c r="F16" s="425"/>
-      <c r="G16" s="425"/>
-      <c r="H16" s="426"/>
+      <c r="A16" s="476"/>
+      <c r="B16" s="424"/>
+      <c r="C16" s="424"/>
+      <c r="D16" s="424"/>
+      <c r="E16" s="424"/>
+      <c r="F16" s="424"/>
+      <c r="G16" s="424"/>
+      <c r="H16" s="425"/>
       <c r="I16" s="167"/>
       <c r="J16" s="167"/>
       <c r="K16" s="167"/>
-      <c r="L16" s="427"/>
-      <c r="P16" s="428"/>
+      <c r="L16" s="426"/>
+      <c r="P16" s="427"/>
       <c r="Q16" s="167"/>
       <c r="R16" s="167"/>
       <c r="S16" s="167"/>
@@ -9068,19 +9065,19 @@
       <c r="BP16" s="169"/>
     </row>
     <row r="17" spans="1:68" s="170" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="478"/>
+      <c r="A17" s="477"/>
       <c r="B17" s="162"/>
       <c r="C17" s="163"/>
       <c r="D17" s="163"/>
       <c r="E17" s="163"/>
       <c r="F17" s="183"/>
       <c r="G17" s="162"/>
-      <c r="H17" s="424"/>
+      <c r="H17" s="423"/>
       <c r="I17" s="167"/>
       <c r="J17" s="167"/>
       <c r="K17" s="167"/>
-      <c r="L17" s="427"/>
-      <c r="P17" s="428"/>
+      <c r="L17" s="426"/>
+      <c r="P17" s="427"/>
       <c r="Q17" s="167"/>
       <c r="R17" s="167"/>
       <c r="S17" s="167"/>
@@ -9135,19 +9132,19 @@
       <c r="BP17" s="169"/>
     </row>
     <row r="18" spans="1:68" s="10" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="474"/>
-      <c r="B18" s="376"/>
-      <c r="C18" s="376"/>
-      <c r="D18" s="376"/>
-      <c r="E18" s="376"/>
-      <c r="F18" s="376"/>
-      <c r="G18" s="376"/>
-      <c r="H18" s="419"/>
+      <c r="A18" s="473"/>
+      <c r="B18" s="375"/>
+      <c r="C18" s="375"/>
+      <c r="D18" s="375"/>
+      <c r="E18" s="375"/>
+      <c r="F18" s="375"/>
+      <c r="G18" s="375"/>
+      <c r="H18" s="418"/>
       <c r="I18" s="25"/>
       <c r="J18" s="25"/>
       <c r="K18" s="25"/>
-      <c r="L18" s="429"/>
-      <c r="P18" s="430"/>
+      <c r="L18" s="428"/>
+      <c r="P18" s="429"/>
       <c r="Q18" s="25"/>
       <c r="R18" s="25"/>
       <c r="S18" s="25"/>
@@ -9202,19 +9199,19 @@
       <c r="BP18" s="26"/>
     </row>
     <row r="19" spans="1:68" s="10" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="474"/>
-      <c r="B19" s="376"/>
-      <c r="C19" s="376"/>
-      <c r="D19" s="376"/>
-      <c r="E19" s="376"/>
-      <c r="F19" s="376"/>
-      <c r="G19" s="376"/>
-      <c r="H19" s="419"/>
+      <c r="A19" s="473"/>
+      <c r="B19" s="375"/>
+      <c r="C19" s="375"/>
+      <c r="D19" s="375"/>
+      <c r="E19" s="375"/>
+      <c r="F19" s="375"/>
+      <c r="G19" s="375"/>
+      <c r="H19" s="418"/>
       <c r="I19" s="25"/>
       <c r="J19" s="25"/>
       <c r="K19" s="25"/>
-      <c r="L19" s="429"/>
-      <c r="P19" s="430"/>
+      <c r="L19" s="428"/>
+      <c r="P19" s="429"/>
       <c r="Q19" s="25"/>
       <c r="R19" s="25"/>
       <c r="S19" s="25"/>
@@ -9269,19 +9266,19 @@
       <c r="BP19" s="26"/>
     </row>
     <row r="20" spans="1:68" s="10" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="474"/>
-      <c r="B20" s="376"/>
-      <c r="C20" s="376"/>
-      <c r="D20" s="376"/>
-      <c r="E20" s="376"/>
-      <c r="F20" s="376"/>
-      <c r="G20" s="376"/>
-      <c r="H20" s="419"/>
+      <c r="A20" s="473"/>
+      <c r="B20" s="375"/>
+      <c r="C20" s="375"/>
+      <c r="D20" s="375"/>
+      <c r="E20" s="375"/>
+      <c r="F20" s="375"/>
+      <c r="G20" s="375"/>
+      <c r="H20" s="418"/>
       <c r="I20" s="25"/>
       <c r="J20" s="25"/>
       <c r="K20" s="25"/>
-      <c r="L20" s="429"/>
-      <c r="P20" s="430"/>
+      <c r="L20" s="428"/>
+      <c r="P20" s="429"/>
       <c r="Q20" s="25"/>
       <c r="R20" s="25"/>
       <c r="S20" s="25"/>
@@ -9336,19 +9333,19 @@
       <c r="BP20" s="26"/>
     </row>
     <row r="21" spans="1:68" s="10" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="476"/>
+      <c r="A21" s="475"/>
       <c r="B21" s="187"/>
       <c r="C21" s="181"/>
       <c r="D21" s="186"/>
       <c r="E21" s="186"/>
       <c r="F21" s="181"/>
       <c r="G21" s="187"/>
-      <c r="H21" s="431"/>
+      <c r="H21" s="430"/>
       <c r="I21" s="25"/>
       <c r="J21" s="25"/>
       <c r="K21" s="25"/>
-      <c r="L21" s="429"/>
-      <c r="P21" s="430"/>
+      <c r="L21" s="428"/>
+      <c r="P21" s="429"/>
       <c r="Q21" s="25"/>
       <c r="R21" s="25"/>
       <c r="S21" s="25"/>
@@ -9403,19 +9400,19 @@
       <c r="BP21" s="26"/>
     </row>
     <row r="22" spans="1:68" s="10" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="476"/>
-      <c r="B22" s="376"/>
-      <c r="C22" s="376"/>
-      <c r="D22" s="376"/>
-      <c r="E22" s="376"/>
-      <c r="F22" s="376"/>
-      <c r="G22" s="376"/>
-      <c r="H22" s="419"/>
+      <c r="A22" s="475"/>
+      <c r="B22" s="375"/>
+      <c r="C22" s="375"/>
+      <c r="D22" s="375"/>
+      <c r="E22" s="375"/>
+      <c r="F22" s="375"/>
+      <c r="G22" s="375"/>
+      <c r="H22" s="418"/>
       <c r="I22" s="25"/>
       <c r="J22" s="25"/>
       <c r="K22" s="25"/>
-      <c r="L22" s="429"/>
-      <c r="P22" s="430"/>
+      <c r="L22" s="428"/>
+      <c r="P22" s="429"/>
       <c r="Q22" s="25"/>
       <c r="R22" s="25"/>
       <c r="S22" s="25"/>
@@ -9470,19 +9467,19 @@
       <c r="BP22" s="26"/>
     </row>
     <row r="23" spans="1:68" s="10" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="474"/>
-      <c r="B23" s="328"/>
+      <c r="A23" s="473"/>
+      <c r="B23" s="327"/>
       <c r="C23" s="31"/>
       <c r="D23" s="30"/>
       <c r="E23" s="30"/>
       <c r="F23" s="31"/>
-      <c r="G23" s="328"/>
-      <c r="H23" s="330"/>
+      <c r="G23" s="327"/>
+      <c r="H23" s="329"/>
       <c r="I23" s="25"/>
       <c r="J23" s="25"/>
       <c r="K23" s="25"/>
-      <c r="L23" s="429"/>
-      <c r="P23" s="430"/>
+      <c r="L23" s="428"/>
+      <c r="P23" s="429"/>
       <c r="Q23" s="25"/>
       <c r="R23" s="25"/>
       <c r="S23" s="25"/>
@@ -9537,19 +9534,19 @@
       <c r="BP23" s="26"/>
     </row>
     <row r="24" spans="1:68" s="170" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="476"/>
+      <c r="A24" s="475"/>
       <c r="B24" s="191"/>
       <c r="C24" s="191"/>
       <c r="D24" s="191"/>
       <c r="E24" s="191"/>
       <c r="F24" s="191"/>
       <c r="G24" s="191"/>
-      <c r="H24" s="432"/>
+      <c r="H24" s="431"/>
       <c r="I24" s="167"/>
       <c r="J24" s="167"/>
       <c r="K24" s="167"/>
-      <c r="L24" s="427"/>
-      <c r="P24" s="428"/>
+      <c r="L24" s="426"/>
+      <c r="P24" s="427"/>
       <c r="Q24" s="167"/>
       <c r="R24" s="167"/>
       <c r="S24" s="167"/>
@@ -9604,19 +9601,19 @@
       <c r="BP24" s="169"/>
     </row>
     <row r="25" spans="1:68" s="10" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="474"/>
-      <c r="B25" s="376"/>
-      <c r="C25" s="376"/>
-      <c r="D25" s="376"/>
-      <c r="E25" s="376"/>
-      <c r="F25" s="376"/>
-      <c r="G25" s="376"/>
-      <c r="H25" s="419"/>
+      <c r="A25" s="473"/>
+      <c r="B25" s="375"/>
+      <c r="C25" s="375"/>
+      <c r="D25" s="375"/>
+      <c r="E25" s="375"/>
+      <c r="F25" s="375"/>
+      <c r="G25" s="375"/>
+      <c r="H25" s="418"/>
       <c r="I25" s="25"/>
       <c r="J25" s="25"/>
       <c r="K25" s="25"/>
-      <c r="L25" s="429"/>
-      <c r="P25" s="430"/>
+      <c r="L25" s="428"/>
+      <c r="P25" s="429"/>
       <c r="Q25" s="25"/>
       <c r="R25" s="25"/>
       <c r="S25" s="25"/>
@@ -9670,422 +9667,422 @@
       <c r="BO25" s="25"/>
       <c r="BP25" s="26"/>
     </row>
-    <row r="26" spans="1:68" s="435" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="474"/>
-      <c r="B26" s="376"/>
-      <c r="C26" s="376"/>
-      <c r="D26" s="376"/>
-      <c r="E26" s="376"/>
-      <c r="F26" s="376"/>
-      <c r="G26" s="376"/>
-      <c r="H26" s="419"/>
-      <c r="I26" s="433"/>
-      <c r="J26" s="433"/>
-      <c r="K26" s="433"/>
-      <c r="L26" s="434"/>
-      <c r="P26" s="436"/>
-      <c r="Q26" s="433"/>
-      <c r="R26" s="433"/>
-      <c r="S26" s="433"/>
-      <c r="T26" s="433"/>
-      <c r="U26" s="433"/>
-      <c r="V26" s="433"/>
-      <c r="W26" s="433"/>
-      <c r="X26" s="433"/>
-      <c r="Y26" s="433"/>
-      <c r="Z26" s="433"/>
-      <c r="AA26" s="433"/>
-      <c r="AB26" s="433"/>
-      <c r="AC26" s="433"/>
-      <c r="AD26" s="433"/>
-      <c r="AE26" s="433"/>
-      <c r="AF26" s="433"/>
-      <c r="AG26" s="433"/>
-      <c r="AH26" s="433"/>
-      <c r="AI26" s="433"/>
-      <c r="AJ26" s="433"/>
-      <c r="AK26" s="433"/>
-      <c r="AL26" s="433"/>
-      <c r="AM26" s="433"/>
-      <c r="AN26" s="433"/>
-      <c r="AO26" s="433"/>
-      <c r="AP26" s="433"/>
-      <c r="AQ26" s="433"/>
-      <c r="AR26" s="433"/>
-      <c r="AS26" s="433"/>
-      <c r="AT26" s="433"/>
-      <c r="AU26" s="433"/>
-      <c r="AV26" s="433"/>
-      <c r="AW26" s="433"/>
-      <c r="AX26" s="433"/>
-      <c r="AY26" s="433"/>
-      <c r="AZ26" s="433"/>
-      <c r="BA26" s="433"/>
-      <c r="BB26" s="433"/>
-      <c r="BC26" s="433"/>
-      <c r="BD26" s="433"/>
-      <c r="BE26" s="433"/>
-      <c r="BF26" s="433"/>
-      <c r="BG26" s="433"/>
-      <c r="BH26" s="433"/>
-      <c r="BI26" s="433"/>
-      <c r="BJ26" s="433"/>
-      <c r="BK26" s="433"/>
-      <c r="BL26" s="433"/>
-      <c r="BM26" s="433"/>
-      <c r="BN26" s="433"/>
-      <c r="BO26" s="433"/>
-      <c r="BP26" s="437"/>
-    </row>
-    <row r="27" spans="1:68" s="435" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="479"/>
-      <c r="B27" s="328"/>
+    <row r="26" spans="1:68" s="434" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="473"/>
+      <c r="B26" s="375"/>
+      <c r="C26" s="375"/>
+      <c r="D26" s="375"/>
+      <c r="E26" s="375"/>
+      <c r="F26" s="375"/>
+      <c r="G26" s="375"/>
+      <c r="H26" s="418"/>
+      <c r="I26" s="432"/>
+      <c r="J26" s="432"/>
+      <c r="K26" s="432"/>
+      <c r="L26" s="433"/>
+      <c r="P26" s="435"/>
+      <c r="Q26" s="432"/>
+      <c r="R26" s="432"/>
+      <c r="S26" s="432"/>
+      <c r="T26" s="432"/>
+      <c r="U26" s="432"/>
+      <c r="V26" s="432"/>
+      <c r="W26" s="432"/>
+      <c r="X26" s="432"/>
+      <c r="Y26" s="432"/>
+      <c r="Z26" s="432"/>
+      <c r="AA26" s="432"/>
+      <c r="AB26" s="432"/>
+      <c r="AC26" s="432"/>
+      <c r="AD26" s="432"/>
+      <c r="AE26" s="432"/>
+      <c r="AF26" s="432"/>
+      <c r="AG26" s="432"/>
+      <c r="AH26" s="432"/>
+      <c r="AI26" s="432"/>
+      <c r="AJ26" s="432"/>
+      <c r="AK26" s="432"/>
+      <c r="AL26" s="432"/>
+      <c r="AM26" s="432"/>
+      <c r="AN26" s="432"/>
+      <c r="AO26" s="432"/>
+      <c r="AP26" s="432"/>
+      <c r="AQ26" s="432"/>
+      <c r="AR26" s="432"/>
+      <c r="AS26" s="432"/>
+      <c r="AT26" s="432"/>
+      <c r="AU26" s="432"/>
+      <c r="AV26" s="432"/>
+      <c r="AW26" s="432"/>
+      <c r="AX26" s="432"/>
+      <c r="AY26" s="432"/>
+      <c r="AZ26" s="432"/>
+      <c r="BA26" s="432"/>
+      <c r="BB26" s="432"/>
+      <c r="BC26" s="432"/>
+      <c r="BD26" s="432"/>
+      <c r="BE26" s="432"/>
+      <c r="BF26" s="432"/>
+      <c r="BG26" s="432"/>
+      <c r="BH26" s="432"/>
+      <c r="BI26" s="432"/>
+      <c r="BJ26" s="432"/>
+      <c r="BK26" s="432"/>
+      <c r="BL26" s="432"/>
+      <c r="BM26" s="432"/>
+      <c r="BN26" s="432"/>
+      <c r="BO26" s="432"/>
+      <c r="BP26" s="436"/>
+    </row>
+    <row r="27" spans="1:68" s="434" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="478"/>
+      <c r="B27" s="327"/>
       <c r="C27" s="30"/>
       <c r="D27" s="30"/>
       <c r="E27" s="30"/>
       <c r="F27" s="31"/>
-      <c r="G27" s="328"/>
-      <c r="H27" s="330"/>
-      <c r="I27" s="433"/>
-      <c r="J27" s="433"/>
-      <c r="K27" s="433"/>
-      <c r="L27" s="434"/>
-      <c r="P27" s="436"/>
-      <c r="Q27" s="433"/>
-      <c r="R27" s="433"/>
-      <c r="S27" s="433"/>
-      <c r="T27" s="433"/>
-      <c r="U27" s="433"/>
-      <c r="V27" s="433"/>
-      <c r="W27" s="433"/>
-      <c r="X27" s="433"/>
-      <c r="Y27" s="433"/>
-      <c r="Z27" s="433"/>
-      <c r="AA27" s="433"/>
-      <c r="AB27" s="433"/>
-      <c r="AC27" s="433"/>
-      <c r="AD27" s="433"/>
-      <c r="AE27" s="433"/>
-      <c r="AF27" s="433"/>
-      <c r="AG27" s="433"/>
-      <c r="AH27" s="433"/>
-      <c r="AI27" s="433"/>
-      <c r="AJ27" s="433"/>
-      <c r="AK27" s="433"/>
-      <c r="AL27" s="433"/>
-      <c r="AM27" s="433"/>
-      <c r="AN27" s="433"/>
-      <c r="AO27" s="433"/>
-      <c r="AP27" s="433"/>
-      <c r="AQ27" s="433"/>
-      <c r="AR27" s="433"/>
-      <c r="AS27" s="433"/>
-      <c r="AT27" s="433"/>
-      <c r="AU27" s="433"/>
-      <c r="AV27" s="433"/>
-      <c r="AW27" s="433"/>
-      <c r="AX27" s="433"/>
-      <c r="AY27" s="433"/>
-      <c r="AZ27" s="433"/>
-      <c r="BA27" s="433"/>
-      <c r="BB27" s="433"/>
-      <c r="BC27" s="433"/>
-      <c r="BD27" s="433"/>
-      <c r="BE27" s="433"/>
-      <c r="BF27" s="433"/>
-      <c r="BG27" s="433"/>
-      <c r="BH27" s="433"/>
-      <c r="BI27" s="433"/>
-      <c r="BJ27" s="433"/>
-      <c r="BK27" s="433"/>
-      <c r="BL27" s="433"/>
-      <c r="BM27" s="433"/>
-      <c r="BN27" s="433"/>
-      <c r="BO27" s="433"/>
-      <c r="BP27" s="437"/>
-    </row>
-    <row r="28" spans="1:68" s="435" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="480"/>
-      <c r="B28" s="328"/>
+      <c r="G27" s="327"/>
+      <c r="H27" s="329"/>
+      <c r="I27" s="432"/>
+      <c r="J27" s="432"/>
+      <c r="K27" s="432"/>
+      <c r="L27" s="433"/>
+      <c r="P27" s="435"/>
+      <c r="Q27" s="432"/>
+      <c r="R27" s="432"/>
+      <c r="S27" s="432"/>
+      <c r="T27" s="432"/>
+      <c r="U27" s="432"/>
+      <c r="V27" s="432"/>
+      <c r="W27" s="432"/>
+      <c r="X27" s="432"/>
+      <c r="Y27" s="432"/>
+      <c r="Z27" s="432"/>
+      <c r="AA27" s="432"/>
+      <c r="AB27" s="432"/>
+      <c r="AC27" s="432"/>
+      <c r="AD27" s="432"/>
+      <c r="AE27" s="432"/>
+      <c r="AF27" s="432"/>
+      <c r="AG27" s="432"/>
+      <c r="AH27" s="432"/>
+      <c r="AI27" s="432"/>
+      <c r="AJ27" s="432"/>
+      <c r="AK27" s="432"/>
+      <c r="AL27" s="432"/>
+      <c r="AM27" s="432"/>
+      <c r="AN27" s="432"/>
+      <c r="AO27" s="432"/>
+      <c r="AP27" s="432"/>
+      <c r="AQ27" s="432"/>
+      <c r="AR27" s="432"/>
+      <c r="AS27" s="432"/>
+      <c r="AT27" s="432"/>
+      <c r="AU27" s="432"/>
+      <c r="AV27" s="432"/>
+      <c r="AW27" s="432"/>
+      <c r="AX27" s="432"/>
+      <c r="AY27" s="432"/>
+      <c r="AZ27" s="432"/>
+      <c r="BA27" s="432"/>
+      <c r="BB27" s="432"/>
+      <c r="BC27" s="432"/>
+      <c r="BD27" s="432"/>
+      <c r="BE27" s="432"/>
+      <c r="BF27" s="432"/>
+      <c r="BG27" s="432"/>
+      <c r="BH27" s="432"/>
+      <c r="BI27" s="432"/>
+      <c r="BJ27" s="432"/>
+      <c r="BK27" s="432"/>
+      <c r="BL27" s="432"/>
+      <c r="BM27" s="432"/>
+      <c r="BN27" s="432"/>
+      <c r="BO27" s="432"/>
+      <c r="BP27" s="436"/>
+    </row>
+    <row r="28" spans="1:68" s="434" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="479"/>
+      <c r="B28" s="327"/>
       <c r="C28" s="30"/>
       <c r="D28" s="30"/>
       <c r="E28" s="30"/>
       <c r="F28" s="31"/>
-      <c r="G28" s="328"/>
-      <c r="H28" s="330"/>
-      <c r="I28" s="433"/>
-      <c r="J28" s="433"/>
-      <c r="K28" s="433"/>
-      <c r="L28" s="434"/>
-      <c r="P28" s="436"/>
-      <c r="Q28" s="433"/>
-      <c r="R28" s="433"/>
-      <c r="S28" s="433"/>
-      <c r="T28" s="433"/>
-      <c r="U28" s="433"/>
-      <c r="V28" s="433"/>
-      <c r="W28" s="433"/>
-      <c r="X28" s="433"/>
-      <c r="Y28" s="433"/>
-      <c r="Z28" s="433"/>
-      <c r="AA28" s="433"/>
-      <c r="AB28" s="433"/>
-      <c r="AC28" s="433"/>
-      <c r="AD28" s="433"/>
-      <c r="AE28" s="433"/>
-      <c r="AF28" s="433"/>
-      <c r="AG28" s="433"/>
-      <c r="AH28" s="433"/>
-      <c r="AI28" s="433"/>
-      <c r="AJ28" s="433"/>
-      <c r="AK28" s="433"/>
-      <c r="AL28" s="433"/>
-      <c r="AM28" s="433"/>
-      <c r="AN28" s="433"/>
-      <c r="AO28" s="433"/>
-      <c r="AP28" s="433"/>
-      <c r="AQ28" s="433"/>
-      <c r="AR28" s="433"/>
-      <c r="AS28" s="433"/>
-      <c r="AT28" s="433"/>
-      <c r="AU28" s="433"/>
-      <c r="AV28" s="433"/>
-      <c r="AW28" s="433"/>
-      <c r="AX28" s="433"/>
-      <c r="AY28" s="433"/>
-      <c r="AZ28" s="433"/>
-      <c r="BA28" s="433"/>
-      <c r="BB28" s="433"/>
-      <c r="BC28" s="433"/>
-      <c r="BD28" s="433"/>
-      <c r="BE28" s="433"/>
-      <c r="BF28" s="433"/>
-      <c r="BG28" s="433"/>
-      <c r="BH28" s="433"/>
-      <c r="BI28" s="433"/>
-      <c r="BJ28" s="433"/>
-      <c r="BK28" s="433"/>
-      <c r="BL28" s="433"/>
-      <c r="BM28" s="433"/>
-      <c r="BN28" s="433"/>
-      <c r="BO28" s="433"/>
-      <c r="BP28" s="437"/>
-    </row>
-    <row r="29" spans="1:68" s="435" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="480"/>
-      <c r="B29" s="328"/>
+      <c r="G28" s="327"/>
+      <c r="H28" s="329"/>
+      <c r="I28" s="432"/>
+      <c r="J28" s="432"/>
+      <c r="K28" s="432"/>
+      <c r="L28" s="433"/>
+      <c r="P28" s="435"/>
+      <c r="Q28" s="432"/>
+      <c r="R28" s="432"/>
+      <c r="S28" s="432"/>
+      <c r="T28" s="432"/>
+      <c r="U28" s="432"/>
+      <c r="V28" s="432"/>
+      <c r="W28" s="432"/>
+      <c r="X28" s="432"/>
+      <c r="Y28" s="432"/>
+      <c r="Z28" s="432"/>
+      <c r="AA28" s="432"/>
+      <c r="AB28" s="432"/>
+      <c r="AC28" s="432"/>
+      <c r="AD28" s="432"/>
+      <c r="AE28" s="432"/>
+      <c r="AF28" s="432"/>
+      <c r="AG28" s="432"/>
+      <c r="AH28" s="432"/>
+      <c r="AI28" s="432"/>
+      <c r="AJ28" s="432"/>
+      <c r="AK28" s="432"/>
+      <c r="AL28" s="432"/>
+      <c r="AM28" s="432"/>
+      <c r="AN28" s="432"/>
+      <c r="AO28" s="432"/>
+      <c r="AP28" s="432"/>
+      <c r="AQ28" s="432"/>
+      <c r="AR28" s="432"/>
+      <c r="AS28" s="432"/>
+      <c r="AT28" s="432"/>
+      <c r="AU28" s="432"/>
+      <c r="AV28" s="432"/>
+      <c r="AW28" s="432"/>
+      <c r="AX28" s="432"/>
+      <c r="AY28" s="432"/>
+      <c r="AZ28" s="432"/>
+      <c r="BA28" s="432"/>
+      <c r="BB28" s="432"/>
+      <c r="BC28" s="432"/>
+      <c r="BD28" s="432"/>
+      <c r="BE28" s="432"/>
+      <c r="BF28" s="432"/>
+      <c r="BG28" s="432"/>
+      <c r="BH28" s="432"/>
+      <c r="BI28" s="432"/>
+      <c r="BJ28" s="432"/>
+      <c r="BK28" s="432"/>
+      <c r="BL28" s="432"/>
+      <c r="BM28" s="432"/>
+      <c r="BN28" s="432"/>
+      <c r="BO28" s="432"/>
+      <c r="BP28" s="436"/>
+    </row>
+    <row r="29" spans="1:68" s="434" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="479"/>
+      <c r="B29" s="327"/>
       <c r="C29" s="30"/>
       <c r="D29" s="30"/>
       <c r="E29" s="30"/>
       <c r="F29" s="31"/>
-      <c r="G29" s="328"/>
-      <c r="H29" s="330"/>
-      <c r="I29" s="433"/>
-      <c r="J29" s="433"/>
-      <c r="K29" s="433"/>
-      <c r="L29" s="434"/>
-      <c r="P29" s="436"/>
-      <c r="Q29" s="433"/>
-      <c r="R29" s="433"/>
-      <c r="S29" s="433"/>
-      <c r="T29" s="433"/>
-      <c r="U29" s="433"/>
-      <c r="V29" s="433"/>
-      <c r="W29" s="433"/>
-      <c r="X29" s="433"/>
-      <c r="Y29" s="433"/>
-      <c r="Z29" s="433"/>
-      <c r="AA29" s="433"/>
-      <c r="AB29" s="433"/>
-      <c r="AC29" s="433"/>
-      <c r="AD29" s="433"/>
-      <c r="AE29" s="433"/>
-      <c r="AF29" s="433"/>
-      <c r="AG29" s="433"/>
-      <c r="AH29" s="433"/>
-      <c r="AI29" s="433"/>
-      <c r="AJ29" s="433"/>
-      <c r="AK29" s="433"/>
-      <c r="AL29" s="433"/>
-      <c r="AM29" s="433"/>
-      <c r="AN29" s="433"/>
-      <c r="AO29" s="433"/>
-      <c r="AP29" s="433"/>
-      <c r="AQ29" s="433"/>
-      <c r="AR29" s="433"/>
-      <c r="AS29" s="433"/>
-      <c r="AT29" s="433"/>
-      <c r="AU29" s="433"/>
-      <c r="AV29" s="433"/>
-      <c r="AW29" s="433"/>
-      <c r="AX29" s="433"/>
-      <c r="AY29" s="433"/>
-      <c r="AZ29" s="433"/>
-      <c r="BA29" s="433"/>
-      <c r="BB29" s="433"/>
-      <c r="BC29" s="433"/>
-      <c r="BD29" s="433"/>
-      <c r="BE29" s="433"/>
-      <c r="BF29" s="433"/>
-      <c r="BG29" s="433"/>
-      <c r="BH29" s="433"/>
-      <c r="BI29" s="433"/>
-      <c r="BJ29" s="433"/>
-      <c r="BK29" s="433"/>
-      <c r="BL29" s="433"/>
-      <c r="BM29" s="433"/>
-      <c r="BN29" s="433"/>
-      <c r="BO29" s="433"/>
-      <c r="BP29" s="437"/>
-    </row>
-    <row r="30" spans="1:68" s="435" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="480"/>
-      <c r="B30" s="328"/>
+      <c r="G29" s="327"/>
+      <c r="H29" s="329"/>
+      <c r="I29" s="432"/>
+      <c r="J29" s="432"/>
+      <c r="K29" s="432"/>
+      <c r="L29" s="433"/>
+      <c r="P29" s="435"/>
+      <c r="Q29" s="432"/>
+      <c r="R29" s="432"/>
+      <c r="S29" s="432"/>
+      <c r="T29" s="432"/>
+      <c r="U29" s="432"/>
+      <c r="V29" s="432"/>
+      <c r="W29" s="432"/>
+      <c r="X29" s="432"/>
+      <c r="Y29" s="432"/>
+      <c r="Z29" s="432"/>
+      <c r="AA29" s="432"/>
+      <c r="AB29" s="432"/>
+      <c r="AC29" s="432"/>
+      <c r="AD29" s="432"/>
+      <c r="AE29" s="432"/>
+      <c r="AF29" s="432"/>
+      <c r="AG29" s="432"/>
+      <c r="AH29" s="432"/>
+      <c r="AI29" s="432"/>
+      <c r="AJ29" s="432"/>
+      <c r="AK29" s="432"/>
+      <c r="AL29" s="432"/>
+      <c r="AM29" s="432"/>
+      <c r="AN29" s="432"/>
+      <c r="AO29" s="432"/>
+      <c r="AP29" s="432"/>
+      <c r="AQ29" s="432"/>
+      <c r="AR29" s="432"/>
+      <c r="AS29" s="432"/>
+      <c r="AT29" s="432"/>
+      <c r="AU29" s="432"/>
+      <c r="AV29" s="432"/>
+      <c r="AW29" s="432"/>
+      <c r="AX29" s="432"/>
+      <c r="AY29" s="432"/>
+      <c r="AZ29" s="432"/>
+      <c r="BA29" s="432"/>
+      <c r="BB29" s="432"/>
+      <c r="BC29" s="432"/>
+      <c r="BD29" s="432"/>
+      <c r="BE29" s="432"/>
+      <c r="BF29" s="432"/>
+      <c r="BG29" s="432"/>
+      <c r="BH29" s="432"/>
+      <c r="BI29" s="432"/>
+      <c r="BJ29" s="432"/>
+      <c r="BK29" s="432"/>
+      <c r="BL29" s="432"/>
+      <c r="BM29" s="432"/>
+      <c r="BN29" s="432"/>
+      <c r="BO29" s="432"/>
+      <c r="BP29" s="436"/>
+    </row>
+    <row r="30" spans="1:68" s="434" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="479"/>
+      <c r="B30" s="327"/>
       <c r="C30" s="30"/>
       <c r="D30" s="30"/>
       <c r="E30" s="30"/>
       <c r="F30" s="31"/>
-      <c r="G30" s="328"/>
-      <c r="H30" s="330"/>
-      <c r="I30" s="433"/>
-      <c r="J30" s="433"/>
-      <c r="K30" s="433"/>
-      <c r="L30" s="434"/>
-      <c r="P30" s="436"/>
-      <c r="Q30" s="433"/>
-      <c r="R30" s="433"/>
-      <c r="S30" s="433"/>
-      <c r="T30" s="433"/>
-      <c r="U30" s="433"/>
-      <c r="V30" s="433"/>
-      <c r="W30" s="433"/>
-      <c r="X30" s="433"/>
-      <c r="Y30" s="433"/>
-      <c r="Z30" s="433"/>
-      <c r="AA30" s="433"/>
-      <c r="AB30" s="433"/>
-      <c r="AC30" s="433"/>
-      <c r="AD30" s="433"/>
-      <c r="AE30" s="433"/>
-      <c r="AF30" s="433"/>
-      <c r="AG30" s="433"/>
-      <c r="AH30" s="433"/>
-      <c r="AI30" s="433"/>
-      <c r="AJ30" s="433"/>
-      <c r="AK30" s="433"/>
-      <c r="AL30" s="433"/>
-      <c r="AM30" s="433"/>
-      <c r="AN30" s="433"/>
-      <c r="AO30" s="433"/>
-      <c r="AP30" s="433"/>
-      <c r="AQ30" s="433"/>
-      <c r="AR30" s="433"/>
-      <c r="AS30" s="433"/>
-      <c r="AT30" s="433"/>
-      <c r="AU30" s="433"/>
-      <c r="AV30" s="433"/>
-      <c r="AW30" s="433"/>
-      <c r="AX30" s="433"/>
-      <c r="AY30" s="433"/>
-      <c r="AZ30" s="433"/>
-      <c r="BA30" s="433"/>
-      <c r="BB30" s="433"/>
-      <c r="BC30" s="433"/>
-      <c r="BD30" s="433"/>
-      <c r="BE30" s="433"/>
-      <c r="BF30" s="433"/>
-      <c r="BG30" s="433"/>
-      <c r="BH30" s="433"/>
-      <c r="BI30" s="433"/>
-      <c r="BJ30" s="433"/>
-      <c r="BK30" s="433"/>
-      <c r="BL30" s="433"/>
-      <c r="BM30" s="433"/>
-      <c r="BN30" s="433"/>
-      <c r="BO30" s="433"/>
-      <c r="BP30" s="437"/>
-    </row>
-    <row r="31" spans="1:68" s="435" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="480"/>
-      <c r="B31" s="328"/>
+      <c r="G30" s="327"/>
+      <c r="H30" s="329"/>
+      <c r="I30" s="432"/>
+      <c r="J30" s="432"/>
+      <c r="K30" s="432"/>
+      <c r="L30" s="433"/>
+      <c r="P30" s="435"/>
+      <c r="Q30" s="432"/>
+      <c r="R30" s="432"/>
+      <c r="S30" s="432"/>
+      <c r="T30" s="432"/>
+      <c r="U30" s="432"/>
+      <c r="V30" s="432"/>
+      <c r="W30" s="432"/>
+      <c r="X30" s="432"/>
+      <c r="Y30" s="432"/>
+      <c r="Z30" s="432"/>
+      <c r="AA30" s="432"/>
+      <c r="AB30" s="432"/>
+      <c r="AC30" s="432"/>
+      <c r="AD30" s="432"/>
+      <c r="AE30" s="432"/>
+      <c r="AF30" s="432"/>
+      <c r="AG30" s="432"/>
+      <c r="AH30" s="432"/>
+      <c r="AI30" s="432"/>
+      <c r="AJ30" s="432"/>
+      <c r="AK30" s="432"/>
+      <c r="AL30" s="432"/>
+      <c r="AM30" s="432"/>
+      <c r="AN30" s="432"/>
+      <c r="AO30" s="432"/>
+      <c r="AP30" s="432"/>
+      <c r="AQ30" s="432"/>
+      <c r="AR30" s="432"/>
+      <c r="AS30" s="432"/>
+      <c r="AT30" s="432"/>
+      <c r="AU30" s="432"/>
+      <c r="AV30" s="432"/>
+      <c r="AW30" s="432"/>
+      <c r="AX30" s="432"/>
+      <c r="AY30" s="432"/>
+      <c r="AZ30" s="432"/>
+      <c r="BA30" s="432"/>
+      <c r="BB30" s="432"/>
+      <c r="BC30" s="432"/>
+      <c r="BD30" s="432"/>
+      <c r="BE30" s="432"/>
+      <c r="BF30" s="432"/>
+      <c r="BG30" s="432"/>
+      <c r="BH30" s="432"/>
+      <c r="BI30" s="432"/>
+      <c r="BJ30" s="432"/>
+      <c r="BK30" s="432"/>
+      <c r="BL30" s="432"/>
+      <c r="BM30" s="432"/>
+      <c r="BN30" s="432"/>
+      <c r="BO30" s="432"/>
+      <c r="BP30" s="436"/>
+    </row>
+    <row r="31" spans="1:68" s="434" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="479"/>
+      <c r="B31" s="327"/>
       <c r="C31" s="30"/>
       <c r="D31" s="30"/>
       <c r="E31" s="30"/>
       <c r="F31" s="31"/>
-      <c r="G31" s="328"/>
-      <c r="H31" s="330"/>
-      <c r="I31" s="433"/>
-      <c r="J31" s="433"/>
-      <c r="K31" s="433"/>
-      <c r="L31" s="434"/>
-      <c r="P31" s="436"/>
-      <c r="Q31" s="433"/>
-      <c r="R31" s="433"/>
-      <c r="S31" s="433"/>
-      <c r="T31" s="433"/>
-      <c r="U31" s="433"/>
-      <c r="V31" s="433"/>
-      <c r="W31" s="433"/>
-      <c r="X31" s="433"/>
-      <c r="Y31" s="433"/>
-      <c r="Z31" s="433"/>
-      <c r="AA31" s="433"/>
-      <c r="AB31" s="433"/>
-      <c r="AC31" s="433"/>
-      <c r="AD31" s="433"/>
-      <c r="AE31" s="433"/>
-      <c r="AF31" s="433"/>
-      <c r="AG31" s="433"/>
-      <c r="AH31" s="433"/>
-      <c r="AI31" s="433"/>
-      <c r="AJ31" s="433"/>
-      <c r="AK31" s="433"/>
-      <c r="AL31" s="433"/>
-      <c r="AM31" s="433"/>
-      <c r="AN31" s="433"/>
-      <c r="AO31" s="433"/>
-      <c r="AP31" s="433"/>
-      <c r="AQ31" s="433"/>
-      <c r="AR31" s="433"/>
-      <c r="AS31" s="433"/>
-      <c r="AT31" s="433"/>
-      <c r="AU31" s="433"/>
-      <c r="AV31" s="433"/>
-      <c r="AW31" s="433"/>
-      <c r="AX31" s="433"/>
-      <c r="AY31" s="433"/>
-      <c r="AZ31" s="433"/>
-      <c r="BA31" s="433"/>
-      <c r="BB31" s="433"/>
-      <c r="BC31" s="433"/>
-      <c r="BD31" s="433"/>
-      <c r="BE31" s="433"/>
-      <c r="BF31" s="433"/>
-      <c r="BG31" s="433"/>
-      <c r="BH31" s="433"/>
-      <c r="BI31" s="433"/>
-      <c r="BJ31" s="433"/>
-      <c r="BK31" s="433"/>
-      <c r="BL31" s="433"/>
-      <c r="BM31" s="433"/>
-      <c r="BN31" s="433"/>
-      <c r="BO31" s="433"/>
-      <c r="BP31" s="437"/>
+      <c r="G31" s="327"/>
+      <c r="H31" s="329"/>
+      <c r="I31" s="432"/>
+      <c r="J31" s="432"/>
+      <c r="K31" s="432"/>
+      <c r="L31" s="433"/>
+      <c r="P31" s="435"/>
+      <c r="Q31" s="432"/>
+      <c r="R31" s="432"/>
+      <c r="S31" s="432"/>
+      <c r="T31" s="432"/>
+      <c r="U31" s="432"/>
+      <c r="V31" s="432"/>
+      <c r="W31" s="432"/>
+      <c r="X31" s="432"/>
+      <c r="Y31" s="432"/>
+      <c r="Z31" s="432"/>
+      <c r="AA31" s="432"/>
+      <c r="AB31" s="432"/>
+      <c r="AC31" s="432"/>
+      <c r="AD31" s="432"/>
+      <c r="AE31" s="432"/>
+      <c r="AF31" s="432"/>
+      <c r="AG31" s="432"/>
+      <c r="AH31" s="432"/>
+      <c r="AI31" s="432"/>
+      <c r="AJ31" s="432"/>
+      <c r="AK31" s="432"/>
+      <c r="AL31" s="432"/>
+      <c r="AM31" s="432"/>
+      <c r="AN31" s="432"/>
+      <c r="AO31" s="432"/>
+      <c r="AP31" s="432"/>
+      <c r="AQ31" s="432"/>
+      <c r="AR31" s="432"/>
+      <c r="AS31" s="432"/>
+      <c r="AT31" s="432"/>
+      <c r="AU31" s="432"/>
+      <c r="AV31" s="432"/>
+      <c r="AW31" s="432"/>
+      <c r="AX31" s="432"/>
+      <c r="AY31" s="432"/>
+      <c r="AZ31" s="432"/>
+      <c r="BA31" s="432"/>
+      <c r="BB31" s="432"/>
+      <c r="BC31" s="432"/>
+      <c r="BD31" s="432"/>
+      <c r="BE31" s="432"/>
+      <c r="BF31" s="432"/>
+      <c r="BG31" s="432"/>
+      <c r="BH31" s="432"/>
+      <c r="BI31" s="432"/>
+      <c r="BJ31" s="432"/>
+      <c r="BK31" s="432"/>
+      <c r="BL31" s="432"/>
+      <c r="BM31" s="432"/>
+      <c r="BN31" s="432"/>
+      <c r="BO31" s="432"/>
+      <c r="BP31" s="436"/>
     </row>
     <row r="32" spans="1:68" s="10" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="474"/>
-      <c r="B32" s="376"/>
-      <c r="C32" s="376"/>
-      <c r="D32" s="376"/>
-      <c r="E32" s="376"/>
-      <c r="F32" s="376"/>
-      <c r="G32" s="376"/>
-      <c r="H32" s="419"/>
+      <c r="A32" s="473"/>
+      <c r="B32" s="375"/>
+      <c r="C32" s="375"/>
+      <c r="D32" s="375"/>
+      <c r="E32" s="375"/>
+      <c r="F32" s="375"/>
+      <c r="G32" s="375"/>
+      <c r="H32" s="418"/>
       <c r="I32" s="25"/>
       <c r="J32" s="25"/>
       <c r="K32" s="25"/>
-      <c r="L32" s="429"/>
-      <c r="P32" s="430"/>
+      <c r="L32" s="428"/>
+      <c r="P32" s="429"/>
       <c r="Q32" s="25"/>
       <c r="R32" s="25"/>
       <c r="S32" s="25"/>
@@ -10140,19 +10137,19 @@
       <c r="BP32" s="26"/>
     </row>
     <row r="33" spans="1:68" s="170" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="481"/>
+      <c r="A33" s="480"/>
       <c r="B33" s="191"/>
       <c r="C33" s="191"/>
       <c r="D33" s="181"/>
       <c r="E33" s="181"/>
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
-      <c r="H33" s="432"/>
+      <c r="H33" s="431"/>
       <c r="I33" s="167"/>
       <c r="J33" s="167"/>
       <c r="K33" s="167"/>
-      <c r="L33" s="427"/>
-      <c r="P33" s="428"/>
+      <c r="L33" s="426"/>
+      <c r="P33" s="427"/>
       <c r="Q33" s="167"/>
       <c r="R33" s="167"/>
       <c r="S33" s="167"/>
@@ -10207,22 +10204,22 @@
       <c r="BP33" s="169"/>
     </row>
     <row r="34" spans="1:68" s="10" customFormat="1" ht="46.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="482"/>
-      <c r="B34" s="438"/>
-      <c r="C34" s="439"/>
-      <c r="D34" s="439"/>
-      <c r="E34" s="439"/>
-      <c r="F34" s="439"/>
-      <c r="G34" s="438"/>
-      <c r="H34" s="440"/>
+      <c r="A34" s="481"/>
+      <c r="B34" s="437"/>
+      <c r="C34" s="438"/>
+      <c r="D34" s="438"/>
+      <c r="E34" s="438"/>
+      <c r="F34" s="438"/>
+      <c r="G34" s="437"/>
+      <c r="H34" s="439"/>
       <c r="I34" s="25"/>
       <c r="J34" s="25"/>
       <c r="K34" s="25"/>
-      <c r="L34" s="441"/>
-      <c r="M34" s="442"/>
-      <c r="N34" s="442"/>
-      <c r="O34" s="442"/>
-      <c r="P34" s="443"/>
+      <c r="L34" s="440"/>
+      <c r="M34" s="441"/>
+      <c r="N34" s="441"/>
+      <c r="O34" s="441"/>
+      <c r="P34" s="442"/>
       <c r="Q34" s="25"/>
       <c r="R34" s="25"/>
       <c r="S34" s="25"/>
@@ -10277,20 +10274,20 @@
       <c r="BP34" s="26"/>
     </row>
     <row r="35" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="250"/>
-      <c r="B35" s="468"/>
-      <c r="C35" s="250"/>
-      <c r="D35" s="250"/>
-      <c r="E35" s="250"/>
-      <c r="F35" s="251"/>
-      <c r="G35" s="469"/>
-      <c r="H35" s="469"/>
+      <c r="A35" s="249"/>
+      <c r="B35" s="467"/>
+      <c r="C35" s="249"/>
+      <c r="D35" s="249"/>
+      <c r="E35" s="249"/>
+      <c r="F35" s="250"/>
+      <c r="G35" s="468"/>
+      <c r="H35" s="468"/>
     </row>
     <row r="36" spans="1:68" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="250" t="s">
+      <c r="A36" s="249" t="s">
         <v>17</v>
       </c>
-      <c r="B36" s="444">
+      <c r="B36" s="443">
         <f>COUNTA(B7:B34)</f>
         <v>0</v>
       </c>
@@ -10298,15 +10295,15 @@
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="L5:R5"/>
-    <mergeCell ref="A1:C3"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:H3"/>
+    <mergeCell ref="A2:C4"/>
     <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:H4"/>
     <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D4:F4"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="39" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="16" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;G</oddFooter>
   </headerFooter>
@@ -10323,10 +10320,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T44"/>
+  <dimension ref="A1:T43"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10365,14 +10362,14 @@
       <c r="N1" s="12"/>
     </row>
     <row r="2" spans="1:20" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="488"/>
-      <c r="B2" s="488"/>
-      <c r="C2" s="488"/>
-      <c r="D2" s="489"/>
-      <c r="E2" s="489"/>
-      <c r="F2" s="489"/>
-      <c r="G2" s="488"/>
-      <c r="H2" s="488"/>
+      <c r="A2" s="487"/>
+      <c r="B2" s="487"/>
+      <c r="C2" s="487"/>
+      <c r="D2" s="488"/>
+      <c r="E2" s="488"/>
+      <c r="F2" s="488"/>
+      <c r="G2" s="487"/>
+      <c r="H2" s="487"/>
       <c r="I2" s="12"/>
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
@@ -10387,16 +10384,16 @@
       <c r="T2" s="12"/>
     </row>
     <row r="3" spans="1:20" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="488"/>
-      <c r="B3" s="488"/>
-      <c r="C3" s="488"/>
-      <c r="D3" s="489" t="s">
+      <c r="A3" s="487"/>
+      <c r="B3" s="487"/>
+      <c r="C3" s="487"/>
+      <c r="D3" s="488" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="489"/>
-      <c r="F3" s="489"/>
-      <c r="G3" s="488"/>
-      <c r="H3" s="488"/>
+      <c r="E3" s="488"/>
+      <c r="F3" s="488"/>
+      <c r="G3" s="487"/>
+      <c r="H3" s="487"/>
       <c r="I3" s="12"/>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
@@ -10411,14 +10408,14 @@
       <c r="T3" s="12"/>
     </row>
     <row r="4" spans="1:20" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="488"/>
-      <c r="B4" s="488"/>
-      <c r="C4" s="488"/>
-      <c r="D4" s="489"/>
-      <c r="E4" s="489"/>
-      <c r="F4" s="489"/>
-      <c r="G4" s="488"/>
-      <c r="H4" s="488"/>
+      <c r="A4" s="487"/>
+      <c r="B4" s="487"/>
+      <c r="C4" s="487"/>
+      <c r="D4" s="488"/>
+      <c r="E4" s="488"/>
+      <c r="F4" s="488"/>
+      <c r="G4" s="487"/>
+      <c r="H4" s="487"/>
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
@@ -10432,13 +10429,13 @@
       <c r="S4" s="12"/>
       <c r="T4" s="12"/>
     </row>
-    <row r="5" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="228"/>
-      <c r="E5" s="228"/>
-      <c r="F5" s="228"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
@@ -10454,21 +10451,47 @@
       <c r="S5" s="12"/>
       <c r="T5" s="12"/>
     </row>
-    <row r="6" spans="1:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
+    <row r="6" spans="1:20" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="457" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="458" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="459" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="458" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="458" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="460" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="461" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="462" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="20"/>
+      <c r="J6" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6" s="13" t="s">
+        <v>30</v>
+      </c>
       <c r="O6" s="12"/>
       <c r="P6" s="12"/>
       <c r="Q6" s="12"/>
@@ -10476,47 +10499,21 @@
       <c r="S6" s="12"/>
       <c r="T6" s="12"/>
     </row>
-    <row r="7" spans="1:20" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="458" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="459" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="460" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="459" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="459" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="461" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="462" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" s="463" t="s">
-        <v>22</v>
-      </c>
+    <row r="7" spans="1:20" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="452"/>
+      <c r="B7" s="154"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="446"/>
       <c r="I7" s="20"/>
-      <c r="J7" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="K7" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="M7" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="N7" s="13" t="s">
-        <v>30</v>
-      </c>
+      <c r="J7" s="21"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
       <c r="O7" s="12"/>
       <c r="P7" s="12"/>
       <c r="Q7" s="12"/>
@@ -10524,21 +10521,27 @@
       <c r="S7" s="12"/>
       <c r="T7" s="12"/>
     </row>
-    <row r="8" spans="1:20" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="453"/>
-      <c r="B8" s="154"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="447"/>
+    <row r="8" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="444"/>
+      <c r="B8" s="171"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="172"/>
+      <c r="E8" s="172"/>
+      <c r="F8" s="172"/>
+      <c r="G8" s="172"/>
+      <c r="H8" s="445"/>
       <c r="I8" s="20"/>
       <c r="J8" s="21"/>
       <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
+      <c r="L8" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="N8" s="13" t="s">
+        <v>26</v>
+      </c>
       <c r="O8" s="12"/>
       <c r="P8" s="12"/>
       <c r="Q8" s="12"/>
@@ -10547,26 +10550,20 @@
       <c r="T8" s="12"/>
     </row>
     <row r="9" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="445"/>
-      <c r="B9" s="171"/>
-      <c r="C9" s="56"/>
-      <c r="D9" s="172"/>
-      <c r="E9" s="172"/>
-      <c r="F9" s="172"/>
-      <c r="G9" s="172"/>
+      <c r="A9" s="444"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
       <c r="H9" s="446"/>
       <c r="I9" s="20"/>
       <c r="J9" s="21"/>
       <c r="K9" s="13"/>
-      <c r="L9" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="M9" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="N9" s="13" t="s">
-        <v>26</v>
-      </c>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
       <c r="O9" s="12"/>
       <c r="P9" s="12"/>
       <c r="Q9" s="12"/>
@@ -10574,59 +10571,59 @@
       <c r="S9" s="12"/>
       <c r="T9" s="12"/>
     </row>
-    <row r="10" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="445"/>
+    <row r="10" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="444"/>
       <c r="B10" s="27"/>
       <c r="C10" s="28"/>
       <c r="D10" s="28"/>
       <c r="E10" s="28"/>
       <c r="F10" s="28"/>
       <c r="G10" s="28"/>
-      <c r="H10" s="447"/>
+      <c r="H10" s="446"/>
       <c r="I10" s="20"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="12"/>
-      <c r="S10" s="12"/>
-      <c r="T10" s="12"/>
-    </row>
-    <row r="11" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="445"/>
+      <c r="J10" s="179"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="M10" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="N10" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="444"/>
       <c r="B11" s="27"/>
       <c r="C11" s="28"/>
       <c r="D11" s="28"/>
       <c r="E11" s="28"/>
       <c r="F11" s="28"/>
       <c r="G11" s="28"/>
-      <c r="H11" s="447"/>
+      <c r="H11" s="446"/>
       <c r="I11" s="20"/>
-      <c r="J11" s="179"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="M11" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="N11" s="11" t="s">
-        <v>26</v>
-      </c>
+      <c r="J11" s="21"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
     </row>
     <row r="12" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="445"/>
+      <c r="A12" s="444"/>
       <c r="B12" s="27"/>
       <c r="C12" s="28"/>
       <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
+      <c r="E12" s="156"/>
+      <c r="F12" s="156"/>
       <c r="G12" s="28"/>
-      <c r="H12" s="447"/>
+      <c r="H12" s="446"/>
       <c r="I12" s="20"/>
       <c r="J12" s="21"/>
       <c r="K12" s="13"/>
@@ -10641,14 +10638,14 @@
       <c r="T12" s="12"/>
     </row>
     <row r="13" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="445"/>
+      <c r="A13" s="444"/>
       <c r="B13" s="27"/>
       <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="156"/>
-      <c r="F13" s="156"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="447"/>
+      <c r="D13" s="152"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="211"/>
+      <c r="G13" s="171"/>
+      <c r="H13" s="446"/>
       <c r="I13" s="20"/>
       <c r="J13" s="21"/>
       <c r="K13" s="13"/>
@@ -10663,14 +10660,14 @@
       <c r="T13" s="12"/>
     </row>
     <row r="14" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="445"/>
+      <c r="A14" s="444"/>
       <c r="B14" s="27"/>
       <c r="C14" s="28"/>
-      <c r="D14" s="152"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="211"/>
-      <c r="G14" s="171"/>
-      <c r="H14" s="447"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="152"/>
+      <c r="F14" s="153"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="446"/>
       <c r="I14" s="20"/>
       <c r="J14" s="21"/>
       <c r="K14" s="13"/>
@@ -10685,14 +10682,14 @@
       <c r="T14" s="12"/>
     </row>
     <row r="15" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="445"/>
+      <c r="A15" s="444"/>
       <c r="B15" s="27"/>
       <c r="C15" s="28"/>
       <c r="D15" s="28"/>
-      <c r="E15" s="152"/>
-      <c r="F15" s="153"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
       <c r="G15" s="28"/>
-      <c r="H15" s="447"/>
+      <c r="H15" s="446"/>
       <c r="I15" s="20"/>
       <c r="J15" s="21"/>
       <c r="K15" s="13"/>
@@ -10706,89 +10703,89 @@
       <c r="S15" s="12"/>
       <c r="T15" s="12"/>
     </row>
-    <row r="16" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="445"/>
+    <row r="16" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="444"/>
       <c r="B16" s="27"/>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
-      <c r="H16" s="447"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="12"/>
-      <c r="R16" s="12"/>
-      <c r="S16" s="12"/>
-      <c r="T16" s="12"/>
-    </row>
-    <row r="17" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="445"/>
+      <c r="H16" s="446"/>
+      <c r="J16" s="155"/>
+      <c r="K16" s="155"/>
+      <c r="L16" s="155"/>
+      <c r="M16" s="155"/>
+      <c r="N16" s="155"/>
+    </row>
+    <row r="17" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="444"/>
       <c r="B17" s="27"/>
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
-      <c r="H17" s="447"/>
-      <c r="J17" s="155"/>
-      <c r="K17" s="155"/>
-      <c r="L17" s="155"/>
-      <c r="M17" s="155"/>
-      <c r="N17" s="155"/>
-    </row>
-    <row r="18" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="445"/>
+      <c r="H17" s="446"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="12"/>
+      <c r="S17" s="12"/>
+      <c r="T17" s="12"/>
+    </row>
+    <row r="18" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="444"/>
       <c r="B18" s="27"/>
       <c r="C18" s="28"/>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
-      <c r="H18" s="447"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="12"/>
-      <c r="P18" s="12"/>
-      <c r="Q18" s="12"/>
-      <c r="R18" s="12"/>
-      <c r="S18" s="12"/>
-      <c r="T18" s="12"/>
-    </row>
-    <row r="19" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="445"/>
+      <c r="H18" s="446"/>
+      <c r="J18" s="155"/>
+      <c r="K18" s="155"/>
+      <c r="L18" s="155"/>
+      <c r="M18" s="155"/>
+      <c r="N18" s="155"/>
+    </row>
+    <row r="19" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="444"/>
       <c r="B19" s="27"/>
       <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
+      <c r="D19" s="156"/>
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
-      <c r="H19" s="447"/>
-      <c r="J19" s="155"/>
-      <c r="K19" s="155"/>
-      <c r="L19" s="155"/>
-      <c r="M19" s="155"/>
-      <c r="N19" s="155"/>
+      <c r="H19" s="446"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="12"/>
+      <c r="S19" s="12"/>
+      <c r="T19" s="12"/>
     </row>
     <row r="20" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="445"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="156"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="447"/>
+      <c r="A20" s="444"/>
+      <c r="B20" s="203"/>
+      <c r="C20" s="204"/>
+      <c r="D20" s="205"/>
+      <c r="E20" s="179"/>
+      <c r="F20" s="206"/>
+      <c r="G20" s="207"/>
+      <c r="H20" s="448"/>
       <c r="I20" s="20"/>
       <c r="J20" s="21"/>
       <c r="K20" s="13"/>
@@ -10803,14 +10800,14 @@
       <c r="T20" s="12"/>
     </row>
     <row r="21" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="445"/>
-      <c r="B21" s="203"/>
-      <c r="C21" s="204"/>
-      <c r="D21" s="205"/>
-      <c r="E21" s="179"/>
-      <c r="F21" s="206"/>
-      <c r="G21" s="207"/>
-      <c r="H21" s="449"/>
+      <c r="A21" s="444"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="446"/>
       <c r="I21" s="20"/>
       <c r="J21" s="21"/>
       <c r="K21" s="13"/>
@@ -10825,14 +10822,14 @@
       <c r="T21" s="12"/>
     </row>
     <row r="22" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="445"/>
+      <c r="A22" s="444"/>
       <c r="B22" s="27"/>
       <c r="C22" s="28"/>
       <c r="D22" s="28"/>
       <c r="E22" s="28"/>
       <c r="F22" s="28"/>
       <c r="G22" s="28"/>
-      <c r="H22" s="447"/>
+      <c r="H22" s="446"/>
       <c r="I22" s="20"/>
       <c r="J22" s="21"/>
       <c r="K22" s="13"/>
@@ -10847,14 +10844,14 @@
       <c r="T22" s="12"/>
     </row>
     <row r="23" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="445"/>
+      <c r="A23" s="444"/>
       <c r="B23" s="27"/>
       <c r="C23" s="28"/>
       <c r="D23" s="28"/>
       <c r="E23" s="28"/>
       <c r="F23" s="28"/>
       <c r="G23" s="28"/>
-      <c r="H23" s="447"/>
+      <c r="H23" s="446"/>
       <c r="I23" s="20"/>
       <c r="J23" s="21"/>
       <c r="K23" s="13"/>
@@ -10869,14 +10866,14 @@
       <c r="T23" s="12"/>
     </row>
     <row r="24" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="445"/>
+      <c r="A24" s="444"/>
       <c r="B24" s="27"/>
       <c r="C24" s="28"/>
       <c r="D24" s="28"/>
       <c r="E24" s="28"/>
       <c r="F24" s="28"/>
       <c r="G24" s="28"/>
-      <c r="H24" s="447"/>
+      <c r="H24" s="446"/>
       <c r="I24" s="20"/>
       <c r="J24" s="21"/>
       <c r="K24" s="13"/>
@@ -10891,52 +10888,52 @@
       <c r="T24" s="12"/>
     </row>
     <row r="25" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="445"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="447"/>
+      <c r="A25" s="444"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="208"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="449"/>
       <c r="I25" s="20"/>
       <c r="J25" s="21"/>
       <c r="K25" s="13"/>
       <c r="L25" s="13"/>
       <c r="M25" s="13"/>
       <c r="N25" s="13"/>
-      <c r="O25" s="12"/>
-      <c r="P25" s="12"/>
-      <c r="Q25" s="12"/>
-      <c r="R25" s="12"/>
-      <c r="S25" s="12"/>
-      <c r="T25" s="12"/>
     </row>
     <row r="26" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="445"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="208"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="450"/>
+      <c r="A26" s="444"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="446"/>
       <c r="I26" s="20"/>
       <c r="J26" s="21"/>
       <c r="K26" s="13"/>
       <c r="L26" s="13"/>
       <c r="M26" s="13"/>
       <c r="N26" s="13"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="12"/>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="12"/>
+      <c r="S26" s="12"/>
+      <c r="T26" s="12"/>
     </row>
     <row r="27" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="445"/>
+      <c r="A27" s="444"/>
       <c r="B27" s="27"/>
       <c r="C27" s="28"/>
       <c r="D27" s="28"/>
       <c r="E27" s="28"/>
       <c r="F27" s="28"/>
       <c r="G27" s="28"/>
-      <c r="H27" s="447"/>
+      <c r="H27" s="446"/>
       <c r="I27" s="20"/>
       <c r="J27" s="21"/>
       <c r="K27" s="13"/>
@@ -10951,14 +10948,14 @@
       <c r="T27" s="12"/>
     </row>
     <row r="28" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="445"/>
+      <c r="A28" s="444"/>
       <c r="B28" s="27"/>
       <c r="C28" s="28"/>
       <c r="D28" s="28"/>
       <c r="E28" s="28"/>
       <c r="F28" s="28"/>
       <c r="G28" s="28"/>
-      <c r="H28" s="447"/>
+      <c r="H28" s="446"/>
       <c r="I28" s="20"/>
       <c r="J28" s="21"/>
       <c r="K28" s="13"/>
@@ -10973,14 +10970,14 @@
       <c r="T28" s="12"/>
     </row>
     <row r="29" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="445"/>
+      <c r="A29" s="444"/>
       <c r="B29" s="27"/>
       <c r="C29" s="28"/>
       <c r="D29" s="28"/>
       <c r="E29" s="28"/>
       <c r="F29" s="28"/>
       <c r="G29" s="28"/>
-      <c r="H29" s="447"/>
+      <c r="H29" s="446"/>
       <c r="I29" s="20"/>
       <c r="J29" s="21"/>
       <c r="K29" s="13"/>
@@ -10995,14 +10992,14 @@
       <c r="T29" s="12"/>
     </row>
     <row r="30" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="445"/>
+      <c r="A30" s="444"/>
       <c r="B30" s="27"/>
       <c r="C30" s="28"/>
       <c r="D30" s="28"/>
       <c r="E30" s="28"/>
       <c r="F30" s="28"/>
       <c r="G30" s="28"/>
-      <c r="H30" s="447"/>
+      <c r="H30" s="446"/>
       <c r="I30" s="20"/>
       <c r="J30" s="21"/>
       <c r="K30" s="13"/>
@@ -11017,14 +11014,14 @@
       <c r="T30" s="12"/>
     </row>
     <row r="31" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="445"/>
+      <c r="A31" s="444"/>
       <c r="B31" s="27"/>
       <c r="C31" s="28"/>
       <c r="D31" s="28"/>
       <c r="E31" s="28"/>
       <c r="F31" s="28"/>
       <c r="G31" s="28"/>
-      <c r="H31" s="447"/>
+      <c r="H31" s="446"/>
       <c r="I31" s="20"/>
       <c r="J31" s="21"/>
       <c r="K31" s="13"/>
@@ -11039,14 +11036,14 @@
       <c r="T31" s="12"/>
     </row>
     <row r="32" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="445"/>
+      <c r="A32" s="444"/>
       <c r="B32" s="27"/>
       <c r="C32" s="28"/>
       <c r="D32" s="28"/>
       <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
+      <c r="F32" s="9"/>
       <c r="G32" s="28"/>
-      <c r="H32" s="447"/>
+      <c r="H32" s="446"/>
       <c r="I32" s="20"/>
       <c r="J32" s="21"/>
       <c r="K32" s="13"/>
@@ -11061,14 +11058,14 @@
       <c r="T32" s="12"/>
     </row>
     <row r="33" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="445"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="28"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="447"/>
+      <c r="A33" s="450"/>
+      <c r="B33" s="177"/>
+      <c r="C33" s="156"/>
+      <c r="D33" s="156"/>
+      <c r="E33" s="156"/>
+      <c r="F33" s="156"/>
+      <c r="G33" s="156"/>
+      <c r="H33" s="451"/>
       <c r="I33" s="20"/>
       <c r="J33" s="21"/>
       <c r="K33" s="13"/>
@@ -11083,14 +11080,14 @@
       <c r="T33" s="12"/>
     </row>
     <row r="34" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="451"/>
-      <c r="B34" s="177"/>
-      <c r="C34" s="156"/>
-      <c r="D34" s="156"/>
-      <c r="E34" s="156"/>
-      <c r="F34" s="156"/>
-      <c r="G34" s="156"/>
-      <c r="H34" s="452"/>
+      <c r="A34" s="444"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="447"/>
       <c r="I34" s="20"/>
       <c r="J34" s="21"/>
       <c r="K34" s="13"/>
@@ -11105,14 +11102,14 @@
       <c r="T34" s="12"/>
     </row>
     <row r="35" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="445"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="448"/>
+      <c r="A35" s="452"/>
+      <c r="B35" s="178"/>
+      <c r="C35" s="178"/>
+      <c r="D35" s="178"/>
+      <c r="E35" s="178"/>
+      <c r="F35" s="178"/>
+      <c r="G35" s="178"/>
+      <c r="H35" s="453"/>
       <c r="I35" s="20"/>
       <c r="J35" s="21"/>
       <c r="K35" s="13"/>
@@ -11126,15 +11123,15 @@
       <c r="S35" s="12"/>
       <c r="T35" s="12"/>
     </row>
-    <row r="36" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="453"/>
-      <c r="B36" s="178"/>
-      <c r="C36" s="178"/>
-      <c r="D36" s="178"/>
-      <c r="E36" s="178"/>
-      <c r="F36" s="178"/>
-      <c r="G36" s="178"/>
-      <c r="H36" s="454"/>
+    <row r="36" spans="1:20" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="454"/>
+      <c r="B36" s="455"/>
+      <c r="C36" s="455"/>
+      <c r="D36" s="455"/>
+      <c r="E36" s="455"/>
+      <c r="F36" s="455"/>
+      <c r="G36" s="455"/>
+      <c r="H36" s="456"/>
       <c r="I36" s="20"/>
       <c r="J36" s="21"/>
       <c r="K36" s="13"/>
@@ -11148,31 +11145,30 @@
       <c r="S36" s="12"/>
       <c r="T36" s="12"/>
     </row>
-    <row r="37" spans="1:20" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="455"/>
-      <c r="B37" s="456"/>
-      <c r="C37" s="456"/>
-      <c r="D37" s="456"/>
-      <c r="E37" s="456"/>
-      <c r="F37" s="456"/>
-      <c r="G37" s="456"/>
-      <c r="H37" s="457"/>
-      <c r="I37" s="20"/>
-      <c r="J37" s="21"/>
-      <c r="K37" s="13"/>
-      <c r="L37" s="13"/>
-      <c r="M37" s="13"/>
-      <c r="N37" s="13"/>
-      <c r="O37" s="12"/>
-      <c r="P37" s="12"/>
-      <c r="Q37" s="12"/>
-      <c r="R37" s="12"/>
-      <c r="S37" s="12"/>
-      <c r="T37" s="12"/>
+    <row r="37" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="12"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="165"/>
+      <c r="K37" s="165"/>
+      <c r="L37" s="165"/>
+      <c r="M37" s="165"/>
+      <c r="N37" s="165"/>
     </row>
     <row r="38" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12"/>
+      <c r="A38" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B38" s="23">
+        <f>COUNTA(B7:B36)</f>
+        <v>0</v>
+      </c>
       <c r="C38" s="18"/>
       <c r="D38" s="12"/>
       <c r="E38" s="12"/>
@@ -11180,20 +11176,15 @@
       <c r="G38" s="22"/>
       <c r="H38" s="12"/>
       <c r="I38" s="12"/>
-      <c r="J38" s="165"/>
-      <c r="K38" s="165"/>
-      <c r="L38" s="165"/>
-      <c r="M38" s="165"/>
-      <c r="N38" s="165"/>
+      <c r="J38" s="12"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="12"/>
+      <c r="M38" s="12"/>
+      <c r="N38" s="12"/>
     </row>
     <row r="39" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B39" s="23">
-        <f>COUNTA(B8:B37)</f>
-        <v>0</v>
-      </c>
+      <c r="A39" s="12"/>
+      <c r="B39" s="12"/>
       <c r="C39" s="18"/>
       <c r="D39" s="12"/>
       <c r="E39" s="12"/>
@@ -11207,21 +11198,8 @@
       <c r="M39" s="12"/>
       <c r="N39" s="12"/>
     </row>
-    <row r="40" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="12"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
+    <row r="40" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="G40" s="22"/>
-      <c r="H40" s="12"/>
-      <c r="I40" s="12"/>
-      <c r="J40" s="12"/>
-      <c r="K40" s="12"/>
-      <c r="L40" s="12"/>
-      <c r="M40" s="12"/>
-      <c r="N40" s="12"/>
     </row>
     <row r="41" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="G41" s="22"/>
@@ -11229,13 +11207,10 @@
     <row r="42" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="G42" s="22"/>
     </row>
-    <row r="43" spans="1:20" ht="16" x14ac:dyDescent="0.2">
-      <c r="G43" s="22"/>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:G37">
-    <sortCondition ref="B9:B37"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:G36">
+    <sortCondition ref="B8:B36"/>
   </sortState>
   <mergeCells count="5">
     <mergeCell ref="G2:H4"/>
@@ -11245,7 +11220,7 @@
     <mergeCell ref="D3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="56" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup scale="35" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
update template to have title and date in middle with same font. update wrap text for gr rcup
</commit_message>
<xml_diff>
--- a/templates/entry_list_template.xlsx
+++ b/templates/entry_list_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brendanwoo/projects/sro_sign_in/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C5A1E4-B377-D741-A579-2821C48CDD20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6E9107-E235-A640-8122-A99D5E008E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{542D648B-9180-43EF-9053-182057C63D4C}"/>
+    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="4" xr2:uid="{542D648B-9180-43EF-9053-182057C63D4C}"/>
   </bookViews>
   <sheets>
     <sheet name="GTWCA" sheetId="10" r:id="rId1"/>
@@ -149,7 +149,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="66" x14ac:knownFonts="1">
+  <fonts count="67" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -577,6 +577,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1783,7 +1789,7 @@
     <xf numFmtId="0" fontId="23" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="56" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="530">
+  <cellXfs count="531">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2767,513 +2773,534 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="85" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="87" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="88" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="59" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="60" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="61" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="59" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="62" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="59" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="60" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="59" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="59" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="59" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="59" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="60" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="60" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="61" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="61" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="59" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="62" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="62" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="59" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="59" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="59" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="59" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="59" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="59" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="61" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="62" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="62" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="59" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="59" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="59" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="60" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="60" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="60" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="60" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="60" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="60" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="59" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="60" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="60" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="60" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="59" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="59" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="60" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="60" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="60" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="60" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="60" fillId="0" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="60" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="60" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="60" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="63" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="64" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="65" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="64" fillId="0" borderId="86" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="63" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="64" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="65" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="64" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="65" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="63" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="63" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="63" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="64" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="65" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="65" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="64" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="63" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="63" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="63" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="63" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="63" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="63" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="63" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="63" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="63" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="63" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="64" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="65" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="64" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="64" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="64" fillId="0" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="64" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="63" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="63" fillId="0" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="63" fillId="0" borderId="91" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="65" fillId="0" borderId="91" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="65" fillId="0" borderId="90" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="63" fillId="0" borderId="91" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="65" fillId="0" borderId="40" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="61" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="45" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="51" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="45" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="39" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="59" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="59" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="60" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="62" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="59" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="59" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="60" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="59" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="59" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="59" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="62" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="60" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="60" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="51" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="56" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="54" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="85" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="87" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="88" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="59" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="60" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="61" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="59" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="62" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="59" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="60" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="59" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="59" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="59" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="59" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="60" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="60" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="61" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="61" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="59" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="62" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="62" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="59" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="59" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="59" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="59" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="59" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="59" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="61" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="62" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="62" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="59" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="59" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="59" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="60" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="60" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="60" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="60" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="60" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="60" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="59" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="60" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="60" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="60" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="59" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="59" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="60" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="60" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="60" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="60" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="60" fillId="0" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="60" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="60" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="60" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="63" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="64" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="65" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="64" fillId="0" borderId="86" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="64" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="64" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="63" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="64" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="65" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="64" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="65" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="64" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="64" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="63" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="63" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="63" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="64" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="65" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="65" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="64" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="63" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="63" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="63" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="63" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="63" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="63" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="63" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="63" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="63" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="63" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="64" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="65" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="64" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="64" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="64" fillId="0" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="64" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="63" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="63" fillId="0" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="63" fillId="0" borderId="91" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="65" fillId="0" borderId="91" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="65" fillId="0" borderId="90" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="63" fillId="0" borderId="91" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="65" fillId="0" borderId="40" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="61" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="45" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="51" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="45" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="14" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="39" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="14" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="59" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="59" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="60" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="62" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="59" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="59" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="60" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="59" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="59" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="59" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="62" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="60" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="60" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3283,26 +3310,8 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="51" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="56" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="54" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3313,73 +3322,6 @@
     <cellStyle name="Normal 2" xfId="2" xr:uid="{561A9865-CE34-4D81-A124-2143BF703225}"/>
   </cellStyles>
   <dxfs count="66">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thick">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -5096,6 +5038,73 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thick">
           <color indexed="64"/>
         </left>
         <right style="thin">
@@ -5800,86 +5809,86 @@
     <sortCondition ref="B28"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="2" xr3:uid="{8EAC187A-4BC7-044D-A24C-EE683FF40EDC}" name="Series" dataDxfId="0" dataCellStyle="Neutral"/>
-    <tableColumn id="10" xr3:uid="{6761E48F-7432-8E4D-983D-FD8CF12204ED}" name="Car #" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{0DF6B8D7-FC4D-5845-A1AC-0C19350700B1}" name="Team " dataDxfId="59" dataCellStyle="Neutral"/>
-    <tableColumn id="4" xr3:uid="{D7958FE6-C778-2340-A370-BF9B62951BE2}" name="Driver 1" dataDxfId="58" dataCellStyle="Neutral"/>
-    <tableColumn id="5" xr3:uid="{A1C4CE74-0FBD-A249-A28E-1AA4F0E32E24}" name="NAT" dataDxfId="57" dataCellStyle="Neutral"/>
-    <tableColumn id="13" xr3:uid="{06D828EC-E323-DA4F-B814-30D97E8751E7}" name="LIC " dataDxfId="56"/>
-    <tableColumn id="6" xr3:uid="{5C59EF6B-E503-B449-BD81-31D0C127B158}" name="CAT" dataDxfId="55"/>
-    <tableColumn id="12" xr3:uid="{FCCDF9C0-43DB-3343-8312-4E0B4B75956D}" name="Driver 2" dataDxfId="54"/>
-    <tableColumn id="11" xr3:uid="{48BAF24C-A19D-1B40-8E87-E8ABF82E4431}" name="  NAT " dataDxfId="53"/>
-    <tableColumn id="14" xr3:uid="{CF8EB17E-A9FE-5E4E-B068-F6226C82985D}" name=" LIC " dataDxfId="52"/>
-    <tableColumn id="1" xr3:uid="{4E58BAAF-4A36-2443-BB6E-FB2F3CD6C045}" name="CAT " dataDxfId="51"/>
-    <tableColumn id="8" xr3:uid="{B01B38E0-90B8-DA4E-A115-23024964F22B}" name="Car Sponsors" dataDxfId="50" dataCellStyle="Neutral"/>
-    <tableColumn id="7" xr3:uid="{A8339886-62FE-D648-99E5-4129118A9D24}" name="Car Make/Model" dataDxfId="49"/>
-    <tableColumn id="9" xr3:uid="{FAA5AA03-0CBD-CD44-B4EA-32A19F875C8B}" name="Championship" dataDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{8EAC187A-4BC7-044D-A24C-EE683FF40EDC}" name="Series" dataDxfId="59" dataCellStyle="Neutral"/>
+    <tableColumn id="10" xr3:uid="{6761E48F-7432-8E4D-983D-FD8CF12204ED}" name="Car #" dataDxfId="58"/>
+    <tableColumn id="3" xr3:uid="{0DF6B8D7-FC4D-5845-A1AC-0C19350700B1}" name="Team " dataDxfId="57" dataCellStyle="Neutral"/>
+    <tableColumn id="4" xr3:uid="{D7958FE6-C778-2340-A370-BF9B62951BE2}" name="Driver 1" dataDxfId="56" dataCellStyle="Neutral"/>
+    <tableColumn id="5" xr3:uid="{A1C4CE74-0FBD-A249-A28E-1AA4F0E32E24}" name="NAT" dataDxfId="55" dataCellStyle="Neutral"/>
+    <tableColumn id="13" xr3:uid="{06D828EC-E323-DA4F-B814-30D97E8751E7}" name="LIC " dataDxfId="54"/>
+    <tableColumn id="6" xr3:uid="{5C59EF6B-E503-B449-BD81-31D0C127B158}" name="CAT" dataDxfId="53"/>
+    <tableColumn id="12" xr3:uid="{FCCDF9C0-43DB-3343-8312-4E0B4B75956D}" name="Driver 2" dataDxfId="52"/>
+    <tableColumn id="11" xr3:uid="{48BAF24C-A19D-1B40-8E87-E8ABF82E4431}" name="  NAT " dataDxfId="51"/>
+    <tableColumn id="14" xr3:uid="{CF8EB17E-A9FE-5E4E-B068-F6226C82985D}" name=" LIC " dataDxfId="50"/>
+    <tableColumn id="1" xr3:uid="{4E58BAAF-4A36-2443-BB6E-FB2F3CD6C045}" name="CAT " dataDxfId="49"/>
+    <tableColumn id="8" xr3:uid="{B01B38E0-90B8-DA4E-A115-23024964F22B}" name="Car Sponsors" dataDxfId="48" dataCellStyle="Neutral"/>
+    <tableColumn id="7" xr3:uid="{A8339886-62FE-D648-99E5-4129118A9D24}" name="Car Make/Model" dataDxfId="47"/>
+    <tableColumn id="9" xr3:uid="{FAA5AA03-0CBD-CD44-B4EA-32A19F875C8B}" name="Championship" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{56F25BC1-6701-4669-AC0F-E1673995674A}" name="Table2267" displayName="Table2267" ref="A6:N38" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="46" tableBorderDxfId="45" totalsRowBorderDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{56F25BC1-6701-4669-AC0F-E1673995674A}" name="Table2267" displayName="Table2267" ref="A6:N38" totalsRowShown="0" headerRowDxfId="45" headerRowBorderDxfId="44" tableBorderDxfId="43" totalsRowBorderDxfId="42">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:N39">
     <sortCondition ref="B9:B39"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="2" xr3:uid="{86C7766F-C815-4642-A792-C792E5CD9B1D}" name="Series" dataDxfId="43" dataCellStyle="Neutral"/>
-    <tableColumn id="10" xr3:uid="{B0849F24-6597-4E76-94D7-2D7E93B5B7E1}" name="Car #" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{C0375D1B-A6A9-4878-94F1-144B367DBFAE}" name="Team " dataDxfId="41" dataCellStyle="Neutral"/>
-    <tableColumn id="4" xr3:uid="{731AF936-9BBC-4114-AF94-6737C2C799AD}" name="Driver 1" dataDxfId="40" dataCellStyle="Neutral"/>
-    <tableColumn id="5" xr3:uid="{4AAAC599-A742-4343-8BE4-F0207EAEB236}" name="NAT" dataDxfId="39" dataCellStyle="Neutral"/>
-    <tableColumn id="13" xr3:uid="{46C8C08D-7690-4908-8D68-9031FA1AAB13}" name="LIC " dataDxfId="38"/>
-    <tableColumn id="6" xr3:uid="{0B42790F-CF16-4A79-97F6-02353851B814}" name="CAT" dataDxfId="37"/>
-    <tableColumn id="12" xr3:uid="{4393EDC9-8099-4851-8BA5-F88B5093FA18}" name="Driver 2" dataDxfId="36"/>
-    <tableColumn id="11" xr3:uid="{022A346F-1EFC-477E-B3FF-234F17FB995D}" name="  NAT " dataDxfId="35"/>
-    <tableColumn id="14" xr3:uid="{4A5DA010-C6D1-49CE-8487-00AC7C736274}" name=" LIC " dataDxfId="34"/>
-    <tableColumn id="1" xr3:uid="{15D47E2B-7108-41F5-BB6D-FABBD704C2C8}" name="CAT " dataDxfId="33"/>
-    <tableColumn id="8" xr3:uid="{5F578104-8A47-4C21-AE4F-A41AFD51CA17}" name="Car Sponsors" dataDxfId="32" dataCellStyle="Neutral"/>
-    <tableColumn id="7" xr3:uid="{37BFAE36-6B5E-4D59-B805-2A4B37B829ED}" name="Car Make/Model" dataDxfId="31"/>
-    <tableColumn id="9" xr3:uid="{C4134C49-64E4-4B01-865E-C1B755B7D04A}" name="Championship" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{86C7766F-C815-4642-A792-C792E5CD9B1D}" name="Series" dataDxfId="41" dataCellStyle="Neutral"/>
+    <tableColumn id="10" xr3:uid="{B0849F24-6597-4E76-94D7-2D7E93B5B7E1}" name="Car #" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{C0375D1B-A6A9-4878-94F1-144B367DBFAE}" name="Team " dataDxfId="39" dataCellStyle="Neutral"/>
+    <tableColumn id="4" xr3:uid="{731AF936-9BBC-4114-AF94-6737C2C799AD}" name="Driver 1" dataDxfId="38" dataCellStyle="Neutral"/>
+    <tableColumn id="5" xr3:uid="{4AAAC599-A742-4343-8BE4-F0207EAEB236}" name="NAT" dataDxfId="37" dataCellStyle="Neutral"/>
+    <tableColumn id="13" xr3:uid="{46C8C08D-7690-4908-8D68-9031FA1AAB13}" name="LIC " dataDxfId="36"/>
+    <tableColumn id="6" xr3:uid="{0B42790F-CF16-4A79-97F6-02353851B814}" name="CAT" dataDxfId="35"/>
+    <tableColumn id="12" xr3:uid="{4393EDC9-8099-4851-8BA5-F88B5093FA18}" name="Driver 2" dataDxfId="34"/>
+    <tableColumn id="11" xr3:uid="{022A346F-1EFC-477E-B3FF-234F17FB995D}" name="  NAT " dataDxfId="33"/>
+    <tableColumn id="14" xr3:uid="{4A5DA010-C6D1-49CE-8487-00AC7C736274}" name=" LIC " dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{15D47E2B-7108-41F5-BB6D-FABBD704C2C8}" name="CAT " dataDxfId="31"/>
+    <tableColumn id="8" xr3:uid="{5F578104-8A47-4C21-AE4F-A41AFD51CA17}" name="Car Sponsors" dataDxfId="30" dataCellStyle="Neutral"/>
+    <tableColumn id="7" xr3:uid="{37BFAE36-6B5E-4D59-B805-2A4B37B829ED}" name="Car Make/Model" dataDxfId="29"/>
+    <tableColumn id="9" xr3:uid="{C4134C49-64E4-4B01-865E-C1B755B7D04A}" name="Championship" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{EEF14E4E-087A-46C7-831D-A668229E00D6}" name="Table226" displayName="Table226" ref="A6:J37" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{EEF14E4E-087A-46C7-831D-A668229E00D6}" name="Table226" displayName="Table226" ref="A6:J37" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26" tableBorderDxfId="24" totalsRowBorderDxfId="23">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:J40">
     <sortCondition descending="1" ref="J8:J40"/>
     <sortCondition ref="B8:B40"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="2" xr3:uid="{29DF6422-9DDA-4F8F-8BEE-5184D2457B57}" name="Series" dataDxfId="24" dataCellStyle="Neutral"/>
-    <tableColumn id="10" xr3:uid="{1486B7A1-2318-4A69-93B1-14B85F40C988}" name="Car #" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{9FCCBAF6-EB7D-44F1-ADEC-A2DF74A549AE}" name="Team " dataDxfId="22" dataCellStyle="Neutral"/>
-    <tableColumn id="4" xr3:uid="{5972D2A1-6086-4595-9053-F6AB4ABD85A7}" name="Driver 1" dataDxfId="21" dataCellStyle="Neutral"/>
-    <tableColumn id="5" xr3:uid="{0273D45B-C8FF-4DBF-A963-B72D55D93954}" name="NAT" dataDxfId="20" dataCellStyle="Neutral"/>
-    <tableColumn id="13" xr3:uid="{26D97A36-D7BA-4D93-9A44-CC528D4BDC4F}" name="LIC " dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{AC25B573-C8BF-40ED-8E09-71D35117CA3A}" name="CAT" dataDxfId="18"/>
-    <tableColumn id="8" xr3:uid="{C3A46578-AA4D-4C94-B592-5AC371A17E14}" name="Car Sponsors" dataDxfId="17" dataCellStyle="Neutral"/>
-    <tableColumn id="7" xr3:uid="{7B3018A6-2A70-4C3E-BE5C-CCFFCABD4796}" name="Car Make/Model" dataDxfId="16"/>
-    <tableColumn id="9" xr3:uid="{C0209330-55B6-42D3-AB23-D1C37AFC6FDA}" name="Class" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{29DF6422-9DDA-4F8F-8BEE-5184D2457B57}" name="Series" dataDxfId="22" dataCellStyle="Neutral"/>
+    <tableColumn id="10" xr3:uid="{1486B7A1-2318-4A69-93B1-14B85F40C988}" name="Car #" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{9FCCBAF6-EB7D-44F1-ADEC-A2DF74A549AE}" name="Team " dataDxfId="20" dataCellStyle="Neutral"/>
+    <tableColumn id="4" xr3:uid="{5972D2A1-6086-4595-9053-F6AB4ABD85A7}" name="Driver 1" dataDxfId="19" dataCellStyle="Neutral"/>
+    <tableColumn id="5" xr3:uid="{0273D45B-C8FF-4DBF-A963-B72D55D93954}" name="NAT" dataDxfId="18" dataCellStyle="Neutral"/>
+    <tableColumn id="13" xr3:uid="{26D97A36-D7BA-4D93-9A44-CC528D4BDC4F}" name="LIC " dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{AC25B573-C8BF-40ED-8E09-71D35117CA3A}" name="CAT" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{C3A46578-AA4D-4C94-B592-5AC371A17E14}" name="Car Sponsors" dataDxfId="15" dataCellStyle="Neutral"/>
+    <tableColumn id="7" xr3:uid="{7B3018A6-2A70-4C3E-BE5C-CCFFCABD4796}" name="Car Make/Model" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{C0209330-55B6-42D3-AB23-D1C37AFC6FDA}" name="Class" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{11330F46-3971-7D44-8FE5-B039A90EF352}" name="Table22683" displayName="Table22683" ref="A6:H34" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11" totalsRowBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{11330F46-3971-7D44-8FE5-B039A90EF352}" name="Table22683" displayName="Table22683" ref="A6:H34" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:H35">
     <sortCondition descending="1" ref="H12:H35"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="2" xr3:uid="{459DFC46-4742-6E42-8DBB-A583077730B7}" name="Series" dataDxfId="9" dataCellStyle="Neutral"/>
-    <tableColumn id="10" xr3:uid="{A735E01E-C722-8046-A3A7-EB4B8E9856D0}" name="Car #" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{6858B568-BE7E-DA44-A760-6A0FEC2B9951}" name="Team " dataDxfId="7" dataCellStyle="Neutral"/>
-    <tableColumn id="4" xr3:uid="{9302466E-96CC-B845-817B-5E7790246EEA}" name="Driver" dataDxfId="6" dataCellStyle="Neutral"/>
-    <tableColumn id="5" xr3:uid="{6F60649D-7A1A-6B47-AF8B-CDFA61A10C71}" name="NAT" dataDxfId="5" dataCellStyle="Neutral"/>
-    <tableColumn id="8" xr3:uid="{8224E110-2012-0E4B-A25F-B837877427FA}" name="Car Sponsors" dataDxfId="4" dataCellStyle="Neutral"/>
-    <tableColumn id="7" xr3:uid="{3ADFDE9D-B3A8-2D47-8CAD-6E4FB830231A}" name="Car Make/Model" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{B7E977BD-C739-704E-A4EB-5D75989E1112}" name="Class" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{459DFC46-4742-6E42-8DBB-A583077730B7}" name="Series" dataDxfId="7" dataCellStyle="Neutral"/>
+    <tableColumn id="10" xr3:uid="{A735E01E-C722-8046-A3A7-EB4B8E9856D0}" name="Car #" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{6858B568-BE7E-DA44-A760-6A0FEC2B9951}" name="Team " dataDxfId="5" dataCellStyle="Neutral"/>
+    <tableColumn id="4" xr3:uid="{9302466E-96CC-B845-817B-5E7790246EEA}" name="Driver" dataDxfId="4" dataCellStyle="Neutral"/>
+    <tableColumn id="5" xr3:uid="{6F60649D-7A1A-6B47-AF8B-CDFA61A10C71}" name="NAT" dataDxfId="3" dataCellStyle="Neutral"/>
+    <tableColumn id="8" xr3:uid="{8224E110-2012-0E4B-A25F-B837877427FA}" name="Car Sponsors" dataDxfId="2" dataCellStyle="Neutral"/>
+    <tableColumn id="7" xr3:uid="{3ADFDE9D-B3A8-2D47-8CAD-6E4FB830231A}" name="Car Make/Model" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{B7E977BD-C739-704E-A4EB-5D75989E1112}" name="Class" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6187,8 +6196,8 @@
   </sheetPr>
   <dimension ref="A2:X34"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="80" zoomScaleNormal="90" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView view="pageLayout" zoomScale="80" zoomScaleNormal="90" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6210,65 +6219,65 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="516"/>
-      <c r="B2" s="516"/>
-      <c r="C2" s="516"/>
-      <c r="D2" s="516"/>
-      <c r="E2" s="516"/>
-      <c r="F2" s="516"/>
-      <c r="G2" s="516"/>
-      <c r="H2" s="516"/>
-      <c r="I2" s="516"/>
-      <c r="J2" s="516"/>
-      <c r="K2" s="516"/>
-      <c r="L2" s="516"/>
-      <c r="M2" s="516"/>
-      <c r="N2" s="516"/>
+      <c r="A2" s="523"/>
+      <c r="B2" s="523"/>
+      <c r="C2" s="523"/>
+      <c r="D2" s="530"/>
+      <c r="E2" s="530"/>
+      <c r="F2" s="530"/>
+      <c r="G2" s="530"/>
+      <c r="H2" s="530"/>
+      <c r="I2" s="530"/>
+      <c r="J2" s="530"/>
+      <c r="K2" s="530"/>
+      <c r="L2" s="530"/>
+      <c r="M2" s="523"/>
+      <c r="N2" s="523"/>
     </row>
     <row r="3" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="516"/>
-      <c r="B3" s="516"/>
-      <c r="C3" s="516"/>
-      <c r="D3" s="520" t="s">
+      <c r="A3" s="523"/>
+      <c r="B3" s="523"/>
+      <c r="C3" s="523"/>
+      <c r="D3" s="524" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="520"/>
-      <c r="F3" s="520"/>
-      <c r="G3" s="520"/>
-      <c r="H3" s="520"/>
-      <c r="I3" s="520"/>
-      <c r="J3" s="520"/>
-      <c r="K3" s="520"/>
-      <c r="L3" s="520"/>
-      <c r="M3" s="516"/>
-      <c r="N3" s="516"/>
+      <c r="E3" s="524"/>
+      <c r="F3" s="524"/>
+      <c r="G3" s="524"/>
+      <c r="H3" s="524"/>
+      <c r="I3" s="524"/>
+      <c r="J3" s="524"/>
+      <c r="K3" s="524"/>
+      <c r="L3" s="524"/>
+      <c r="M3" s="523"/>
+      <c r="N3" s="523"/>
     </row>
     <row r="4" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="516"/>
-      <c r="B4" s="516"/>
-      <c r="C4" s="516"/>
-      <c r="D4" s="516"/>
-      <c r="E4" s="516"/>
-      <c r="F4" s="516"/>
-      <c r="G4" s="516"/>
-      <c r="H4" s="516"/>
-      <c r="I4" s="516"/>
-      <c r="J4" s="516"/>
-      <c r="K4" s="516"/>
-      <c r="L4" s="516"/>
-      <c r="M4" s="516"/>
-      <c r="N4" s="516"/>
+      <c r="A4" s="523"/>
+      <c r="B4" s="523"/>
+      <c r="C4" s="523"/>
+      <c r="D4" s="530"/>
+      <c r="E4" s="530"/>
+      <c r="F4" s="530"/>
+      <c r="G4" s="530"/>
+      <c r="H4" s="530"/>
+      <c r="I4" s="530"/>
+      <c r="J4" s="530"/>
+      <c r="K4" s="530"/>
+      <c r="L4" s="530"/>
+      <c r="M4" s="523"/>
+      <c r="N4" s="523"/>
     </row>
     <row r="5" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="R5" s="516" t="s">
+      <c r="R5" s="523" t="s">
         <v>0</v>
       </c>
-      <c r="S5" s="516"/>
-      <c r="T5" s="516"/>
-      <c r="U5" s="516"/>
-      <c r="V5" s="516"/>
-      <c r="W5" s="516"/>
-      <c r="X5" s="516"/>
+      <c r="S5" s="523"/>
+      <c r="T5" s="523"/>
+      <c r="U5" s="523"/>
+      <c r="V5" s="523"/>
+      <c r="W5" s="523"/>
+      <c r="X5" s="523"/>
     </row>
     <row r="6" spans="1:24" ht="32.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A6" s="224" t="s">
@@ -6339,8 +6348,8 @@
       </c>
     </row>
     <row r="7" spans="1:24" s="235" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="492"/>
-      <c r="B7" s="493"/>
+      <c r="A7" s="488"/>
+      <c r="B7" s="489"/>
       <c r="C7" s="230"/>
       <c r="D7" s="230"/>
       <c r="E7" s="230"/>
@@ -6365,8 +6374,8 @@
       <c r="X7" s="234"/>
     </row>
     <row r="8" spans="1:24" s="235" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="523"/>
-      <c r="B8" s="494"/>
+      <c r="A8" s="512"/>
+      <c r="B8" s="490"/>
       <c r="C8" s="236"/>
       <c r="D8" s="236"/>
       <c r="E8" s="236"/>
@@ -6391,8 +6400,8 @@
       <c r="X8" s="244"/>
     </row>
     <row r="9" spans="1:24" s="235" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="523"/>
-      <c r="B9" s="494"/>
+      <c r="A9" s="512"/>
+      <c r="B9" s="490"/>
       <c r="C9" s="237"/>
       <c r="D9" s="237"/>
       <c r="E9" s="237"/>
@@ -6417,8 +6426,8 @@
       <c r="X9" s="244"/>
     </row>
     <row r="10" spans="1:24" s="255" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="524"/>
-      <c r="B10" s="495"/>
+      <c r="A10" s="513"/>
+      <c r="B10" s="491"/>
       <c r="C10" s="247"/>
       <c r="D10" s="248"/>
       <c r="E10" s="248"/>
@@ -6440,8 +6449,8 @@
       <c r="X10" s="258"/>
     </row>
     <row r="11" spans="1:24" s="235" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="525"/>
-      <c r="B11" s="496"/>
+      <c r="A11" s="514"/>
+      <c r="B11" s="492"/>
       <c r="C11" s="30"/>
       <c r="D11" s="30"/>
       <c r="E11" s="30"/>
@@ -6463,8 +6472,8 @@
       <c r="X11" s="264"/>
     </row>
     <row r="12" spans="1:24" s="235" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="492"/>
-      <c r="B12" s="497"/>
+      <c r="A12" s="488"/>
+      <c r="B12" s="493"/>
       <c r="C12" s="230"/>
       <c r="D12" s="230"/>
       <c r="E12" s="230"/>
@@ -6486,8 +6495,8 @@
       <c r="X12" s="264"/>
     </row>
     <row r="13" spans="1:24" s="235" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="526"/>
-      <c r="B13" s="498"/>
+      <c r="A13" s="515"/>
+      <c r="B13" s="494"/>
       <c r="C13" s="265"/>
       <c r="D13" s="265"/>
       <c r="E13" s="265"/>
@@ -6509,8 +6518,8 @@
       <c r="X13" s="271"/>
     </row>
     <row r="14" spans="1:24" s="235" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="492"/>
-      <c r="B14" s="497"/>
+      <c r="A14" s="488"/>
+      <c r="B14" s="493"/>
       <c r="C14" s="230"/>
       <c r="D14" s="230"/>
       <c r="E14" s="230"/>
@@ -6532,8 +6541,8 @@
       <c r="X14" s="271"/>
     </row>
     <row r="15" spans="1:24" s="255" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="523"/>
-      <c r="B15" s="499"/>
+      <c r="A15" s="512"/>
+      <c r="B15" s="495"/>
       <c r="C15" s="30"/>
       <c r="D15" s="30"/>
       <c r="E15" s="30"/>
@@ -6555,8 +6564,8 @@
       <c r="X15" s="275"/>
     </row>
     <row r="16" spans="1:24" s="279" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="527"/>
-      <c r="B16" s="498"/>
+      <c r="A16" s="516"/>
+      <c r="B16" s="494"/>
       <c r="C16" s="265"/>
       <c r="D16" s="276"/>
       <c r="E16" s="238"/>
@@ -6578,8 +6587,8 @@
       <c r="X16" s="282"/>
     </row>
     <row r="17" spans="1:24" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="528"/>
-      <c r="B17" s="497"/>
+      <c r="A17" s="517"/>
+      <c r="B17" s="493"/>
       <c r="C17" s="230"/>
       <c r="D17" s="230"/>
       <c r="E17" s="230"/>
@@ -6601,8 +6610,8 @@
       <c r="X17" s="285"/>
     </row>
     <row r="18" spans="1:24" s="292" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="526"/>
-      <c r="B18" s="498"/>
+      <c r="A18" s="515"/>
+      <c r="B18" s="494"/>
       <c r="C18" s="286"/>
       <c r="D18" s="287"/>
       <c r="E18" s="265"/>
@@ -6624,8 +6633,8 @@
       <c r="X18" s="295"/>
     </row>
     <row r="19" spans="1:24" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="523"/>
-      <c r="B19" s="494"/>
+      <c r="A19" s="512"/>
+      <c r="B19" s="490"/>
       <c r="C19" s="296"/>
       <c r="D19" s="236"/>
       <c r="E19" s="236"/>
@@ -6647,8 +6656,8 @@
       <c r="X19" s="285"/>
     </row>
     <row r="20" spans="1:24" s="105" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="525"/>
-      <c r="B20" s="500"/>
+      <c r="A20" s="514"/>
+      <c r="B20" s="496"/>
       <c r="C20" s="30"/>
       <c r="D20" s="30"/>
       <c r="E20" s="30"/>
@@ -6670,8 +6679,8 @@
       <c r="X20" s="301"/>
     </row>
     <row r="21" spans="1:24" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="529"/>
-      <c r="B21" s="500"/>
+      <c r="A21" s="518"/>
+      <c r="B21" s="496"/>
       <c r="C21" s="260"/>
       <c r="D21" s="260"/>
       <c r="E21" s="260"/>
@@ -6693,8 +6702,8 @@
       <c r="X21" s="285"/>
     </row>
     <row r="22" spans="1:24" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="529"/>
-      <c r="B22" s="501"/>
+      <c r="A22" s="518"/>
+      <c r="B22" s="497"/>
       <c r="C22" s="303"/>
       <c r="D22" s="303"/>
       <c r="E22" s="303"/>
@@ -6716,8 +6725,8 @@
       <c r="X22" s="285"/>
     </row>
     <row r="23" spans="1:24" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="529"/>
-      <c r="B23" s="501"/>
+      <c r="A23" s="518"/>
+      <c r="B23" s="497"/>
       <c r="C23" s="303"/>
       <c r="D23" s="303"/>
       <c r="E23" s="303"/>
@@ -6739,8 +6748,8 @@
       <c r="X23" s="285"/>
     </row>
     <row r="24" spans="1:24" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="529"/>
-      <c r="B24" s="501"/>
+      <c r="A24" s="518"/>
+      <c r="B24" s="497"/>
       <c r="C24" s="303"/>
       <c r="D24" s="303"/>
       <c r="E24" s="303"/>
@@ -6762,8 +6771,8 @@
       <c r="X24" s="285"/>
     </row>
     <row r="25" spans="1:24" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="529"/>
-      <c r="B25" s="501"/>
+      <c r="A25" s="518"/>
+      <c r="B25" s="497"/>
       <c r="C25" s="303"/>
       <c r="D25" s="303"/>
       <c r="E25" s="303"/>
@@ -6785,8 +6794,8 @@
       <c r="X25" s="285"/>
     </row>
     <row r="26" spans="1:24" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="529"/>
-      <c r="B26" s="502"/>
+      <c r="A26" s="518"/>
+      <c r="B26" s="498"/>
       <c r="C26" s="304"/>
       <c r="D26" s="304"/>
       <c r="E26" s="304"/>
@@ -6808,8 +6817,8 @@
       <c r="X26" s="285"/>
     </row>
     <row r="27" spans="1:24" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="529"/>
-      <c r="B27" s="500"/>
+      <c r="A27" s="518"/>
+      <c r="B27" s="496"/>
       <c r="C27" s="260"/>
       <c r="D27" s="260"/>
       <c r="E27" s="260"/>
@@ -6918,8 +6927,8 @@
   </sheetPr>
   <dimension ref="A2:Y40"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A2" zoomScale="80" zoomScaleNormal="115" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView view="pageLayout" zoomScale="80" zoomScaleNormal="115" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6940,65 +6949,65 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="517"/>
-      <c r="B2" s="517"/>
-      <c r="C2" s="517"/>
-      <c r="D2" s="517"/>
-      <c r="E2" s="517"/>
-      <c r="F2" s="517"/>
-      <c r="G2" s="517"/>
-      <c r="H2" s="517"/>
-      <c r="I2" s="517"/>
-      <c r="J2" s="517"/>
-      <c r="K2" s="517"/>
-      <c r="L2" s="517"/>
-      <c r="M2" s="517"/>
-      <c r="N2" s="517"/>
+      <c r="A2" s="525"/>
+      <c r="B2" s="525"/>
+      <c r="C2" s="525"/>
+      <c r="D2" s="530"/>
+      <c r="E2" s="530"/>
+      <c r="F2" s="530"/>
+      <c r="G2" s="530"/>
+      <c r="H2" s="530"/>
+      <c r="I2" s="530"/>
+      <c r="J2" s="530"/>
+      <c r="K2" s="530"/>
+      <c r="L2" s="530"/>
+      <c r="M2" s="525"/>
+      <c r="N2" s="525"/>
     </row>
     <row r="3" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="517"/>
-      <c r="B3" s="517"/>
-      <c r="C3" s="517"/>
-      <c r="D3" s="519" t="s">
+      <c r="A3" s="525"/>
+      <c r="B3" s="525"/>
+      <c r="C3" s="525"/>
+      <c r="D3" s="524" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="519"/>
-      <c r="F3" s="519"/>
-      <c r="G3" s="519"/>
-      <c r="H3" s="519"/>
-      <c r="I3" s="519"/>
-      <c r="J3" s="519"/>
-      <c r="K3" s="519"/>
-      <c r="L3" s="519"/>
-      <c r="M3" s="517"/>
-      <c r="N3" s="517"/>
+      <c r="E3" s="524"/>
+      <c r="F3" s="524"/>
+      <c r="G3" s="524"/>
+      <c r="H3" s="524"/>
+      <c r="I3" s="524"/>
+      <c r="J3" s="524"/>
+      <c r="K3" s="524"/>
+      <c r="L3" s="524"/>
+      <c r="M3" s="525"/>
+      <c r="N3" s="525"/>
     </row>
     <row r="4" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="517"/>
-      <c r="B4" s="517"/>
-      <c r="C4" s="517"/>
-      <c r="D4" s="517"/>
-      <c r="E4" s="517"/>
-      <c r="F4" s="517"/>
-      <c r="G4" s="517"/>
-      <c r="H4" s="517"/>
-      <c r="I4" s="517"/>
-      <c r="J4" s="517"/>
-      <c r="K4" s="517"/>
-      <c r="L4" s="517"/>
-      <c r="M4" s="517"/>
-      <c r="N4" s="517"/>
+      <c r="A4" s="525"/>
+      <c r="B4" s="525"/>
+      <c r="C4" s="525"/>
+      <c r="D4" s="530"/>
+      <c r="E4" s="530"/>
+      <c r="F4" s="530"/>
+      <c r="G4" s="530"/>
+      <c r="H4" s="530"/>
+      <c r="I4" s="530"/>
+      <c r="J4" s="530"/>
+      <c r="K4" s="530"/>
+      <c r="L4" s="530"/>
+      <c r="M4" s="525"/>
+      <c r="N4" s="525"/>
     </row>
     <row r="5" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="R5" s="518" t="s">
+      <c r="R5" s="526" t="s">
         <v>0</v>
       </c>
-      <c r="S5" s="518"/>
-      <c r="T5" s="518"/>
-      <c r="U5" s="518"/>
-      <c r="V5" s="518"/>
-      <c r="W5" s="518"/>
-      <c r="X5" s="518"/>
+      <c r="S5" s="526"/>
+      <c r="T5" s="526"/>
+      <c r="U5" s="526"/>
+      <c r="V5" s="526"/>
+      <c r="W5" s="526"/>
+      <c r="X5" s="526"/>
     </row>
     <row r="6" spans="1:24" s="2" customFormat="1" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="219" t="s">
@@ -7844,7 +7853,7 @@
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.8"/>
-  <pageSetup scale="44" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="34" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;G</oddFooter>
   </headerFooter>
@@ -7864,7 +7873,7 @@
   <dimension ref="A2:R41"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScale="80" zoomScaleNormal="90" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D4" sqref="D4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7884,51 +7893,51 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="517"/>
-      <c r="B2" s="517"/>
-      <c r="C2" s="517"/>
-      <c r="D2" s="520"/>
-      <c r="E2" s="520"/>
-      <c r="F2" s="520"/>
-      <c r="G2" s="520"/>
-      <c r="H2" s="520"/>
-      <c r="I2" s="517"/>
-      <c r="J2" s="517"/>
+      <c r="A2" s="525"/>
+      <c r="B2" s="525"/>
+      <c r="C2" s="525"/>
+      <c r="D2" s="527"/>
+      <c r="E2" s="527"/>
+      <c r="F2" s="527"/>
+      <c r="G2" s="527"/>
+      <c r="H2" s="527"/>
+      <c r="I2" s="525"/>
+      <c r="J2" s="525"/>
     </row>
     <row r="3" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="517"/>
-      <c r="B3" s="517"/>
-      <c r="C3" s="517"/>
-      <c r="D3" s="520" t="s">
+      <c r="A3" s="525"/>
+      <c r="B3" s="525"/>
+      <c r="C3" s="525"/>
+      <c r="D3" s="527" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="520"/>
-      <c r="F3" s="520"/>
-      <c r="G3" s="520"/>
-      <c r="H3" s="520"/>
-      <c r="I3" s="517"/>
-      <c r="J3" s="517"/>
+      <c r="E3" s="527"/>
+      <c r="F3" s="527"/>
+      <c r="G3" s="527"/>
+      <c r="H3" s="527"/>
+      <c r="I3" s="525"/>
+      <c r="J3" s="525"/>
     </row>
     <row r="4" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="517"/>
-      <c r="B4" s="517"/>
-      <c r="C4" s="517"/>
-      <c r="D4" s="520"/>
-      <c r="E4" s="520"/>
-      <c r="F4" s="520"/>
-      <c r="G4" s="520"/>
-      <c r="H4" s="520"/>
-      <c r="I4" s="517"/>
-      <c r="J4" s="517"/>
+      <c r="A4" s="525"/>
+      <c r="B4" s="525"/>
+      <c r="C4" s="525"/>
+      <c r="D4" s="527"/>
+      <c r="E4" s="527"/>
+      <c r="F4" s="527"/>
+      <c r="G4" s="527"/>
+      <c r="H4" s="527"/>
+      <c r="I4" s="525"/>
+      <c r="J4" s="525"/>
     </row>
     <row r="5" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="N5" s="517" t="s">
+      <c r="N5" s="525" t="s">
         <v>0</v>
       </c>
-      <c r="O5" s="517"/>
-      <c r="P5" s="517"/>
-      <c r="Q5" s="517"/>
-      <c r="R5" s="517"/>
+      <c r="O5" s="525"/>
+      <c r="P5" s="525"/>
+      <c r="Q5" s="525"/>
+      <c r="R5" s="525"/>
     </row>
     <row r="6" spans="1:18" s="2" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -7981,16 +7990,16 @@
       </c>
     </row>
     <row r="7" spans="1:18" ht="54" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="375"/>
-      <c r="B7" s="503"/>
-      <c r="C7" s="382"/>
-      <c r="D7" s="383"/>
-      <c r="E7" s="382"/>
-      <c r="F7" s="382"/>
-      <c r="G7" s="383"/>
-      <c r="H7" s="384"/>
-      <c r="I7" s="385"/>
-      <c r="J7" s="382"/>
+      <c r="A7" s="371"/>
+      <c r="B7" s="499"/>
+      <c r="C7" s="378"/>
+      <c r="D7" s="379"/>
+      <c r="E7" s="378"/>
+      <c r="F7" s="378"/>
+      <c r="G7" s="379"/>
+      <c r="H7" s="380"/>
+      <c r="I7" s="381"/>
+      <c r="J7" s="378"/>
       <c r="N7" s="193"/>
       <c r="O7" s="46"/>
       <c r="P7" s="48"/>
@@ -7998,16 +8007,16 @@
       <c r="R7" s="194"/>
     </row>
     <row r="8" spans="1:18" s="45" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="375"/>
-      <c r="B8" s="504"/>
-      <c r="C8" s="386"/>
-      <c r="D8" s="386"/>
-      <c r="E8" s="386"/>
-      <c r="F8" s="387"/>
-      <c r="G8" s="386"/>
-      <c r="H8" s="386"/>
-      <c r="I8" s="386"/>
-      <c r="J8" s="386"/>
+      <c r="A8" s="371"/>
+      <c r="B8" s="500"/>
+      <c r="C8" s="382"/>
+      <c r="D8" s="382"/>
+      <c r="E8" s="382"/>
+      <c r="F8" s="383"/>
+      <c r="G8" s="382"/>
+      <c r="H8" s="382"/>
+      <c r="I8" s="382"/>
+      <c r="J8" s="382"/>
       <c r="N8" s="193"/>
       <c r="O8" s="46"/>
       <c r="P8" s="47"/>
@@ -8015,16 +8024,16 @@
       <c r="R8" s="195"/>
     </row>
     <row r="9" spans="1:18" s="32" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="376"/>
-      <c r="B9" s="505"/>
-      <c r="C9" s="388"/>
-      <c r="D9" s="389"/>
-      <c r="E9" s="389"/>
-      <c r="F9" s="389"/>
-      <c r="G9" s="389"/>
-      <c r="H9" s="390"/>
-      <c r="I9" s="391"/>
-      <c r="J9" s="389"/>
+      <c r="A9" s="372"/>
+      <c r="B9" s="501"/>
+      <c r="C9" s="384"/>
+      <c r="D9" s="385"/>
+      <c r="E9" s="385"/>
+      <c r="F9" s="385"/>
+      <c r="G9" s="385"/>
+      <c r="H9" s="386"/>
+      <c r="I9" s="387"/>
+      <c r="J9" s="385"/>
       <c r="N9" s="196"/>
       <c r="O9" s="46"/>
       <c r="P9" s="33"/>
@@ -8032,16 +8041,16 @@
       <c r="R9" s="197"/>
     </row>
     <row r="10" spans="1:18" s="32" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="377"/>
-      <c r="B10" s="506"/>
-      <c r="C10" s="392"/>
-      <c r="D10" s="392"/>
-      <c r="E10" s="393"/>
-      <c r="F10" s="394"/>
-      <c r="G10" s="395"/>
-      <c r="H10" s="396"/>
-      <c r="I10" s="395"/>
-      <c r="J10" s="397"/>
+      <c r="A10" s="373"/>
+      <c r="B10" s="502"/>
+      <c r="C10" s="388"/>
+      <c r="D10" s="388"/>
+      <c r="E10" s="389"/>
+      <c r="F10" s="390"/>
+      <c r="G10" s="391"/>
+      <c r="H10" s="392"/>
+      <c r="I10" s="391"/>
+      <c r="J10" s="393"/>
       <c r="N10" s="196"/>
       <c r="O10" s="46"/>
       <c r="P10" s="33"/>
@@ -8049,16 +8058,16 @@
       <c r="R10" s="197"/>
     </row>
     <row r="11" spans="1:18" s="43" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="378"/>
-      <c r="B11" s="507"/>
-      <c r="C11" s="398"/>
-      <c r="D11" s="399"/>
-      <c r="E11" s="399"/>
-      <c r="F11" s="398"/>
-      <c r="G11" s="398"/>
-      <c r="H11" s="400"/>
-      <c r="I11" s="401"/>
-      <c r="J11" s="398"/>
+      <c r="A11" s="374"/>
+      <c r="B11" s="503"/>
+      <c r="C11" s="394"/>
+      <c r="D11" s="395"/>
+      <c r="E11" s="395"/>
+      <c r="F11" s="394"/>
+      <c r="G11" s="394"/>
+      <c r="H11" s="396"/>
+      <c r="I11" s="397"/>
+      <c r="J11" s="394"/>
       <c r="N11" s="196"/>
       <c r="O11" s="46"/>
       <c r="P11" s="44"/>
@@ -8066,16 +8075,16 @@
       <c r="R11" s="198"/>
     </row>
     <row r="12" spans="1:18" s="43" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="378"/>
-      <c r="B12" s="508"/>
-      <c r="C12" s="392"/>
-      <c r="D12" s="392"/>
-      <c r="E12" s="393"/>
-      <c r="F12" s="394"/>
-      <c r="G12" s="402"/>
-      <c r="H12" s="403"/>
-      <c r="I12" s="402"/>
-      <c r="J12" s="397"/>
+      <c r="A12" s="374"/>
+      <c r="B12" s="504"/>
+      <c r="C12" s="388"/>
+      <c r="D12" s="388"/>
+      <c r="E12" s="389"/>
+      <c r="F12" s="390"/>
+      <c r="G12" s="398"/>
+      <c r="H12" s="399"/>
+      <c r="I12" s="398"/>
+      <c r="J12" s="393"/>
       <c r="N12" s="196"/>
       <c r="O12" s="46"/>
       <c r="P12" s="44"/>
@@ -8083,16 +8092,16 @@
       <c r="R12" s="198"/>
     </row>
     <row r="13" spans="1:18" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="375"/>
-      <c r="B13" s="504"/>
-      <c r="C13" s="386"/>
-      <c r="D13" s="386"/>
-      <c r="E13" s="386"/>
-      <c r="F13" s="387"/>
-      <c r="G13" s="386"/>
-      <c r="H13" s="386"/>
-      <c r="I13" s="386"/>
-      <c r="J13" s="386"/>
+      <c r="A13" s="371"/>
+      <c r="B13" s="500"/>
+      <c r="C13" s="382"/>
+      <c r="D13" s="382"/>
+      <c r="E13" s="382"/>
+      <c r="F13" s="383"/>
+      <c r="G13" s="382"/>
+      <c r="H13" s="382"/>
+      <c r="I13" s="382"/>
+      <c r="J13" s="382"/>
       <c r="N13" s="199"/>
       <c r="O13" s="46"/>
       <c r="P13" s="103"/>
@@ -8100,16 +8109,16 @@
       <c r="R13" s="200"/>
     </row>
     <row r="14" spans="1:18" s="105" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="376"/>
-      <c r="B14" s="509"/>
-      <c r="C14" s="388"/>
-      <c r="D14" s="388"/>
-      <c r="E14" s="388"/>
-      <c r="F14" s="388"/>
-      <c r="G14" s="404"/>
-      <c r="H14" s="405"/>
-      <c r="I14" s="388"/>
-      <c r="J14" s="406"/>
+      <c r="A14" s="372"/>
+      <c r="B14" s="505"/>
+      <c r="C14" s="384"/>
+      <c r="D14" s="384"/>
+      <c r="E14" s="384"/>
+      <c r="F14" s="384"/>
+      <c r="G14" s="400"/>
+      <c r="H14" s="401"/>
+      <c r="I14" s="384"/>
+      <c r="J14" s="402"/>
       <c r="N14" s="201"/>
       <c r="O14" s="46"/>
       <c r="P14" s="106"/>
@@ -8117,16 +8126,16 @@
       <c r="R14" s="202"/>
     </row>
     <row r="15" spans="1:18" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="375"/>
-      <c r="B15" s="510"/>
-      <c r="C15" s="408"/>
-      <c r="D15" s="408"/>
-      <c r="E15" s="408"/>
-      <c r="F15" s="409"/>
-      <c r="G15" s="407"/>
-      <c r="H15" s="408"/>
-      <c r="I15" s="408"/>
-      <c r="J15" s="408"/>
+      <c r="A15" s="371"/>
+      <c r="B15" s="506"/>
+      <c r="C15" s="404"/>
+      <c r="D15" s="404"/>
+      <c r="E15" s="404"/>
+      <c r="F15" s="405"/>
+      <c r="G15" s="403"/>
+      <c r="H15" s="404"/>
+      <c r="I15" s="404"/>
+      <c r="J15" s="404"/>
       <c r="N15" s="193"/>
       <c r="O15" s="46"/>
       <c r="P15" s="48"/>
@@ -8134,16 +8143,16 @@
       <c r="R15" s="194"/>
     </row>
     <row r="16" spans="1:18" s="89" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="375"/>
-      <c r="B16" s="511"/>
-      <c r="C16" s="386"/>
-      <c r="D16" s="386"/>
-      <c r="E16" s="386"/>
-      <c r="F16" s="410"/>
-      <c r="G16" s="386"/>
-      <c r="H16" s="386"/>
-      <c r="I16" s="398"/>
-      <c r="J16" s="386"/>
+      <c r="A16" s="371"/>
+      <c r="B16" s="507"/>
+      <c r="C16" s="382"/>
+      <c r="D16" s="382"/>
+      <c r="E16" s="382"/>
+      <c r="F16" s="406"/>
+      <c r="G16" s="382"/>
+      <c r="H16" s="382"/>
+      <c r="I16" s="394"/>
+      <c r="J16" s="382"/>
       <c r="N16" s="203"/>
       <c r="O16" s="46"/>
       <c r="P16" s="90"/>
@@ -8151,16 +8160,16 @@
       <c r="R16" s="204"/>
     </row>
     <row r="17" spans="1:18" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="375"/>
-      <c r="B17" s="511"/>
-      <c r="C17" s="386"/>
-      <c r="D17" s="386"/>
-      <c r="E17" s="386"/>
-      <c r="F17" s="387"/>
-      <c r="G17" s="411"/>
-      <c r="H17" s="412"/>
-      <c r="I17" s="412"/>
-      <c r="J17" s="386"/>
+      <c r="A17" s="371"/>
+      <c r="B17" s="507"/>
+      <c r="C17" s="382"/>
+      <c r="D17" s="382"/>
+      <c r="E17" s="382"/>
+      <c r="F17" s="383"/>
+      <c r="G17" s="407"/>
+      <c r="H17" s="408"/>
+      <c r="I17" s="408"/>
+      <c r="J17" s="382"/>
       <c r="N17" s="193"/>
       <c r="O17" s="46"/>
       <c r="P17" s="50"/>
@@ -8168,16 +8177,16 @@
       <c r="R17" s="205"/>
     </row>
     <row r="18" spans="1:18" s="45" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="375"/>
-      <c r="B18" s="512"/>
-      <c r="C18" s="392"/>
-      <c r="D18" s="392"/>
-      <c r="E18" s="393"/>
-      <c r="F18" s="394"/>
-      <c r="G18" s="402"/>
-      <c r="H18" s="403"/>
-      <c r="I18" s="402"/>
-      <c r="J18" s="397"/>
+      <c r="A18" s="371"/>
+      <c r="B18" s="508"/>
+      <c r="C18" s="388"/>
+      <c r="D18" s="388"/>
+      <c r="E18" s="389"/>
+      <c r="F18" s="390"/>
+      <c r="G18" s="398"/>
+      <c r="H18" s="399"/>
+      <c r="I18" s="398"/>
+      <c r="J18" s="393"/>
       <c r="N18" s="193"/>
       <c r="O18" s="46"/>
       <c r="P18" s="47"/>
@@ -8185,16 +8194,16 @@
       <c r="R18" s="195"/>
     </row>
     <row r="19" spans="1:18" s="45" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="379"/>
-      <c r="B19" s="513"/>
-      <c r="C19" s="413"/>
-      <c r="D19" s="413"/>
-      <c r="E19" s="414"/>
-      <c r="F19" s="394"/>
-      <c r="G19" s="402"/>
-      <c r="H19" s="403"/>
-      <c r="I19" s="402"/>
-      <c r="J19" s="397"/>
+      <c r="A19" s="375"/>
+      <c r="B19" s="509"/>
+      <c r="C19" s="409"/>
+      <c r="D19" s="409"/>
+      <c r="E19" s="410"/>
+      <c r="F19" s="390"/>
+      <c r="G19" s="398"/>
+      <c r="H19" s="399"/>
+      <c r="I19" s="398"/>
+      <c r="J19" s="393"/>
       <c r="N19" s="206"/>
       <c r="O19" s="46"/>
       <c r="P19" s="171"/>
@@ -8202,16 +8211,16 @@
       <c r="R19" s="207"/>
     </row>
     <row r="20" spans="1:18" s="45" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="380"/>
-      <c r="B20" s="512"/>
-      <c r="C20" s="415"/>
-      <c r="D20" s="416"/>
-      <c r="E20" s="417"/>
-      <c r="F20" s="394"/>
-      <c r="G20" s="402"/>
-      <c r="H20" s="415"/>
-      <c r="I20" s="402"/>
-      <c r="J20" s="397"/>
+      <c r="A20" s="376"/>
+      <c r="B20" s="508"/>
+      <c r="C20" s="411"/>
+      <c r="D20" s="412"/>
+      <c r="E20" s="413"/>
+      <c r="F20" s="390"/>
+      <c r="G20" s="398"/>
+      <c r="H20" s="411"/>
+      <c r="I20" s="398"/>
+      <c r="J20" s="393"/>
       <c r="N20" s="193"/>
       <c r="O20" s="46"/>
       <c r="P20" s="46"/>
@@ -8219,16 +8228,16 @@
       <c r="R20" s="208"/>
     </row>
     <row r="21" spans="1:18" s="45" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="375"/>
-      <c r="B21" s="510"/>
-      <c r="C21" s="407"/>
-      <c r="D21" s="407"/>
-      <c r="E21" s="407"/>
-      <c r="F21" s="418"/>
-      <c r="G21" s="419"/>
-      <c r="H21" s="420"/>
-      <c r="I21" s="386"/>
-      <c r="J21" s="407"/>
+      <c r="A21" s="371"/>
+      <c r="B21" s="506"/>
+      <c r="C21" s="403"/>
+      <c r="D21" s="403"/>
+      <c r="E21" s="403"/>
+      <c r="F21" s="414"/>
+      <c r="G21" s="415"/>
+      <c r="H21" s="416"/>
+      <c r="I21" s="382"/>
+      <c r="J21" s="403"/>
       <c r="N21" s="199"/>
       <c r="O21" s="46"/>
       <c r="P21" s="172"/>
@@ -8236,16 +8245,16 @@
       <c r="R21" s="209"/>
     </row>
     <row r="22" spans="1:18" s="34" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="376"/>
-      <c r="B22" s="514"/>
-      <c r="C22" s="421"/>
-      <c r="D22" s="422"/>
-      <c r="E22" s="423"/>
-      <c r="F22" s="423"/>
-      <c r="G22" s="422"/>
-      <c r="H22" s="424"/>
-      <c r="I22" s="425"/>
-      <c r="J22" s="426"/>
+      <c r="A22" s="372"/>
+      <c r="B22" s="510"/>
+      <c r="C22" s="417"/>
+      <c r="D22" s="418"/>
+      <c r="E22" s="419"/>
+      <c r="F22" s="419"/>
+      <c r="G22" s="418"/>
+      <c r="H22" s="420"/>
+      <c r="I22" s="421"/>
+      <c r="J22" s="422"/>
       <c r="N22" s="196"/>
       <c r="O22" s="46"/>
       <c r="P22" s="35"/>
@@ -8253,16 +8262,16 @@
       <c r="R22" s="210"/>
     </row>
     <row r="23" spans="1:18" s="98" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="375"/>
-      <c r="B23" s="508"/>
-      <c r="C23" s="416"/>
-      <c r="D23" s="416"/>
-      <c r="E23" s="417"/>
-      <c r="F23" s="394"/>
-      <c r="G23" s="427"/>
-      <c r="H23" s="428"/>
-      <c r="I23" s="382"/>
-      <c r="J23" s="397"/>
+      <c r="A23" s="371"/>
+      <c r="B23" s="504"/>
+      <c r="C23" s="412"/>
+      <c r="D23" s="412"/>
+      <c r="E23" s="413"/>
+      <c r="F23" s="390"/>
+      <c r="G23" s="423"/>
+      <c r="H23" s="424"/>
+      <c r="I23" s="378"/>
+      <c r="J23" s="393"/>
       <c r="N23" s="193"/>
       <c r="O23" s="46"/>
       <c r="P23" s="99"/>
@@ -8270,16 +8279,16 @@
       <c r="R23" s="211"/>
     </row>
     <row r="24" spans="1:18" s="34" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="376"/>
-      <c r="B24" s="508"/>
-      <c r="C24" s="392"/>
-      <c r="D24" s="392"/>
-      <c r="E24" s="393"/>
-      <c r="F24" s="394"/>
-      <c r="G24" s="416"/>
-      <c r="H24" s="403"/>
-      <c r="I24" s="402"/>
-      <c r="J24" s="397"/>
+      <c r="A24" s="372"/>
+      <c r="B24" s="504"/>
+      <c r="C24" s="388"/>
+      <c r="D24" s="388"/>
+      <c r="E24" s="389"/>
+      <c r="F24" s="390"/>
+      <c r="G24" s="412"/>
+      <c r="H24" s="399"/>
+      <c r="I24" s="398"/>
+      <c r="J24" s="393"/>
       <c r="N24" s="196"/>
       <c r="O24" s="46"/>
       <c r="P24" s="35"/>
@@ -8287,16 +8296,16 @@
       <c r="R24" s="210"/>
     </row>
     <row r="25" spans="1:18" s="98" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="376"/>
-      <c r="B25" s="514"/>
-      <c r="C25" s="422"/>
-      <c r="D25" s="422"/>
-      <c r="E25" s="429"/>
-      <c r="F25" s="421"/>
-      <c r="G25" s="421"/>
-      <c r="H25" s="430"/>
-      <c r="I25" s="421"/>
-      <c r="J25" s="431"/>
+      <c r="A25" s="372"/>
+      <c r="B25" s="510"/>
+      <c r="C25" s="418"/>
+      <c r="D25" s="418"/>
+      <c r="E25" s="425"/>
+      <c r="F25" s="417"/>
+      <c r="G25" s="417"/>
+      <c r="H25" s="426"/>
+      <c r="I25" s="417"/>
+      <c r="J25" s="427"/>
       <c r="N25" s="193"/>
       <c r="O25" s="46"/>
       <c r="P25" s="99"/>
@@ -8304,16 +8313,16 @@
       <c r="R25" s="211"/>
     </row>
     <row r="26" spans="1:18" s="98" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="376"/>
-      <c r="B26" s="514"/>
-      <c r="C26" s="422"/>
-      <c r="D26" s="422"/>
-      <c r="E26" s="429"/>
-      <c r="F26" s="421"/>
-      <c r="G26" s="421"/>
-      <c r="H26" s="430"/>
-      <c r="I26" s="421"/>
-      <c r="J26" s="443"/>
+      <c r="A26" s="372"/>
+      <c r="B26" s="510"/>
+      <c r="C26" s="418"/>
+      <c r="D26" s="418"/>
+      <c r="E26" s="425"/>
+      <c r="F26" s="417"/>
+      <c r="G26" s="417"/>
+      <c r="H26" s="426"/>
+      <c r="I26" s="417"/>
+      <c r="J26" s="439"/>
       <c r="N26" s="193"/>
       <c r="O26" s="46"/>
       <c r="P26" s="99"/>
@@ -8321,16 +8330,16 @@
       <c r="R26" s="211"/>
     </row>
     <row r="27" spans="1:18" s="98" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="376"/>
-      <c r="B27" s="514"/>
-      <c r="C27" s="422"/>
-      <c r="D27" s="422"/>
-      <c r="E27" s="429"/>
-      <c r="F27" s="421"/>
-      <c r="G27" s="421"/>
-      <c r="H27" s="430"/>
-      <c r="I27" s="421"/>
-      <c r="J27" s="443"/>
+      <c r="A27" s="372"/>
+      <c r="B27" s="510"/>
+      <c r="C27" s="418"/>
+      <c r="D27" s="418"/>
+      <c r="E27" s="425"/>
+      <c r="F27" s="417"/>
+      <c r="G27" s="417"/>
+      <c r="H27" s="426"/>
+      <c r="I27" s="417"/>
+      <c r="J27" s="439"/>
       <c r="N27" s="193"/>
       <c r="O27" s="46"/>
       <c r="P27" s="99"/>
@@ -8338,16 +8347,16 @@
       <c r="R27" s="211"/>
     </row>
     <row r="28" spans="1:18" s="98" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="376"/>
-      <c r="B28" s="514"/>
-      <c r="C28" s="422"/>
-      <c r="D28" s="422"/>
-      <c r="E28" s="429"/>
-      <c r="F28" s="421"/>
-      <c r="G28" s="421"/>
-      <c r="H28" s="430"/>
-      <c r="I28" s="421"/>
-      <c r="J28" s="443"/>
+      <c r="A28" s="372"/>
+      <c r="B28" s="510"/>
+      <c r="C28" s="418"/>
+      <c r="D28" s="418"/>
+      <c r="E28" s="425"/>
+      <c r="F28" s="417"/>
+      <c r="G28" s="417"/>
+      <c r="H28" s="426"/>
+      <c r="I28" s="417"/>
+      <c r="J28" s="439"/>
       <c r="N28" s="193"/>
       <c r="O28" s="46"/>
       <c r="P28" s="99"/>
@@ -8355,16 +8364,16 @@
       <c r="R28" s="211"/>
     </row>
     <row r="29" spans="1:18" s="98" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="376"/>
-      <c r="B29" s="514"/>
-      <c r="C29" s="422"/>
-      <c r="D29" s="422"/>
-      <c r="E29" s="429"/>
-      <c r="F29" s="421"/>
-      <c r="G29" s="421"/>
-      <c r="H29" s="430"/>
-      <c r="I29" s="421"/>
-      <c r="J29" s="443"/>
+      <c r="A29" s="372"/>
+      <c r="B29" s="510"/>
+      <c r="C29" s="418"/>
+      <c r="D29" s="418"/>
+      <c r="E29" s="425"/>
+      <c r="F29" s="417"/>
+      <c r="G29" s="417"/>
+      <c r="H29" s="426"/>
+      <c r="I29" s="417"/>
+      <c r="J29" s="439"/>
       <c r="N29" s="193"/>
       <c r="O29" s="46"/>
       <c r="P29" s="99"/>
@@ -8372,16 +8381,16 @@
       <c r="R29" s="211"/>
     </row>
     <row r="30" spans="1:18" s="98" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="376"/>
-      <c r="B30" s="514"/>
-      <c r="C30" s="422"/>
-      <c r="D30" s="422"/>
-      <c r="E30" s="429"/>
-      <c r="F30" s="421"/>
-      <c r="G30" s="421"/>
-      <c r="H30" s="430"/>
-      <c r="I30" s="421"/>
-      <c r="J30" s="443"/>
+      <c r="A30" s="372"/>
+      <c r="B30" s="510"/>
+      <c r="C30" s="418"/>
+      <c r="D30" s="418"/>
+      <c r="E30" s="425"/>
+      <c r="F30" s="417"/>
+      <c r="G30" s="417"/>
+      <c r="H30" s="426"/>
+      <c r="I30" s="417"/>
+      <c r="J30" s="439"/>
       <c r="N30" s="193"/>
       <c r="O30" s="46"/>
       <c r="P30" s="99"/>
@@ -8389,16 +8398,16 @@
       <c r="R30" s="211"/>
     </row>
     <row r="31" spans="1:18" s="98" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="376"/>
-      <c r="B31" s="514"/>
-      <c r="C31" s="422"/>
-      <c r="D31" s="422"/>
-      <c r="E31" s="429"/>
-      <c r="F31" s="421"/>
-      <c r="G31" s="421"/>
-      <c r="H31" s="430"/>
-      <c r="I31" s="421"/>
-      <c r="J31" s="443"/>
+      <c r="A31" s="372"/>
+      <c r="B31" s="510"/>
+      <c r="C31" s="418"/>
+      <c r="D31" s="418"/>
+      <c r="E31" s="425"/>
+      <c r="F31" s="417"/>
+      <c r="G31" s="417"/>
+      <c r="H31" s="426"/>
+      <c r="I31" s="417"/>
+      <c r="J31" s="439"/>
       <c r="N31" s="193"/>
       <c r="O31" s="46"/>
       <c r="P31" s="99"/>
@@ -8406,16 +8415,16 @@
       <c r="R31" s="211"/>
     </row>
     <row r="32" spans="1:18" s="98" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="376"/>
-      <c r="B32" s="514"/>
-      <c r="C32" s="422"/>
-      <c r="D32" s="422"/>
-      <c r="E32" s="429"/>
-      <c r="F32" s="421"/>
-      <c r="G32" s="421"/>
-      <c r="H32" s="430"/>
-      <c r="I32" s="421"/>
-      <c r="J32" s="443"/>
+      <c r="A32" s="372"/>
+      <c r="B32" s="510"/>
+      <c r="C32" s="418"/>
+      <c r="D32" s="418"/>
+      <c r="E32" s="425"/>
+      <c r="F32" s="417"/>
+      <c r="G32" s="417"/>
+      <c r="H32" s="426"/>
+      <c r="I32" s="417"/>
+      <c r="J32" s="439"/>
       <c r="N32" s="193"/>
       <c r="O32" s="46"/>
       <c r="P32" s="99"/>
@@ -8423,16 +8432,16 @@
       <c r="R32" s="211"/>
     </row>
     <row r="33" spans="1:18" s="45" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="375"/>
-      <c r="B33" s="508"/>
-      <c r="C33" s="402"/>
-      <c r="D33" s="432"/>
-      <c r="E33" s="394"/>
-      <c r="F33" s="402"/>
-      <c r="G33" s="416"/>
-      <c r="H33" s="432"/>
-      <c r="I33" s="433"/>
-      <c r="J33" s="397"/>
+      <c r="A33" s="371"/>
+      <c r="B33" s="504"/>
+      <c r="C33" s="398"/>
+      <c r="D33" s="428"/>
+      <c r="E33" s="390"/>
+      <c r="F33" s="398"/>
+      <c r="G33" s="412"/>
+      <c r="H33" s="428"/>
+      <c r="I33" s="429"/>
+      <c r="J33" s="393"/>
       <c r="N33" s="193"/>
       <c r="O33" s="46"/>
       <c r="P33" s="46"/>
@@ -8440,16 +8449,16 @@
       <c r="R33" s="195"/>
     </row>
     <row r="34" spans="1:18" s="45" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="375"/>
-      <c r="B34" s="508"/>
-      <c r="C34" s="402"/>
-      <c r="D34" s="432"/>
-      <c r="E34" s="394"/>
-      <c r="F34" s="402"/>
-      <c r="G34" s="416"/>
-      <c r="H34" s="432"/>
-      <c r="I34" s="433"/>
-      <c r="J34" s="397"/>
+      <c r="A34" s="371"/>
+      <c r="B34" s="504"/>
+      <c r="C34" s="398"/>
+      <c r="D34" s="428"/>
+      <c r="E34" s="390"/>
+      <c r="F34" s="398"/>
+      <c r="G34" s="412"/>
+      <c r="H34" s="428"/>
+      <c r="I34" s="429"/>
+      <c r="J34" s="393"/>
       <c r="N34" s="193"/>
       <c r="O34" s="46"/>
       <c r="P34" s="46"/>
@@ -8457,16 +8466,16 @@
       <c r="R34" s="195"/>
     </row>
     <row r="35" spans="1:18" s="45" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="375"/>
-      <c r="B35" s="508"/>
-      <c r="C35" s="402"/>
-      <c r="D35" s="432"/>
-      <c r="E35" s="394"/>
-      <c r="F35" s="394"/>
-      <c r="G35" s="427"/>
-      <c r="H35" s="432"/>
-      <c r="I35" s="433"/>
-      <c r="J35" s="397"/>
+      <c r="A35" s="371"/>
+      <c r="B35" s="504"/>
+      <c r="C35" s="398"/>
+      <c r="D35" s="428"/>
+      <c r="E35" s="390"/>
+      <c r="F35" s="390"/>
+      <c r="G35" s="423"/>
+      <c r="H35" s="428"/>
+      <c r="I35" s="429"/>
+      <c r="J35" s="393"/>
       <c r="N35" s="193"/>
       <c r="O35" s="46"/>
       <c r="P35" s="46"/>
@@ -8474,16 +8483,16 @@
       <c r="R35" s="195"/>
     </row>
     <row r="36" spans="1:18" s="45" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="375"/>
-      <c r="B36" s="510"/>
-      <c r="C36" s="407"/>
-      <c r="D36" s="407"/>
-      <c r="E36" s="407"/>
-      <c r="F36" s="418"/>
-      <c r="G36" s="419"/>
-      <c r="H36" s="407"/>
-      <c r="I36" s="407"/>
-      <c r="J36" s="434"/>
+      <c r="A36" s="371"/>
+      <c r="B36" s="506"/>
+      <c r="C36" s="403"/>
+      <c r="D36" s="403"/>
+      <c r="E36" s="403"/>
+      <c r="F36" s="414"/>
+      <c r="G36" s="415"/>
+      <c r="H36" s="403"/>
+      <c r="I36" s="403"/>
+      <c r="J36" s="430"/>
       <c r="N36" s="193"/>
       <c r="O36" s="46"/>
       <c r="P36" s="47"/>
@@ -8491,16 +8500,16 @@
       <c r="R36" s="195"/>
     </row>
     <row r="37" spans="1:18" s="96" customFormat="1" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="381"/>
-      <c r="B37" s="515"/>
-      <c r="C37" s="435"/>
-      <c r="D37" s="436"/>
-      <c r="E37" s="437"/>
-      <c r="F37" s="438"/>
-      <c r="G37" s="439"/>
-      <c r="H37" s="440"/>
-      <c r="I37" s="441"/>
-      <c r="J37" s="442"/>
+      <c r="A37" s="377"/>
+      <c r="B37" s="511"/>
+      <c r="C37" s="431"/>
+      <c r="D37" s="432"/>
+      <c r="E37" s="433"/>
+      <c r="F37" s="434"/>
+      <c r="G37" s="435"/>
+      <c r="H37" s="436"/>
+      <c r="I37" s="437"/>
+      <c r="J37" s="438"/>
       <c r="N37" s="212"/>
       <c r="O37" s="213"/>
       <c r="P37" s="214"/>
@@ -8592,8 +8601,8 @@
   </sheetPr>
   <dimension ref="A2:BP36"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A23" zoomScale="80" zoomScaleNormal="70" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView view="pageLayout" zoomScale="80" zoomScaleNormal="70" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8612,71 +8621,71 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:68" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="517"/>
-      <c r="B2" s="517"/>
-      <c r="C2" s="517"/>
-      <c r="D2" s="520"/>
-      <c r="E2" s="520"/>
-      <c r="F2" s="520"/>
-      <c r="G2" s="517"/>
-      <c r="H2" s="517"/>
+      <c r="A2" s="525"/>
+      <c r="B2" s="525"/>
+      <c r="C2" s="525"/>
+      <c r="D2" s="527"/>
+      <c r="E2" s="527"/>
+      <c r="F2" s="527"/>
+      <c r="G2" s="525"/>
+      <c r="H2" s="525"/>
     </row>
     <row r="3" spans="1:68" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="517"/>
-      <c r="B3" s="517"/>
-      <c r="C3" s="517"/>
-      <c r="D3" s="520" t="s">
+      <c r="A3" s="525"/>
+      <c r="B3" s="525"/>
+      <c r="C3" s="525"/>
+      <c r="D3" s="527" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="520"/>
-      <c r="F3" s="520"/>
-      <c r="G3" s="517"/>
-      <c r="H3" s="517"/>
+      <c r="E3" s="527"/>
+      <c r="F3" s="527"/>
+      <c r="G3" s="525"/>
+      <c r="H3" s="525"/>
     </row>
     <row r="4" spans="1:68" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="517"/>
-      <c r="B4" s="517"/>
-      <c r="C4" s="517"/>
-      <c r="D4" s="520"/>
-      <c r="E4" s="520"/>
-      <c r="F4" s="520"/>
-      <c r="G4" s="517"/>
-      <c r="H4" s="517"/>
+      <c r="A4" s="525"/>
+      <c r="B4" s="525"/>
+      <c r="C4" s="525"/>
+      <c r="D4" s="527"/>
+      <c r="E4" s="527"/>
+      <c r="F4" s="527"/>
+      <c r="G4" s="525"/>
+      <c r="H4" s="525"/>
     </row>
     <row r="5" spans="1:68" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L5" s="517" t="s">
+      <c r="L5" s="525" t="s">
         <v>0</v>
       </c>
-      <c r="M5" s="517"/>
-      <c r="N5" s="517"/>
-      <c r="O5" s="517"/>
-      <c r="P5" s="517"/>
-      <c r="Q5" s="517"/>
-      <c r="R5" s="517"/>
+      <c r="M5" s="525"/>
+      <c r="N5" s="525"/>
+      <c r="O5" s="525"/>
+      <c r="P5" s="525"/>
+      <c r="Q5" s="525"/>
+      <c r="R5" s="525"/>
     </row>
     <row r="6" spans="1:68" s="10" customFormat="1" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="372" t="s">
+      <c r="A6" s="368" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="373" t="s">
+      <c r="B6" s="369" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="373" t="s">
+      <c r="C6" s="369" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="373" t="s">
+      <c r="D6" s="369" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="373" t="s">
+      <c r="E6" s="369" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="373" t="s">
+      <c r="F6" s="369" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="373" t="s">
+      <c r="G6" s="369" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="374" t="s">
+      <c r="H6" s="370" t="s">
         <v>10</v>
       </c>
       <c r="I6" s="25"/>
@@ -8753,14 +8762,14 @@
       <c r="BP6" s="26"/>
     </row>
     <row r="7" spans="1:68" s="25" customFormat="1" ht="46.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="481"/>
-      <c r="B7" s="444"/>
-      <c r="C7" s="445"/>
-      <c r="D7" s="446"/>
-      <c r="E7" s="445"/>
-      <c r="F7" s="445"/>
-      <c r="G7" s="445"/>
-      <c r="H7" s="447"/>
+      <c r="A7" s="477"/>
+      <c r="B7" s="440"/>
+      <c r="C7" s="441"/>
+      <c r="D7" s="442"/>
+      <c r="E7" s="441"/>
+      <c r="F7" s="441"/>
+      <c r="G7" s="441"/>
+      <c r="H7" s="443"/>
       <c r="L7" s="326"/>
       <c r="M7" s="327"/>
       <c r="N7" s="328"/>
@@ -8770,14 +8779,14 @@
       <c r="R7" s="85"/>
     </row>
     <row r="8" spans="1:68" s="10" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="482"/>
-      <c r="B8" s="448"/>
-      <c r="C8" s="448"/>
-      <c r="D8" s="448"/>
-      <c r="E8" s="448"/>
-      <c r="F8" s="448"/>
-      <c r="G8" s="448"/>
-      <c r="H8" s="449"/>
+      <c r="A8" s="478"/>
+      <c r="B8" s="444"/>
+      <c r="C8" s="444"/>
+      <c r="D8" s="444"/>
+      <c r="E8" s="444"/>
+      <c r="F8" s="444"/>
+      <c r="G8" s="444"/>
+      <c r="H8" s="445"/>
       <c r="I8" s="25"/>
       <c r="J8" s="25"/>
       <c r="K8" s="25"/>
@@ -8840,14 +8849,14 @@
       <c r="BP8" s="26"/>
     </row>
     <row r="9" spans="1:68" s="10" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="483"/>
-      <c r="B9" s="450"/>
-      <c r="C9" s="451"/>
-      <c r="D9" s="452"/>
-      <c r="E9" s="451"/>
-      <c r="F9" s="451"/>
-      <c r="G9" s="451"/>
-      <c r="H9" s="453"/>
+      <c r="A9" s="479"/>
+      <c r="B9" s="446"/>
+      <c r="C9" s="447"/>
+      <c r="D9" s="448"/>
+      <c r="E9" s="447"/>
+      <c r="F9" s="447"/>
+      <c r="G9" s="447"/>
+      <c r="H9" s="449"/>
       <c r="I9" s="333"/>
       <c r="J9" s="334"/>
       <c r="K9" s="333"/>
@@ -8910,14 +8919,14 @@
       <c r="BP9" s="26"/>
     </row>
     <row r="10" spans="1:68" s="10" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="483"/>
-      <c r="B10" s="450"/>
-      <c r="C10" s="451"/>
-      <c r="D10" s="452"/>
-      <c r="E10" s="452"/>
-      <c r="F10" s="454"/>
-      <c r="G10" s="454"/>
-      <c r="H10" s="453"/>
+      <c r="A10" s="479"/>
+      <c r="B10" s="446"/>
+      <c r="C10" s="447"/>
+      <c r="D10" s="448"/>
+      <c r="E10" s="448"/>
+      <c r="F10" s="450"/>
+      <c r="G10" s="450"/>
+      <c r="H10" s="449"/>
       <c r="I10" s="25"/>
       <c r="J10" s="25"/>
       <c r="K10" s="25"/>
@@ -8980,14 +8989,14 @@
       <c r="BP10" s="26"/>
     </row>
     <row r="11" spans="1:68" s="10" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="483"/>
-      <c r="B11" s="455"/>
-      <c r="C11" s="451"/>
-      <c r="D11" s="452"/>
-      <c r="E11" s="451"/>
-      <c r="F11" s="451"/>
-      <c r="G11" s="454"/>
-      <c r="H11" s="453"/>
+      <c r="A11" s="479"/>
+      <c r="B11" s="451"/>
+      <c r="C11" s="447"/>
+      <c r="D11" s="448"/>
+      <c r="E11" s="447"/>
+      <c r="F11" s="447"/>
+      <c r="G11" s="450"/>
+      <c r="H11" s="449"/>
       <c r="I11" s="25"/>
       <c r="J11" s="25"/>
       <c r="K11" s="25"/>
@@ -9050,14 +9059,14 @@
       <c r="BP11" s="26"/>
     </row>
     <row r="12" spans="1:68" s="10" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="482"/>
-      <c r="B12" s="456"/>
-      <c r="C12" s="456"/>
-      <c r="D12" s="456"/>
-      <c r="E12" s="456"/>
-      <c r="F12" s="456"/>
-      <c r="G12" s="456"/>
-      <c r="H12" s="457"/>
+      <c r="A12" s="478"/>
+      <c r="B12" s="452"/>
+      <c r="C12" s="452"/>
+      <c r="D12" s="452"/>
+      <c r="E12" s="452"/>
+      <c r="F12" s="452"/>
+      <c r="G12" s="452"/>
+      <c r="H12" s="453"/>
       <c r="I12" s="25"/>
       <c r="J12" s="25"/>
       <c r="K12" s="25"/>
@@ -9120,14 +9129,14 @@
       <c r="BP12" s="26"/>
     </row>
     <row r="13" spans="1:68" s="124" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="484"/>
-      <c r="B13" s="458"/>
-      <c r="C13" s="459"/>
-      <c r="D13" s="459"/>
-      <c r="E13" s="459"/>
-      <c r="F13" s="459"/>
-      <c r="G13" s="459"/>
-      <c r="H13" s="460"/>
+      <c r="A13" s="480"/>
+      <c r="B13" s="454"/>
+      <c r="C13" s="455"/>
+      <c r="D13" s="455"/>
+      <c r="E13" s="455"/>
+      <c r="F13" s="455"/>
+      <c r="G13" s="455"/>
+      <c r="H13" s="456"/>
       <c r="I13" s="121"/>
       <c r="J13" s="121"/>
       <c r="K13" s="121"/>
@@ -9190,14 +9199,14 @@
       <c r="BP13" s="123"/>
     </row>
     <row r="14" spans="1:68" s="10" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="482"/>
-      <c r="B14" s="461"/>
-      <c r="C14" s="462"/>
-      <c r="D14" s="462"/>
-      <c r="E14" s="462"/>
-      <c r="F14" s="463"/>
-      <c r="G14" s="461"/>
-      <c r="H14" s="464"/>
+      <c r="A14" s="478"/>
+      <c r="B14" s="457"/>
+      <c r="C14" s="458"/>
+      <c r="D14" s="458"/>
+      <c r="E14" s="458"/>
+      <c r="F14" s="459"/>
+      <c r="G14" s="457"/>
+      <c r="H14" s="460"/>
       <c r="I14" s="25"/>
       <c r="J14" s="25"/>
       <c r="K14" s="25"/>
@@ -9260,14 +9269,14 @@
       <c r="BP14" s="26"/>
     </row>
     <row r="15" spans="1:68" s="124" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="484"/>
-      <c r="B15" s="465"/>
-      <c r="C15" s="466"/>
-      <c r="D15" s="466"/>
-      <c r="E15" s="466"/>
-      <c r="F15" s="467"/>
-      <c r="G15" s="465"/>
-      <c r="H15" s="468"/>
+      <c r="A15" s="480"/>
+      <c r="B15" s="461"/>
+      <c r="C15" s="462"/>
+      <c r="D15" s="462"/>
+      <c r="E15" s="462"/>
+      <c r="F15" s="463"/>
+      <c r="G15" s="461"/>
+      <c r="H15" s="464"/>
       <c r="I15" s="121"/>
       <c r="J15" s="121"/>
       <c r="K15" s="121"/>
@@ -9330,14 +9339,14 @@
       <c r="BP15" s="123"/>
     </row>
     <row r="16" spans="1:68" s="124" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="485"/>
-      <c r="B16" s="469"/>
-      <c r="C16" s="469"/>
-      <c r="D16" s="469"/>
-      <c r="E16" s="469"/>
-      <c r="F16" s="469"/>
-      <c r="G16" s="469"/>
-      <c r="H16" s="470"/>
+      <c r="A16" s="481"/>
+      <c r="B16" s="465"/>
+      <c r="C16" s="465"/>
+      <c r="D16" s="465"/>
+      <c r="E16" s="465"/>
+      <c r="F16" s="465"/>
+      <c r="G16" s="465"/>
+      <c r="H16" s="466"/>
       <c r="I16" s="121"/>
       <c r="J16" s="121"/>
       <c r="K16" s="121"/>
@@ -9397,14 +9406,14 @@
       <c r="BP16" s="123"/>
     </row>
     <row r="17" spans="1:68" s="124" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="486"/>
-      <c r="B17" s="465"/>
-      <c r="C17" s="466"/>
-      <c r="D17" s="466"/>
-      <c r="E17" s="466"/>
-      <c r="F17" s="467"/>
-      <c r="G17" s="465"/>
-      <c r="H17" s="468"/>
+      <c r="A17" s="482"/>
+      <c r="B17" s="461"/>
+      <c r="C17" s="462"/>
+      <c r="D17" s="462"/>
+      <c r="E17" s="462"/>
+      <c r="F17" s="463"/>
+      <c r="G17" s="461"/>
+      <c r="H17" s="464"/>
       <c r="I17" s="121"/>
       <c r="J17" s="121"/>
       <c r="K17" s="121"/>
@@ -9464,14 +9473,14 @@
       <c r="BP17" s="123"/>
     </row>
     <row r="18" spans="1:68" s="10" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="482"/>
-      <c r="B18" s="456"/>
-      <c r="C18" s="456"/>
-      <c r="D18" s="456"/>
-      <c r="E18" s="456"/>
-      <c r="F18" s="456"/>
-      <c r="G18" s="456"/>
-      <c r="H18" s="457"/>
+      <c r="A18" s="478"/>
+      <c r="B18" s="452"/>
+      <c r="C18" s="452"/>
+      <c r="D18" s="452"/>
+      <c r="E18" s="452"/>
+      <c r="F18" s="452"/>
+      <c r="G18" s="452"/>
+      <c r="H18" s="453"/>
       <c r="I18" s="25"/>
       <c r="J18" s="25"/>
       <c r="K18" s="25"/>
@@ -9531,14 +9540,14 @@
       <c r="BP18" s="26"/>
     </row>
     <row r="19" spans="1:68" s="10" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="482"/>
-      <c r="B19" s="456"/>
-      <c r="C19" s="456"/>
-      <c r="D19" s="456"/>
-      <c r="E19" s="456"/>
-      <c r="F19" s="456"/>
-      <c r="G19" s="456"/>
-      <c r="H19" s="457"/>
+      <c r="A19" s="478"/>
+      <c r="B19" s="452"/>
+      <c r="C19" s="452"/>
+      <c r="D19" s="452"/>
+      <c r="E19" s="452"/>
+      <c r="F19" s="452"/>
+      <c r="G19" s="452"/>
+      <c r="H19" s="453"/>
       <c r="I19" s="25"/>
       <c r="J19" s="25"/>
       <c r="K19" s="25"/>
@@ -9598,14 +9607,14 @@
       <c r="BP19" s="26"/>
     </row>
     <row r="20" spans="1:68" s="10" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="482"/>
-      <c r="B20" s="456"/>
-      <c r="C20" s="456"/>
-      <c r="D20" s="456"/>
-      <c r="E20" s="456"/>
-      <c r="F20" s="456"/>
-      <c r="G20" s="456"/>
-      <c r="H20" s="457"/>
+      <c r="A20" s="478"/>
+      <c r="B20" s="452"/>
+      <c r="C20" s="452"/>
+      <c r="D20" s="452"/>
+      <c r="E20" s="452"/>
+      <c r="F20" s="452"/>
+      <c r="G20" s="452"/>
+      <c r="H20" s="453"/>
       <c r="I20" s="25"/>
       <c r="J20" s="25"/>
       <c r="K20" s="25"/>
@@ -9665,14 +9674,14 @@
       <c r="BP20" s="26"/>
     </row>
     <row r="21" spans="1:68" s="10" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="484"/>
-      <c r="B21" s="471"/>
-      <c r="C21" s="472"/>
-      <c r="D21" s="473"/>
-      <c r="E21" s="473"/>
-      <c r="F21" s="472"/>
-      <c r="G21" s="471"/>
-      <c r="H21" s="474"/>
+      <c r="A21" s="480"/>
+      <c r="B21" s="467"/>
+      <c r="C21" s="468"/>
+      <c r="D21" s="469"/>
+      <c r="E21" s="469"/>
+      <c r="F21" s="468"/>
+      <c r="G21" s="467"/>
+      <c r="H21" s="470"/>
       <c r="I21" s="25"/>
       <c r="J21" s="25"/>
       <c r="K21" s="25"/>
@@ -9732,14 +9741,14 @@
       <c r="BP21" s="26"/>
     </row>
     <row r="22" spans="1:68" s="10" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="484"/>
-      <c r="B22" s="456"/>
-      <c r="C22" s="456"/>
-      <c r="D22" s="456"/>
-      <c r="E22" s="456"/>
-      <c r="F22" s="456"/>
-      <c r="G22" s="456"/>
-      <c r="H22" s="457"/>
+      <c r="A22" s="480"/>
+      <c r="B22" s="452"/>
+      <c r="C22" s="452"/>
+      <c r="D22" s="452"/>
+      <c r="E22" s="452"/>
+      <c r="F22" s="452"/>
+      <c r="G22" s="452"/>
+      <c r="H22" s="453"/>
       <c r="I22" s="25"/>
       <c r="J22" s="25"/>
       <c r="K22" s="25"/>
@@ -9799,14 +9808,14 @@
       <c r="BP22" s="26"/>
     </row>
     <row r="23" spans="1:68" s="10" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="482"/>
-      <c r="B23" s="461"/>
-      <c r="C23" s="463"/>
-      <c r="D23" s="462"/>
-      <c r="E23" s="462"/>
-      <c r="F23" s="463"/>
-      <c r="G23" s="461"/>
-      <c r="H23" s="464"/>
+      <c r="A23" s="478"/>
+      <c r="B23" s="457"/>
+      <c r="C23" s="459"/>
+      <c r="D23" s="458"/>
+      <c r="E23" s="458"/>
+      <c r="F23" s="459"/>
+      <c r="G23" s="457"/>
+      <c r="H23" s="460"/>
       <c r="I23" s="25"/>
       <c r="J23" s="25"/>
       <c r="K23" s="25"/>
@@ -9866,14 +9875,14 @@
       <c r="BP23" s="26"/>
     </row>
     <row r="24" spans="1:68" s="124" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="484"/>
-      <c r="B24" s="475"/>
-      <c r="C24" s="475"/>
-      <c r="D24" s="475"/>
-      <c r="E24" s="475"/>
-      <c r="F24" s="475"/>
-      <c r="G24" s="475"/>
-      <c r="H24" s="476"/>
+      <c r="A24" s="480"/>
+      <c r="B24" s="471"/>
+      <c r="C24" s="471"/>
+      <c r="D24" s="471"/>
+      <c r="E24" s="471"/>
+      <c r="F24" s="471"/>
+      <c r="G24" s="471"/>
+      <c r="H24" s="472"/>
       <c r="I24" s="121"/>
       <c r="J24" s="121"/>
       <c r="K24" s="121"/>
@@ -9933,14 +9942,14 @@
       <c r="BP24" s="123"/>
     </row>
     <row r="25" spans="1:68" s="10" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="482"/>
-      <c r="B25" s="456"/>
-      <c r="C25" s="456"/>
-      <c r="D25" s="456"/>
-      <c r="E25" s="456"/>
-      <c r="F25" s="456"/>
-      <c r="G25" s="456"/>
-      <c r="H25" s="457"/>
+      <c r="A25" s="478"/>
+      <c r="B25" s="452"/>
+      <c r="C25" s="452"/>
+      <c r="D25" s="452"/>
+      <c r="E25" s="452"/>
+      <c r="F25" s="452"/>
+      <c r="G25" s="452"/>
+      <c r="H25" s="453"/>
       <c r="I25" s="25"/>
       <c r="J25" s="25"/>
       <c r="K25" s="25"/>
@@ -10000,14 +10009,14 @@
       <c r="BP25" s="26"/>
     </row>
     <row r="26" spans="1:68" s="344" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="482"/>
-      <c r="B26" s="456"/>
-      <c r="C26" s="456"/>
-      <c r="D26" s="456"/>
-      <c r="E26" s="456"/>
-      <c r="F26" s="456"/>
-      <c r="G26" s="456"/>
-      <c r="H26" s="457"/>
+      <c r="A26" s="478"/>
+      <c r="B26" s="452"/>
+      <c r="C26" s="452"/>
+      <c r="D26" s="452"/>
+      <c r="E26" s="452"/>
+      <c r="F26" s="452"/>
+      <c r="G26" s="452"/>
+      <c r="H26" s="453"/>
       <c r="I26" s="342"/>
       <c r="J26" s="342"/>
       <c r="K26" s="342"/>
@@ -10067,14 +10076,14 @@
       <c r="BP26" s="346"/>
     </row>
     <row r="27" spans="1:68" s="344" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="487"/>
-      <c r="B27" s="461"/>
-      <c r="C27" s="462"/>
-      <c r="D27" s="462"/>
-      <c r="E27" s="462"/>
-      <c r="F27" s="463"/>
-      <c r="G27" s="461"/>
-      <c r="H27" s="464"/>
+      <c r="A27" s="483"/>
+      <c r="B27" s="457"/>
+      <c r="C27" s="458"/>
+      <c r="D27" s="458"/>
+      <c r="E27" s="458"/>
+      <c r="F27" s="459"/>
+      <c r="G27" s="457"/>
+      <c r="H27" s="460"/>
       <c r="I27" s="342"/>
       <c r="J27" s="342"/>
       <c r="K27" s="342"/>
@@ -10134,14 +10143,14 @@
       <c r="BP27" s="346"/>
     </row>
     <row r="28" spans="1:68" s="344" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="488"/>
-      <c r="B28" s="461"/>
-      <c r="C28" s="462"/>
-      <c r="D28" s="462"/>
-      <c r="E28" s="462"/>
-      <c r="F28" s="463"/>
-      <c r="G28" s="461"/>
-      <c r="H28" s="464"/>
+      <c r="A28" s="484"/>
+      <c r="B28" s="457"/>
+      <c r="C28" s="458"/>
+      <c r="D28" s="458"/>
+      <c r="E28" s="458"/>
+      <c r="F28" s="459"/>
+      <c r="G28" s="457"/>
+      <c r="H28" s="460"/>
       <c r="I28" s="342"/>
       <c r="J28" s="342"/>
       <c r="K28" s="342"/>
@@ -10201,14 +10210,14 @@
       <c r="BP28" s="346"/>
     </row>
     <row r="29" spans="1:68" s="344" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="488"/>
-      <c r="B29" s="461"/>
-      <c r="C29" s="462"/>
-      <c r="D29" s="462"/>
-      <c r="E29" s="462"/>
-      <c r="F29" s="463"/>
-      <c r="G29" s="461"/>
-      <c r="H29" s="464"/>
+      <c r="A29" s="484"/>
+      <c r="B29" s="457"/>
+      <c r="C29" s="458"/>
+      <c r="D29" s="458"/>
+      <c r="E29" s="458"/>
+      <c r="F29" s="459"/>
+      <c r="G29" s="457"/>
+      <c r="H29" s="460"/>
       <c r="I29" s="342"/>
       <c r="J29" s="342"/>
       <c r="K29" s="342"/>
@@ -10268,14 +10277,14 @@
       <c r="BP29" s="346"/>
     </row>
     <row r="30" spans="1:68" s="344" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="488"/>
-      <c r="B30" s="461"/>
-      <c r="C30" s="462"/>
-      <c r="D30" s="462"/>
-      <c r="E30" s="462"/>
-      <c r="F30" s="463"/>
-      <c r="G30" s="461"/>
-      <c r="H30" s="464"/>
+      <c r="A30" s="484"/>
+      <c r="B30" s="457"/>
+      <c r="C30" s="458"/>
+      <c r="D30" s="458"/>
+      <c r="E30" s="458"/>
+      <c r="F30" s="459"/>
+      <c r="G30" s="457"/>
+      <c r="H30" s="460"/>
       <c r="I30" s="342"/>
       <c r="J30" s="342"/>
       <c r="K30" s="342"/>
@@ -10335,14 +10344,14 @@
       <c r="BP30" s="346"/>
     </row>
     <row r="31" spans="1:68" s="344" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="488"/>
-      <c r="B31" s="461"/>
-      <c r="C31" s="462"/>
-      <c r="D31" s="462"/>
-      <c r="E31" s="462"/>
-      <c r="F31" s="463"/>
-      <c r="G31" s="461"/>
-      <c r="H31" s="464"/>
+      <c r="A31" s="484"/>
+      <c r="B31" s="457"/>
+      <c r="C31" s="458"/>
+      <c r="D31" s="458"/>
+      <c r="E31" s="458"/>
+      <c r="F31" s="459"/>
+      <c r="G31" s="457"/>
+      <c r="H31" s="460"/>
       <c r="I31" s="342"/>
       <c r="J31" s="342"/>
       <c r="K31" s="342"/>
@@ -10402,14 +10411,14 @@
       <c r="BP31" s="346"/>
     </row>
     <row r="32" spans="1:68" s="10" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="482"/>
-      <c r="B32" s="456"/>
-      <c r="C32" s="456"/>
-      <c r="D32" s="456"/>
-      <c r="E32" s="456"/>
-      <c r="F32" s="456"/>
-      <c r="G32" s="456"/>
-      <c r="H32" s="457"/>
+      <c r="A32" s="478"/>
+      <c r="B32" s="452"/>
+      <c r="C32" s="452"/>
+      <c r="D32" s="452"/>
+      <c r="E32" s="452"/>
+      <c r="F32" s="452"/>
+      <c r="G32" s="452"/>
+      <c r="H32" s="453"/>
       <c r="I32" s="25"/>
       <c r="J32" s="25"/>
       <c r="K32" s="25"/>
@@ -10469,14 +10478,14 @@
       <c r="BP32" s="26"/>
     </row>
     <row r="33" spans="1:68" s="124" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="489"/>
-      <c r="B33" s="475"/>
-      <c r="C33" s="475"/>
-      <c r="D33" s="472"/>
-      <c r="E33" s="472"/>
-      <c r="F33" s="477"/>
-      <c r="G33" s="477"/>
-      <c r="H33" s="476"/>
+      <c r="A33" s="485"/>
+      <c r="B33" s="471"/>
+      <c r="C33" s="471"/>
+      <c r="D33" s="468"/>
+      <c r="E33" s="468"/>
+      <c r="F33" s="473"/>
+      <c r="G33" s="473"/>
+      <c r="H33" s="472"/>
       <c r="I33" s="121"/>
       <c r="J33" s="121"/>
       <c r="K33" s="121"/>
@@ -10536,14 +10545,14 @@
       <c r="BP33" s="123"/>
     </row>
     <row r="34" spans="1:68" s="10" customFormat="1" ht="46.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="490"/>
-      <c r="B34" s="478"/>
-      <c r="C34" s="479"/>
-      <c r="D34" s="479"/>
-      <c r="E34" s="479"/>
-      <c r="F34" s="479"/>
-      <c r="G34" s="478"/>
-      <c r="H34" s="480"/>
+      <c r="A34" s="486"/>
+      <c r="B34" s="474"/>
+      <c r="C34" s="475"/>
+      <c r="D34" s="475"/>
+      <c r="E34" s="475"/>
+      <c r="F34" s="475"/>
+      <c r="G34" s="474"/>
+      <c r="H34" s="476"/>
       <c r="I34" s="25"/>
       <c r="J34" s="25"/>
       <c r="K34" s="25"/>
@@ -10607,16 +10616,16 @@
     </row>
     <row r="35" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="188"/>
-      <c r="B35" s="370"/>
+      <c r="B35" s="366"/>
       <c r="C35" s="188"/>
       <c r="D35" s="188"/>
       <c r="E35" s="188"/>
       <c r="F35" s="189"/>
-      <c r="G35" s="371"/>
-      <c r="H35" s="371"/>
+      <c r="G35" s="367"/>
+      <c r="H35" s="367"/>
     </row>
     <row r="36" spans="1:68" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="491" t="s">
+      <c r="A36" s="487" t="s">
         <v>17</v>
       </c>
       <c r="B36" s="350">
@@ -10654,8 +10663,8 @@
   </sheetPr>
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10694,14 +10703,14 @@
       <c r="N1" s="12"/>
     </row>
     <row r="2" spans="1:20" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="521"/>
-      <c r="B2" s="521"/>
-      <c r="C2" s="521"/>
-      <c r="D2" s="522"/>
-      <c r="E2" s="522"/>
-      <c r="F2" s="522"/>
-      <c r="G2" s="521"/>
-      <c r="H2" s="521"/>
+      <c r="A2" s="528"/>
+      <c r="B2" s="528"/>
+      <c r="C2" s="528"/>
+      <c r="D2" s="529"/>
+      <c r="E2" s="529"/>
+      <c r="F2" s="529"/>
+      <c r="G2" s="528"/>
+      <c r="H2" s="528"/>
       <c r="I2" s="12"/>
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
@@ -10716,16 +10725,16 @@
       <c r="T2" s="12"/>
     </row>
     <row r="3" spans="1:20" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="521"/>
-      <c r="B3" s="521"/>
-      <c r="C3" s="521"/>
-      <c r="D3" s="522" t="s">
+      <c r="A3" s="528"/>
+      <c r="B3" s="528"/>
+      <c r="C3" s="528"/>
+      <c r="D3" s="529" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="522"/>
-      <c r="F3" s="522"/>
-      <c r="G3" s="521"/>
-      <c r="H3" s="521"/>
+      <c r="E3" s="529"/>
+      <c r="F3" s="529"/>
+      <c r="G3" s="528"/>
+      <c r="H3" s="528"/>
       <c r="I3" s="12"/>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
@@ -10740,14 +10749,14 @@
       <c r="T3" s="12"/>
     </row>
     <row r="4" spans="1:20" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="521"/>
-      <c r="B4" s="521"/>
-      <c r="C4" s="521"/>
-      <c r="D4" s="522"/>
-      <c r="E4" s="522"/>
-      <c r="F4" s="522"/>
-      <c r="G4" s="521"/>
-      <c r="H4" s="521"/>
+      <c r="A4" s="528"/>
+      <c r="B4" s="528"/>
+      <c r="C4" s="528"/>
+      <c r="D4" s="529"/>
+      <c r="E4" s="529"/>
+      <c r="F4" s="529"/>
+      <c r="G4" s="528"/>
+      <c r="H4" s="528"/>
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
@@ -10784,28 +10793,28 @@
       <c r="T5" s="12"/>
     </row>
     <row r="6" spans="1:20" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="364" t="s">
+      <c r="A6" s="360" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="365" t="s">
+      <c r="B6" s="361" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="366" t="s">
+      <c r="C6" s="362" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="365" t="s">
+      <c r="D6" s="361" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="365" t="s">
+      <c r="E6" s="361" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="367" t="s">
+      <c r="F6" s="363" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="368" t="s">
+      <c r="G6" s="364" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="369" t="s">
+      <c r="H6" s="365" t="s">
         <v>22</v>
       </c>
       <c r="I6" s="20"/>
@@ -10832,14 +10841,14 @@
       <c r="T6" s="12"/>
     </row>
     <row r="7" spans="1:20" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="359"/>
+      <c r="A7" s="519"/>
       <c r="B7" s="109"/>
       <c r="C7" s="28"/>
       <c r="D7" s="28"/>
       <c r="E7" s="28"/>
       <c r="F7" s="28"/>
       <c r="G7" s="28"/>
-      <c r="H7" s="353"/>
+      <c r="H7" s="352"/>
       <c r="I7" s="20"/>
       <c r="J7" s="21"/>
       <c r="K7" s="13"/>
@@ -10854,14 +10863,14 @@
       <c r="T7" s="12"/>
     </row>
     <row r="8" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="351"/>
+      <c r="A8" s="520"/>
       <c r="B8" s="125"/>
       <c r="C8" s="49"/>
       <c r="D8" s="126"/>
       <c r="E8" s="126"/>
       <c r="F8" s="126"/>
       <c r="G8" s="126"/>
-      <c r="H8" s="352"/>
+      <c r="H8" s="351"/>
       <c r="I8" s="20"/>
       <c r="J8" s="21"/>
       <c r="K8" s="13"/>
@@ -10882,14 +10891,14 @@
       <c r="T8" s="12"/>
     </row>
     <row r="9" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="351"/>
+      <c r="A9" s="520"/>
       <c r="B9" s="27"/>
       <c r="C9" s="28"/>
       <c r="D9" s="28"/>
       <c r="E9" s="28"/>
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
-      <c r="H9" s="353"/>
+      <c r="H9" s="352"/>
       <c r="I9" s="20"/>
       <c r="J9" s="21"/>
       <c r="K9" s="13"/>
@@ -10904,14 +10913,14 @@
       <c r="T9" s="12"/>
     </row>
     <row r="10" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="351"/>
+      <c r="A10" s="520"/>
       <c r="B10" s="27"/>
       <c r="C10" s="28"/>
       <c r="D10" s="28"/>
       <c r="E10" s="28"/>
       <c r="F10" s="28"/>
       <c r="G10" s="28"/>
-      <c r="H10" s="353"/>
+      <c r="H10" s="352"/>
       <c r="I10" s="20"/>
       <c r="J10" s="132"/>
       <c r="K10" s="11"/>
@@ -10926,14 +10935,14 @@
       </c>
     </row>
     <row r="11" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="351"/>
+      <c r="A11" s="520"/>
       <c r="B11" s="27"/>
       <c r="C11" s="28"/>
       <c r="D11" s="28"/>
       <c r="E11" s="28"/>
       <c r="F11" s="28"/>
       <c r="G11" s="28"/>
-      <c r="H11" s="353"/>
+      <c r="H11" s="352"/>
       <c r="I11" s="20"/>
       <c r="J11" s="21"/>
       <c r="K11" s="13"/>
@@ -10948,14 +10957,14 @@
       <c r="T11" s="12"/>
     </row>
     <row r="12" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="351"/>
+      <c r="A12" s="520"/>
       <c r="B12" s="27"/>
       <c r="C12" s="28"/>
       <c r="D12" s="28"/>
       <c r="E12" s="111"/>
       <c r="F12" s="111"/>
       <c r="G12" s="28"/>
-      <c r="H12" s="353"/>
+      <c r="H12" s="352"/>
       <c r="I12" s="20"/>
       <c r="J12" s="21"/>
       <c r="K12" s="13"/>
@@ -10970,14 +10979,14 @@
       <c r="T12" s="12"/>
     </row>
     <row r="13" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="351"/>
+      <c r="A13" s="520"/>
       <c r="B13" s="27"/>
       <c r="C13" s="28"/>
       <c r="D13" s="107"/>
       <c r="E13" s="9"/>
       <c r="F13" s="162"/>
       <c r="G13" s="125"/>
-      <c r="H13" s="353"/>
+      <c r="H13" s="352"/>
       <c r="I13" s="20"/>
       <c r="J13" s="21"/>
       <c r="K13" s="13"/>
@@ -10992,14 +11001,14 @@
       <c r="T13" s="12"/>
     </row>
     <row r="14" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="351"/>
+      <c r="A14" s="520"/>
       <c r="B14" s="27"/>
       <c r="C14" s="28"/>
       <c r="D14" s="28"/>
       <c r="E14" s="107"/>
       <c r="F14" s="108"/>
       <c r="G14" s="28"/>
-      <c r="H14" s="353"/>
+      <c r="H14" s="352"/>
       <c r="I14" s="20"/>
       <c r="J14" s="21"/>
       <c r="K14" s="13"/>
@@ -11014,14 +11023,14 @@
       <c r="T14" s="12"/>
     </row>
     <row r="15" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="351"/>
+      <c r="A15" s="520"/>
       <c r="B15" s="27"/>
       <c r="C15" s="28"/>
       <c r="D15" s="28"/>
       <c r="E15" s="28"/>
       <c r="F15" s="28"/>
       <c r="G15" s="28"/>
-      <c r="H15" s="353"/>
+      <c r="H15" s="352"/>
       <c r="I15" s="20"/>
       <c r="J15" s="21"/>
       <c r="K15" s="13"/>
@@ -11036,14 +11045,14 @@
       <c r="T15" s="12"/>
     </row>
     <row r="16" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="351"/>
+      <c r="A16" s="520"/>
       <c r="B16" s="27"/>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
-      <c r="H16" s="353"/>
+      <c r="H16" s="352"/>
       <c r="J16" s="110"/>
       <c r="K16" s="110"/>
       <c r="L16" s="110"/>
@@ -11051,14 +11060,14 @@
       <c r="N16" s="110"/>
     </row>
     <row r="17" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="351"/>
+      <c r="A17" s="520"/>
       <c r="B17" s="27"/>
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
-      <c r="H17" s="353"/>
+      <c r="H17" s="352"/>
       <c r="I17" s="20"/>
       <c r="J17" s="21"/>
       <c r="K17" s="13"/>
@@ -11073,14 +11082,14 @@
       <c r="T17" s="12"/>
     </row>
     <row r="18" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="351"/>
+      <c r="A18" s="520"/>
       <c r="B18" s="27"/>
       <c r="C18" s="28"/>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
-      <c r="H18" s="353"/>
+      <c r="H18" s="352"/>
       <c r="J18" s="110"/>
       <c r="K18" s="110"/>
       <c r="L18" s="110"/>
@@ -11088,14 +11097,14 @@
       <c r="N18" s="110"/>
     </row>
     <row r="19" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="351"/>
+      <c r="A19" s="520"/>
       <c r="B19" s="27"/>
       <c r="C19" s="28"/>
       <c r="D19" s="111"/>
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
-      <c r="H19" s="353"/>
+      <c r="H19" s="352"/>
       <c r="I19" s="20"/>
       <c r="J19" s="21"/>
       <c r="K19" s="13"/>
@@ -11110,14 +11119,14 @@
       <c r="T19" s="12"/>
     </row>
     <row r="20" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="351"/>
+      <c r="A20" s="520"/>
       <c r="B20" s="154"/>
       <c r="C20" s="155"/>
       <c r="D20" s="156"/>
       <c r="E20" s="132"/>
       <c r="F20" s="157"/>
       <c r="G20" s="158"/>
-      <c r="H20" s="355"/>
+      <c r="H20" s="354"/>
       <c r="I20" s="20"/>
       <c r="J20" s="21"/>
       <c r="K20" s="13"/>
@@ -11132,14 +11141,14 @@
       <c r="T20" s="12"/>
     </row>
     <row r="21" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="351"/>
+      <c r="A21" s="520"/>
       <c r="B21" s="27"/>
       <c r="C21" s="28"/>
       <c r="D21" s="28"/>
       <c r="E21" s="28"/>
       <c r="F21" s="28"/>
       <c r="G21" s="28"/>
-      <c r="H21" s="353"/>
+      <c r="H21" s="352"/>
       <c r="I21" s="20"/>
       <c r="J21" s="21"/>
       <c r="K21" s="13"/>
@@ -11154,14 +11163,14 @@
       <c r="T21" s="12"/>
     </row>
     <row r="22" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="351"/>
+      <c r="A22" s="520"/>
       <c r="B22" s="27"/>
       <c r="C22" s="28"/>
       <c r="D22" s="28"/>
       <c r="E22" s="28"/>
       <c r="F22" s="28"/>
       <c r="G22" s="28"/>
-      <c r="H22" s="353"/>
+      <c r="H22" s="352"/>
       <c r="I22" s="20"/>
       <c r="J22" s="21"/>
       <c r="K22" s="13"/>
@@ -11176,14 +11185,14 @@
       <c r="T22" s="12"/>
     </row>
     <row r="23" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="351"/>
+      <c r="A23" s="520"/>
       <c r="B23" s="27"/>
       <c r="C23" s="28"/>
       <c r="D23" s="28"/>
       <c r="E23" s="28"/>
       <c r="F23" s="28"/>
       <c r="G23" s="28"/>
-      <c r="H23" s="353"/>
+      <c r="H23" s="352"/>
       <c r="I23" s="20"/>
       <c r="J23" s="21"/>
       <c r="K23" s="13"/>
@@ -11198,14 +11207,14 @@
       <c r="T23" s="12"/>
     </row>
     <row r="24" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="351"/>
+      <c r="A24" s="520"/>
       <c r="B24" s="27"/>
       <c r="C24" s="28"/>
       <c r="D24" s="28"/>
       <c r="E24" s="28"/>
       <c r="F24" s="28"/>
       <c r="G24" s="28"/>
-      <c r="H24" s="353"/>
+      <c r="H24" s="352"/>
       <c r="I24" s="20"/>
       <c r="J24" s="21"/>
       <c r="K24" s="13"/>
@@ -11220,14 +11229,14 @@
       <c r="T24" s="12"/>
     </row>
     <row r="25" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="351"/>
+      <c r="A25" s="520"/>
       <c r="B25" s="11"/>
       <c r="C25" s="14"/>
       <c r="D25" s="159"/>
       <c r="E25" s="11"/>
       <c r="F25" s="15"/>
       <c r="G25" s="24"/>
-      <c r="H25" s="356"/>
+      <c r="H25" s="355"/>
       <c r="I25" s="20"/>
       <c r="J25" s="21"/>
       <c r="K25" s="13"/>
@@ -11236,14 +11245,14 @@
       <c r="N25" s="13"/>
     </row>
     <row r="26" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="351"/>
+      <c r="A26" s="520"/>
       <c r="B26" s="27"/>
       <c r="C26" s="28"/>
       <c r="D26" s="28"/>
       <c r="E26" s="28"/>
       <c r="F26" s="28"/>
       <c r="G26" s="28"/>
-      <c r="H26" s="353"/>
+      <c r="H26" s="352"/>
       <c r="I26" s="20"/>
       <c r="J26" s="21"/>
       <c r="K26" s="13"/>
@@ -11258,14 +11267,14 @@
       <c r="T26" s="12"/>
     </row>
     <row r="27" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="351"/>
+      <c r="A27" s="520"/>
       <c r="B27" s="27"/>
       <c r="C27" s="28"/>
       <c r="D27" s="28"/>
       <c r="E27" s="28"/>
       <c r="F27" s="28"/>
       <c r="G27" s="28"/>
-      <c r="H27" s="353"/>
+      <c r="H27" s="352"/>
       <c r="I27" s="20"/>
       <c r="J27" s="21"/>
       <c r="K27" s="13"/>
@@ -11280,14 +11289,14 @@
       <c r="T27" s="12"/>
     </row>
     <row r="28" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="351"/>
+      <c r="A28" s="520"/>
       <c r="B28" s="27"/>
       <c r="C28" s="28"/>
       <c r="D28" s="28"/>
       <c r="E28" s="28"/>
       <c r="F28" s="28"/>
       <c r="G28" s="28"/>
-      <c r="H28" s="353"/>
+      <c r="H28" s="352"/>
       <c r="I28" s="20"/>
       <c r="J28" s="21"/>
       <c r="K28" s="13"/>
@@ -11302,14 +11311,14 @@
       <c r="T28" s="12"/>
     </row>
     <row r="29" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="351"/>
+      <c r="A29" s="520"/>
       <c r="B29" s="27"/>
       <c r="C29" s="28"/>
       <c r="D29" s="28"/>
       <c r="E29" s="28"/>
       <c r="F29" s="28"/>
       <c r="G29" s="28"/>
-      <c r="H29" s="353"/>
+      <c r="H29" s="352"/>
       <c r="I29" s="20"/>
       <c r="J29" s="21"/>
       <c r="K29" s="13"/>
@@ -11324,14 +11333,14 @@
       <c r="T29" s="12"/>
     </row>
     <row r="30" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="351"/>
+      <c r="A30" s="520"/>
       <c r="B30" s="27"/>
       <c r="C30" s="28"/>
       <c r="D30" s="28"/>
       <c r="E30" s="28"/>
       <c r="F30" s="28"/>
       <c r="G30" s="28"/>
-      <c r="H30" s="353"/>
+      <c r="H30" s="352"/>
       <c r="I30" s="20"/>
       <c r="J30" s="21"/>
       <c r="K30" s="13"/>
@@ -11346,14 +11355,14 @@
       <c r="T30" s="12"/>
     </row>
     <row r="31" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="351"/>
+      <c r="A31" s="520"/>
       <c r="B31" s="27"/>
       <c r="C31" s="28"/>
       <c r="D31" s="28"/>
       <c r="E31" s="28"/>
       <c r="F31" s="28"/>
       <c r="G31" s="28"/>
-      <c r="H31" s="353"/>
+      <c r="H31" s="352"/>
       <c r="I31" s="20"/>
       <c r="J31" s="21"/>
       <c r="K31" s="13"/>
@@ -11368,14 +11377,14 @@
       <c r="T31" s="12"/>
     </row>
     <row r="32" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="351"/>
+      <c r="A32" s="520"/>
       <c r="B32" s="27"/>
       <c r="C32" s="28"/>
       <c r="D32" s="28"/>
       <c r="E32" s="28"/>
       <c r="F32" s="9"/>
       <c r="G32" s="28"/>
-      <c r="H32" s="353"/>
+      <c r="H32" s="352"/>
       <c r="I32" s="20"/>
       <c r="J32" s="21"/>
       <c r="K32" s="13"/>
@@ -11390,14 +11399,14 @@
       <c r="T32" s="12"/>
     </row>
     <row r="33" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="357"/>
+      <c r="A33" s="521"/>
       <c r="B33" s="130"/>
       <c r="C33" s="111"/>
       <c r="D33" s="111"/>
       <c r="E33" s="111"/>
       <c r="F33" s="111"/>
       <c r="G33" s="111"/>
-      <c r="H33" s="358"/>
+      <c r="H33" s="356"/>
       <c r="I33" s="20"/>
       <c r="J33" s="21"/>
       <c r="K33" s="13"/>
@@ -11412,14 +11421,14 @@
       <c r="T33" s="12"/>
     </row>
     <row r="34" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="351"/>
+      <c r="A34" s="520"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
-      <c r="H34" s="354"/>
+      <c r="H34" s="353"/>
       <c r="I34" s="20"/>
       <c r="J34" s="21"/>
       <c r="K34" s="13"/>
@@ -11434,14 +11443,14 @@
       <c r="T34" s="12"/>
     </row>
     <row r="35" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="359"/>
+      <c r="A35" s="519"/>
       <c r="B35" s="131"/>
       <c r="C35" s="131"/>
       <c r="D35" s="131"/>
       <c r="E35" s="131"/>
       <c r="F35" s="131"/>
       <c r="G35" s="131"/>
-      <c r="H35" s="360"/>
+      <c r="H35" s="357"/>
       <c r="I35" s="20"/>
       <c r="J35" s="21"/>
       <c r="K35" s="13"/>
@@ -11456,14 +11465,14 @@
       <c r="T35" s="12"/>
     </row>
     <row r="36" spans="1:20" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="361"/>
-      <c r="B36" s="362"/>
-      <c r="C36" s="362"/>
-      <c r="D36" s="362"/>
-      <c r="E36" s="362"/>
-      <c r="F36" s="362"/>
-      <c r="G36" s="362"/>
-      <c r="H36" s="363"/>
+      <c r="A36" s="522"/>
+      <c r="B36" s="358"/>
+      <c r="C36" s="358"/>
+      <c r="D36" s="358"/>
+      <c r="E36" s="358"/>
+      <c r="F36" s="358"/>
+      <c r="G36" s="358"/>
+      <c r="H36" s="359"/>
       <c r="I36" s="20"/>
       <c r="J36" s="21"/>
       <c r="K36" s="13"/>
@@ -11558,14 +11567,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c298f69c-7e32-4d69-8a4f-44b776bc75e5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="27d18e64-52d1-4030-b5cf-9c691bb829da" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11812,21 +11819,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c298f69c-7e32-4d69-8a4f-44b776bc75e5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="27d18e64-52d1-4030-b5cf-9c691bb829da" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B37A3888-C326-48DF-AE4A-829BED1A658A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18B17227-D4F1-4BA2-A533-34BDC1F9C7F0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c298f69c-7e32-4d69-8a4f-44b776bc75e5"/>
-    <ds:schemaRef ds:uri="27d18e64-52d1-4030-b5cf-9c691bb829da"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -11851,9 +11857,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18B17227-D4F1-4BA2-A533-34BDC1F9C7F0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B37A3888-C326-48DF-AE4A-829BED1A658A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c298f69c-7e32-4d69-8a4f-44b776bc75e5"/>
+    <ds:schemaRef ds:uri="27d18e64-52d1-4030-b5cf-9c691bb829da"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update sro logo to load properly on each sheet
</commit_message>
<xml_diff>
--- a/templates/entry_list_template.xlsx
+++ b/templates/entry_list_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brendanwoo/projects/sro_sign_in/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6E9107-E235-A640-8122-A99D5E008E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21176FAD-B3F1-9E4E-AAD9-2F4CC2569A2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="4" xr2:uid="{542D648B-9180-43EF-9053-182057C63D4C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="4" xr2:uid="{542D648B-9180-43EF-9053-182057C63D4C}"/>
   </bookViews>
   <sheets>
     <sheet name="GTWCA" sheetId="10" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="33">
   <si>
     <t>Admin Checks</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>Driver</t>
+  </si>
+  <si>
+    <t>`</t>
   </si>
 </sst>
 </file>
@@ -3292,6 +3295,9 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3309,9 +3315,6 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -5275,60 +5278,49 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>503398</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>384068</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>623082</xdr:colOff>
+      <xdr:colOff>866775</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>234137</xdr:rowOff>
+      <xdr:rowOff>492125</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A51C616-3BF1-7347-BCBC-9235B2260A5E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1553D589-A35F-89C6-A47C-4464E7BE9664}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="15400498" y="574568"/>
-          <a:ext cx="2837484" cy="993069"/>
+          <a:off x="15033625" y="333375"/>
+          <a:ext cx="3581400" cy="1492250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -5391,60 +5383,49 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>164227</xdr:colOff>
+      <xdr:colOff>95250</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>257449</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>809487</xdr:colOff>
+      <xdr:colOff>660400</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>396875</xdr:rowOff>
+      <xdr:rowOff>492125</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25852A11-DF67-474F-9384-7244EFE161D0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70433529-B030-6A49-B644-1D4AE883AA45}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="14975602" y="447949"/>
-          <a:ext cx="3661510" cy="1282426"/>
+          <a:off x="15478125" y="333375"/>
+          <a:ext cx="3581400" cy="1492250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -5454,67 +5435,6 @@
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>51975</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>221422</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>782562</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>292100</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4E44926-91F0-45EE-82FD-5A96F85CCC0B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="10846975" y="411922"/>
-          <a:ext cx="3448387" cy="1213678"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -5545,7 +5465,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -5560,6 +5480,56 @@
         <a:xfrm>
           <a:off x="165100" y="482600"/>
           <a:ext cx="3573904" cy="1181100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>79375</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>41275</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>428625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A372E33E-0A3D-7440-A09D-9D8C60624E2B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13081000" y="269875"/>
+          <a:ext cx="3581400" cy="1492250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5626,63 +5596,49 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>308972</xdr:colOff>
+      <xdr:colOff>285751</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>332773</xdr:rowOff>
+      <xdr:rowOff>206375</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>854364</xdr:colOff>
+      <xdr:colOff>783134</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>461816</xdr:rowOff>
+      <xdr:rowOff>553847</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CE623A5-A694-764D-91D7-7FC16F16E9F0}"/>
-            </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{BB4D49F0-7C12-4E0F-AE96-C6F582C70233}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD484D61-E706-3942-8448-DAFA0CC0EA2B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="12477881" y="332773"/>
-          <a:ext cx="3639574" cy="1283589"/>
+          <a:off x="12446001" y="396875"/>
+          <a:ext cx="3577133" cy="1490472"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -5739,63 +5695,49 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>2038350</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>1651000</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>746125</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1167434</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>396875</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CC8B1CD-E151-4723-A81D-1B2D3C762B9E}"/>
-            </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{23A0F608-4A61-A5A6-2E50-6990CFC54CEC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F3D3831-BE8B-264C-826B-C11262B496AF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="8483600" y="1130300"/>
-          <a:ext cx="2986709" cy="987425"/>
+          <a:off x="8096250" y="936625"/>
+          <a:ext cx="3581400" cy="1492250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -6196,8 +6138,8 @@
   </sheetPr>
   <dimension ref="A2:X34"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScale="80" zoomScaleNormal="90" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView showGridLines="0" view="pageLayout" zoomScale="80" zoomScaleNormal="90" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6222,15 +6164,15 @@
       <c r="A2" s="523"/>
       <c r="B2" s="523"/>
       <c r="C2" s="523"/>
-      <c r="D2" s="530"/>
-      <c r="E2" s="530"/>
-      <c r="F2" s="530"/>
-      <c r="G2" s="530"/>
-      <c r="H2" s="530"/>
-      <c r="I2" s="530"/>
-      <c r="J2" s="530"/>
-      <c r="K2" s="530"/>
-      <c r="L2" s="530"/>
+      <c r="D2" s="524"/>
+      <c r="E2" s="524"/>
+      <c r="F2" s="524"/>
+      <c r="G2" s="524"/>
+      <c r="H2" s="524"/>
+      <c r="I2" s="524"/>
+      <c r="J2" s="524"/>
+      <c r="K2" s="524"/>
+      <c r="L2" s="524"/>
       <c r="M2" s="523"/>
       <c r="N2" s="523"/>
     </row>
@@ -6238,17 +6180,17 @@
       <c r="A3" s="523"/>
       <c r="B3" s="523"/>
       <c r="C3" s="523"/>
-      <c r="D3" s="524" t="s">
+      <c r="D3" s="525" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="524"/>
-      <c r="F3" s="524"/>
-      <c r="G3" s="524"/>
-      <c r="H3" s="524"/>
-      <c r="I3" s="524"/>
-      <c r="J3" s="524"/>
-      <c r="K3" s="524"/>
-      <c r="L3" s="524"/>
+      <c r="E3" s="525"/>
+      <c r="F3" s="525"/>
+      <c r="G3" s="525"/>
+      <c r="H3" s="525"/>
+      <c r="I3" s="525"/>
+      <c r="J3" s="525"/>
+      <c r="K3" s="525"/>
+      <c r="L3" s="525"/>
       <c r="M3" s="523"/>
       <c r="N3" s="523"/>
     </row>
@@ -6256,15 +6198,15 @@
       <c r="A4" s="523"/>
       <c r="B4" s="523"/>
       <c r="C4" s="523"/>
-      <c r="D4" s="530"/>
-      <c r="E4" s="530"/>
-      <c r="F4" s="530"/>
-      <c r="G4" s="530"/>
-      <c r="H4" s="530"/>
-      <c r="I4" s="530"/>
-      <c r="J4" s="530"/>
-      <c r="K4" s="530"/>
-      <c r="L4" s="530"/>
+      <c r="D4" s="524"/>
+      <c r="E4" s="524"/>
+      <c r="F4" s="524"/>
+      <c r="G4" s="524"/>
+      <c r="H4" s="524"/>
+      <c r="I4" s="524"/>
+      <c r="J4" s="524"/>
+      <c r="K4" s="524"/>
+      <c r="L4" s="524"/>
       <c r="M4" s="523"/>
       <c r="N4" s="523"/>
     </row>
@@ -6928,7 +6870,7 @@
   <dimension ref="A2:Y40"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScale="80" zoomScaleNormal="115" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6949,65 +6891,65 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="525"/>
-      <c r="B2" s="525"/>
-      <c r="C2" s="525"/>
-      <c r="D2" s="530"/>
-      <c r="E2" s="530"/>
-      <c r="F2" s="530"/>
-      <c r="G2" s="530"/>
-      <c r="H2" s="530"/>
-      <c r="I2" s="530"/>
-      <c r="J2" s="530"/>
-      <c r="K2" s="530"/>
-      <c r="L2" s="530"/>
-      <c r="M2" s="525"/>
-      <c r="N2" s="525"/>
+      <c r="A2" s="526"/>
+      <c r="B2" s="526"/>
+      <c r="C2" s="526"/>
+      <c r="D2" s="524"/>
+      <c r="E2" s="524"/>
+      <c r="F2" s="524"/>
+      <c r="G2" s="524"/>
+      <c r="H2" s="524"/>
+      <c r="I2" s="524"/>
+      <c r="J2" s="524"/>
+      <c r="K2" s="524"/>
+      <c r="L2" s="524"/>
+      <c r="M2" s="526"/>
+      <c r="N2" s="526"/>
     </row>
     <row r="3" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="525"/>
-      <c r="B3" s="525"/>
-      <c r="C3" s="525"/>
-      <c r="D3" s="524" t="s">
+      <c r="A3" s="526"/>
+      <c r="B3" s="526"/>
+      <c r="C3" s="526"/>
+      <c r="D3" s="525" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="524"/>
-      <c r="F3" s="524"/>
-      <c r="G3" s="524"/>
-      <c r="H3" s="524"/>
-      <c r="I3" s="524"/>
-      <c r="J3" s="524"/>
-      <c r="K3" s="524"/>
-      <c r="L3" s="524"/>
-      <c r="M3" s="525"/>
-      <c r="N3" s="525"/>
+      <c r="E3" s="525"/>
+      <c r="F3" s="525"/>
+      <c r="G3" s="525"/>
+      <c r="H3" s="525"/>
+      <c r="I3" s="525"/>
+      <c r="J3" s="525"/>
+      <c r="K3" s="525"/>
+      <c r="L3" s="525"/>
+      <c r="M3" s="526"/>
+      <c r="N3" s="526"/>
     </row>
     <row r="4" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="525"/>
-      <c r="B4" s="525"/>
-      <c r="C4" s="525"/>
-      <c r="D4" s="530"/>
-      <c r="E4" s="530"/>
-      <c r="F4" s="530"/>
-      <c r="G4" s="530"/>
-      <c r="H4" s="530"/>
-      <c r="I4" s="530"/>
-      <c r="J4" s="530"/>
-      <c r="K4" s="530"/>
-      <c r="L4" s="530"/>
-      <c r="M4" s="525"/>
-      <c r="N4" s="525"/>
+      <c r="A4" s="526"/>
+      <c r="B4" s="526"/>
+      <c r="C4" s="526"/>
+      <c r="D4" s="524"/>
+      <c r="E4" s="524"/>
+      <c r="F4" s="524"/>
+      <c r="G4" s="524"/>
+      <c r="H4" s="524"/>
+      <c r="I4" s="524"/>
+      <c r="J4" s="524"/>
+      <c r="K4" s="524"/>
+      <c r="L4" s="524"/>
+      <c r="M4" s="526"/>
+      <c r="N4" s="526"/>
     </row>
     <row r="5" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="R5" s="526" t="s">
+      <c r="R5" s="527" t="s">
         <v>0</v>
       </c>
-      <c r="S5" s="526"/>
-      <c r="T5" s="526"/>
-      <c r="U5" s="526"/>
-      <c r="V5" s="526"/>
-      <c r="W5" s="526"/>
-      <c r="X5" s="526"/>
+      <c r="S5" s="527"/>
+      <c r="T5" s="527"/>
+      <c r="U5" s="527"/>
+      <c r="V5" s="527"/>
+      <c r="W5" s="527"/>
+      <c r="X5" s="527"/>
     </row>
     <row r="6" spans="1:24" s="2" customFormat="1" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="219" t="s">
@@ -7873,7 +7815,7 @@
   <dimension ref="A2:R41"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScale="80" zoomScaleNormal="90" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:H4"/>
+      <selection activeCell="I2" sqref="I2:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7893,51 +7835,51 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="525"/>
-      <c r="B2" s="525"/>
-      <c r="C2" s="525"/>
-      <c r="D2" s="527"/>
-      <c r="E2" s="527"/>
-      <c r="F2" s="527"/>
-      <c r="G2" s="527"/>
-      <c r="H2" s="527"/>
-      <c r="I2" s="525"/>
-      <c r="J2" s="525"/>
+      <c r="A2" s="526"/>
+      <c r="B2" s="526"/>
+      <c r="C2" s="526"/>
+      <c r="D2" s="528"/>
+      <c r="E2" s="528"/>
+      <c r="F2" s="528"/>
+      <c r="G2" s="528"/>
+      <c r="H2" s="528"/>
+      <c r="I2" s="526"/>
+      <c r="J2" s="526"/>
     </row>
     <row r="3" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="525"/>
-      <c r="B3" s="525"/>
-      <c r="C3" s="525"/>
-      <c r="D3" s="527" t="s">
+      <c r="A3" s="526"/>
+      <c r="B3" s="526"/>
+      <c r="C3" s="526"/>
+      <c r="D3" s="528" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="527"/>
-      <c r="F3" s="527"/>
-      <c r="G3" s="527"/>
-      <c r="H3" s="527"/>
-      <c r="I3" s="525"/>
-      <c r="J3" s="525"/>
+      <c r="E3" s="528"/>
+      <c r="F3" s="528"/>
+      <c r="G3" s="528"/>
+      <c r="H3" s="528"/>
+      <c r="I3" s="526"/>
+      <c r="J3" s="526"/>
     </row>
     <row r="4" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="525"/>
-      <c r="B4" s="525"/>
-      <c r="C4" s="525"/>
-      <c r="D4" s="527"/>
-      <c r="E4" s="527"/>
-      <c r="F4" s="527"/>
-      <c r="G4" s="527"/>
-      <c r="H4" s="527"/>
-      <c r="I4" s="525"/>
-      <c r="J4" s="525"/>
+      <c r="A4" s="526"/>
+      <c r="B4" s="526"/>
+      <c r="C4" s="526"/>
+      <c r="D4" s="528"/>
+      <c r="E4" s="528"/>
+      <c r="F4" s="528"/>
+      <c r="G4" s="528"/>
+      <c r="H4" s="528"/>
+      <c r="I4" s="526"/>
+      <c r="J4" s="526"/>
     </row>
     <row r="5" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="N5" s="525" t="s">
+      <c r="N5" s="526" t="s">
         <v>0</v>
       </c>
-      <c r="O5" s="525"/>
-      <c r="P5" s="525"/>
-      <c r="Q5" s="525"/>
-      <c r="R5" s="525"/>
+      <c r="O5" s="526"/>
+      <c r="P5" s="526"/>
+      <c r="Q5" s="526"/>
+      <c r="R5" s="526"/>
     </row>
     <row r="6" spans="1:18" s="2" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -8602,7 +8544,7 @@
   <dimension ref="A2:BP36"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScale="80" zoomScaleNormal="70" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:F3"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8621,47 +8563,47 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:68" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="525"/>
-      <c r="B2" s="525"/>
-      <c r="C2" s="525"/>
-      <c r="D2" s="527"/>
-      <c r="E2" s="527"/>
-      <c r="F2" s="527"/>
-      <c r="G2" s="525"/>
-      <c r="H2" s="525"/>
+      <c r="A2" s="526"/>
+      <c r="B2" s="526"/>
+      <c r="C2" s="526"/>
+      <c r="D2" s="528"/>
+      <c r="E2" s="528"/>
+      <c r="F2" s="528"/>
+      <c r="G2" s="526"/>
+      <c r="H2" s="526"/>
     </row>
     <row r="3" spans="1:68" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="525"/>
-      <c r="B3" s="525"/>
-      <c r="C3" s="525"/>
-      <c r="D3" s="527" t="s">
+      <c r="A3" s="526"/>
+      <c r="B3" s="526"/>
+      <c r="C3" s="526"/>
+      <c r="D3" s="528" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="527"/>
-      <c r="F3" s="527"/>
-      <c r="G3" s="525"/>
-      <c r="H3" s="525"/>
+      <c r="E3" s="528"/>
+      <c r="F3" s="528"/>
+      <c r="G3" s="526"/>
+      <c r="H3" s="526"/>
     </row>
     <row r="4" spans="1:68" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="525"/>
-      <c r="B4" s="525"/>
-      <c r="C4" s="525"/>
-      <c r="D4" s="527"/>
-      <c r="E4" s="527"/>
-      <c r="F4" s="527"/>
-      <c r="G4" s="525"/>
-      <c r="H4" s="525"/>
+      <c r="A4" s="526"/>
+      <c r="B4" s="526"/>
+      <c r="C4" s="526"/>
+      <c r="D4" s="528"/>
+      <c r="E4" s="528"/>
+      <c r="F4" s="528"/>
+      <c r="G4" s="526"/>
+      <c r="H4" s="526"/>
     </row>
     <row r="5" spans="1:68" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L5" s="525" t="s">
+      <c r="L5" s="526" t="s">
         <v>0</v>
       </c>
-      <c r="M5" s="525"/>
-      <c r="N5" s="525"/>
-      <c r="O5" s="525"/>
-      <c r="P5" s="525"/>
-      <c r="Q5" s="525"/>
-      <c r="R5" s="525"/>
+      <c r="M5" s="526"/>
+      <c r="N5" s="526"/>
+      <c r="O5" s="526"/>
+      <c r="P5" s="526"/>
+      <c r="Q5" s="526"/>
+      <c r="R5" s="526"/>
     </row>
     <row r="6" spans="1:68" s="10" customFormat="1" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="368" t="s">
@@ -10664,7 +10606,7 @@
   <dimension ref="A1:T43"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:F2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10703,14 +10645,14 @@
       <c r="N1" s="12"/>
     </row>
     <row r="2" spans="1:20" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="528"/>
-      <c r="B2" s="528"/>
-      <c r="C2" s="528"/>
-      <c r="D2" s="529"/>
-      <c r="E2" s="529"/>
-      <c r="F2" s="529"/>
-      <c r="G2" s="528"/>
-      <c r="H2" s="528"/>
+      <c r="A2" s="529"/>
+      <c r="B2" s="529"/>
+      <c r="C2" s="529"/>
+      <c r="D2" s="530"/>
+      <c r="E2" s="530"/>
+      <c r="F2" s="530"/>
+      <c r="G2" s="529"/>
+      <c r="H2" s="529"/>
       <c r="I2" s="12"/>
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
@@ -10725,16 +10667,16 @@
       <c r="T2" s="12"/>
     </row>
     <row r="3" spans="1:20" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="528"/>
-      <c r="B3" s="528"/>
-      <c r="C3" s="528"/>
-      <c r="D3" s="529" t="s">
+      <c r="A3" s="529"/>
+      <c r="B3" s="529"/>
+      <c r="C3" s="529"/>
+      <c r="D3" s="530" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="529"/>
-      <c r="F3" s="529"/>
-      <c r="G3" s="528"/>
-      <c r="H3" s="528"/>
+      <c r="E3" s="530"/>
+      <c r="F3" s="530"/>
+      <c r="G3" s="529"/>
+      <c r="H3" s="529"/>
       <c r="I3" s="12"/>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
@@ -10749,14 +10691,14 @@
       <c r="T3" s="12"/>
     </row>
     <row r="4" spans="1:20" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="528"/>
-      <c r="B4" s="528"/>
-      <c r="C4" s="528"/>
-      <c r="D4" s="529"/>
-      <c r="E4" s="529"/>
-      <c r="F4" s="529"/>
-      <c r="G4" s="528"/>
-      <c r="H4" s="528"/>
+      <c r="A4" s="529"/>
+      <c r="B4" s="529"/>
+      <c r="C4" s="529"/>
+      <c r="D4" s="530"/>
+      <c r="E4" s="530"/>
+      <c r="F4" s="530"/>
+      <c r="G4" s="529"/>
+      <c r="H4" s="529"/>
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
@@ -10963,7 +10905,9 @@
       <c r="D12" s="28"/>
       <c r="E12" s="111"/>
       <c r="F12" s="111"/>
-      <c r="G12" s="28"/>
+      <c r="G12" s="28" t="s">
+        <v>32</v>
+      </c>
       <c r="H12" s="352"/>
       <c r="I12" s="20"/>
       <c r="J12" s="21"/>
@@ -11567,15 +11511,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004E036A3F1E15E94A92324F6304EC7433" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f8e394c60fea3207393e1a1a2f77ce3d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c298f69c-7e32-4d69-8a4f-44b776bc75e5" xmlns:ns3="27d18e64-52d1-4030-b5cf-9c691bb829da" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a2c9b44cd906c8c5eef4b4317d39d060" ns2:_="" ns3:_="">
     <xsd:import namespace="c298f69c-7e32-4d69-8a4f-44b776bc75e5"/>
@@ -11818,6 +11753,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -11830,14 +11774,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18B17227-D4F1-4BA2-A533-34BDC1F9C7F0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5E7BAE2-04CC-4A41-8857-4BCE57D1DFAA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11856,6 +11792,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18B17227-D4F1-4BA2-A533-34BDC1F9C7F0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B37A3888-C326-48DF-AE4A-829BED1A658A}">
   <ds:schemaRefs>

</xml_diff>